<commit_message>
- Added a couple of Falchions and Twohanded swords
</commit_message>
<xml_diff>
--- a/Items+Troops Spreadsheets/HYW Item Balance.xlsx
+++ b/Items+Troops Spreadsheets/HYW Item Balance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoanne\Desktop\Deeds - Repository\Items+Troops Spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoann\OneDrive\Ambiente de Trabalho\Deeds_Modsys\Items+Troops Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E205D6-5A49-465E-9935-DE649E094D05}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38ACB4AD-B942-4BB5-A67B-92D32D566B5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10695" yWindow="660" windowWidth="21600" windowHeight="11385" firstSheet="7" activeTab="9" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
   </bookViews>
   <sheets>
     <sheet name="Maces" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="339">
   <si>
     <t>ID</t>
   </si>
@@ -384,18 +386,12 @@
     <t>w_bastard_sword_sempach</t>
   </si>
   <si>
-    <t>w_twohanded_messer</t>
-  </si>
-  <si>
     <t>w_twohanded_sword_claymore</t>
   </si>
   <si>
     <t>w_twohanded_sword_danish</t>
   </si>
   <si>
-    <t>w_twohanded_talhoffer</t>
-  </si>
-  <si>
     <t>w_twohanded_sword_steward</t>
   </si>
   <si>
@@ -1024,6 +1020,45 @@
   </si>
   <si>
     <t>w_bolt_broadhead</t>
+  </si>
+  <si>
+    <t>w_twohanded_sword_messer</t>
+  </si>
+  <si>
+    <t>w_twohanded_sword_talhoffer</t>
+  </si>
+  <si>
+    <t>w_twohanded_sword_munich</t>
+  </si>
+  <si>
+    <t>Munich Greatsword</t>
+  </si>
+  <si>
+    <t>w_twohanded_sword_earl</t>
+  </si>
+  <si>
+    <t>Earl Greatsword</t>
+  </si>
+  <si>
+    <t>w_onehanded_falchion_peasant</t>
+  </si>
+  <si>
+    <t>Peasant Falchion</t>
+  </si>
+  <si>
+    <t>Falchion</t>
+  </si>
+  <si>
+    <t>w_bastard_falchion</t>
+  </si>
+  <si>
+    <t>Hand-and-a-half Falchion</t>
+  </si>
+  <si>
+    <t>w_onehanded_falchion_a</t>
+  </si>
+  <si>
+    <t>w_onehanded_falchion_b</t>
   </si>
 </sst>
 </file>
@@ -1203,7 +1238,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1506,13 +1541,13 @@
       <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.5546875" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1541,7 +1576,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1568,7 +1603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1595,7 +1630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1622,7 +1657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -1649,7 +1684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -1676,7 +1711,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -1703,7 +1738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1732,7 +1767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -1759,7 +1794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1786,7 +1821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -1813,7 +1848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -1840,7 +1875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -1867,7 +1902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -1903,16 +1938,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3C8FEF-B598-4AEC-9E3E-97CE35ABD837}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="1" max="1" width="27.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1926,15 +1961,15 @@
         <v>5</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B2" s="6">
         <v>72</v>
@@ -1952,9 +1987,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B3" s="6">
         <v>104</v>
@@ -1972,9 +2007,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B4" s="6">
         <v>162</v>
@@ -1992,9 +2027,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B5" s="6">
         <v>98</v>
@@ -2012,9 +2047,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B6" s="6">
         <v>146</v>
@@ -2032,9 +2067,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B7" s="6">
         <v>86</v>
@@ -2052,9 +2087,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B9" s="6">
         <v>64</v>
@@ -2072,9 +2107,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B10" s="6">
         <v>92</v>
@@ -2092,9 +2127,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B11" s="6">
         <v>125</v>
@@ -2112,9 +2147,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B12" s="6">
         <v>100</v>
@@ -2132,9 +2167,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B13" s="6">
         <v>118</v>
@@ -2165,13 +2200,13 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2200,7 +2235,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -2227,7 +2262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>36</v>
       </c>
@@ -2254,7 +2289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>37</v>
       </c>
@@ -2281,7 +2316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>38</v>
       </c>
@@ -2308,7 +2343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>39</v>
       </c>
@@ -2335,7 +2370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="15"/>
@@ -2346,7 +2381,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>40</v>
       </c>
@@ -2373,7 +2408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>41</v>
       </c>
@@ -2400,7 +2435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>42</v>
       </c>
@@ -2427,7 +2462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>43</v>
       </c>
@@ -2454,7 +2489,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>44</v>
       </c>
@@ -2481,7 +2516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>45</v>
       </c>
@@ -2508,7 +2543,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="15"/>
@@ -2519,7 +2554,7 @@
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>46</v>
       </c>
@@ -2546,7 +2581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>47</v>
       </c>
@@ -2573,7 +2608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>48</v>
       </c>
@@ -2600,7 +2635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>49</v>
       </c>
@@ -2627,7 +2662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="15"/>
@@ -2638,7 +2673,7 @@
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>50</v>
       </c>
@@ -2665,7 +2700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>51</v>
       </c>
@@ -2692,7 +2727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>52</v>
       </c>
@@ -2719,7 +2754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>53</v>
       </c>
@@ -2746,7 +2781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>54</v>
       </c>
@@ -2773,7 +2808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>55</v>
       </c>
@@ -2800,7 +2835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>56</v>
       </c>
@@ -2827,7 +2862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>57</v>
       </c>
@@ -2854,7 +2889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>58</v>
       </c>
@@ -2888,20 +2923,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76258844-B7FB-4720-B431-7E6F0F318E31}">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2930,12 +2965,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C2" s="6">
         <v>73</v>
@@ -2959,12 +2994,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C3" s="6">
         <v>122</v>
@@ -2988,12 +3023,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C4" s="6">
         <v>136</v>
@@ -3017,7 +3052,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="6"/>
@@ -3028,12 +3063,12 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C6" s="6">
         <v>325</v>
@@ -3065,12 +3100,12 @@
         <v>325.44</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C7" s="6">
         <v>488</v>
@@ -3102,12 +3137,12 @@
         <v>488.03999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C8" s="6">
         <v>572</v>
@@ -3139,12 +3174,12 @@
         <v>571.5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C9" s="6">
         <v>488</v>
@@ -3176,12 +3211,12 @@
         <v>488.03999999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C10" s="6">
         <v>572</v>
@@ -3213,12 +3248,12 @@
         <v>571.5</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C11" s="6">
         <v>400</v>
@@ -3250,12 +3285,12 @@
         <v>400.53000000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C12" s="6">
         <v>488</v>
@@ -3287,12 +3322,12 @@
         <v>488.03999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C13" s="6">
         <v>572</v>
@@ -3324,12 +3359,12 @@
         <v>571.5</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C14" s="6">
         <v>506</v>
@@ -3361,12 +3396,12 @@
         <v>505.67999999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C15" s="6">
         <v>402</v>
@@ -3398,12 +3433,12 @@
         <v>402.22</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C16" s="6">
         <v>406</v>
@@ -3435,7 +3470,7 @@
         <v>405.6</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="6"/>
@@ -3446,12 +3481,12 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C18" s="6">
         <v>415</v>
@@ -3483,12 +3518,12 @@
         <v>414.55700000000007</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C19" s="6">
         <v>487</v>
@@ -3520,12 +3555,12 @@
         <v>486.86399999999992</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C20" s="6">
         <v>582</v>
@@ -3557,12 +3592,12 @@
         <v>581.625</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C21" s="6">
         <v>508</v>
@@ -3594,12 +3629,12 @@
         <v>508.42399999999986</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C22" s="6">
         <v>514</v>
@@ -3631,12 +3666,12 @@
         <v>514.30399999999986</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C23" s="6">
         <v>582</v>
@@ -3668,12 +3703,12 @@
         <v>581.625</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C24" s="6">
         <v>577</v>
@@ -3705,12 +3740,12 @@
         <v>577.125</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C25" s="6">
         <v>670</v>
@@ -3742,12 +3777,12 @@
         <v>669.69600000000014</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C26" s="6">
         <v>491</v>
@@ -3779,12 +3814,12 @@
         <v>490.78399999999993</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C27" s="6">
         <v>491</v>
@@ -3814,12 +3849,12 @@
         <v>490.78399999999993</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C28" s="6">
         <v>406</v>
@@ -3851,12 +3886,12 @@
         <v>406.10700000000008</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C29" s="6">
         <v>497</v>
@@ -3888,12 +3923,12 @@
         <v>496.66399999999993</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C30" s="6">
         <v>505</v>
@@ -3925,12 +3960,12 @@
         <v>504.50399999999991</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C31" s="6">
         <v>570</v>
@@ -3962,12 +3997,12 @@
         <v>570.375</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C32" s="6">
         <v>406</v>
@@ -3999,12 +4034,12 @@
         <v>406.10700000000008</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C33" s="6">
         <v>499</v>
@@ -4036,12 +4071,12 @@
         <v>498.62399999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>97</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C34" s="6">
         <v>577</v>
@@ -4071,6 +4106,117 @@
       <c r="K34">
         <f t="shared" si="3"/>
         <v>577.125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C36" s="6">
+        <v>312</v>
+      </c>
+      <c r="D36" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E36" s="7">
+        <v>0</v>
+      </c>
+      <c r="F36" s="5">
+        <v>99</v>
+      </c>
+      <c r="G36" s="3">
+        <v>76</v>
+      </c>
+      <c r="H36" s="1">
+        <v>32</v>
+      </c>
+      <c r="I36" s="1">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <f t="shared" ref="J36:J37" si="4">SUM(D36:I36)</f>
+        <v>208.1</v>
+      </c>
+      <c r="K36">
+        <f>J36*D36^2</f>
+        <v>251.80100000000004</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C37" s="6">
+        <v>555</v>
+      </c>
+      <c r="D37" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="E37" s="7">
+        <v>0</v>
+      </c>
+      <c r="F37" s="5">
+        <v>96</v>
+      </c>
+      <c r="G37" s="3">
+        <v>88</v>
+      </c>
+      <c r="H37" s="1">
+        <v>35</v>
+      </c>
+      <c r="I37" s="1">
+        <v>26</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="4"/>
+        <v>246.5</v>
+      </c>
+      <c r="K37">
+        <f t="shared" ref="K37" si="5">J37*D37^2</f>
+        <v>554.625</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C38" s="6">
+        <v>644</v>
+      </c>
+      <c r="D38" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="E38" s="7">
+        <v>0</v>
+      </c>
+      <c r="F38" s="5">
+        <v>95</v>
+      </c>
+      <c r="G38" s="3">
+        <v>93</v>
+      </c>
+      <c r="H38" s="1">
+        <v>34</v>
+      </c>
+      <c r="I38" s="1">
+        <v>28</v>
+      </c>
+      <c r="J38">
+        <f t="shared" ref="J38" si="6">SUM(D38:I38)</f>
+        <v>251.6</v>
+      </c>
+      <c r="K38">
+        <f t="shared" ref="K38" si="7">J38*D38^2</f>
+        <v>644.09600000000012</v>
       </c>
     </row>
   </sheetData>
@@ -4080,19 +4226,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03FAF929-B978-461F-BC5C-F0B53573D36C}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4122,12 +4268,12 @@
       </c>
       <c r="J1" s="16"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C2" s="6">
         <v>294</v>
@@ -4151,12 +4297,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>99</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C3" s="6">
         <v>526</v>
@@ -4180,12 +4326,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C4" s="6">
         <v>548</v>
@@ -4209,12 +4355,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C5" s="6">
         <v>676</v>
@@ -4238,12 +4384,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C6" s="6">
         <v>724</v>
@@ -4267,12 +4413,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C7" s="6">
         <v>638</v>
@@ -4296,7 +4442,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="6"/>
@@ -4307,12 +4453,12 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C9" s="6">
         <v>698</v>
@@ -4336,12 +4482,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>105</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C10" s="6">
         <v>892</v>
@@ -4365,12 +4511,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C11" s="6">
         <v>831</v>
@@ -4394,15 +4540,15 @@
         <v>30</v>
       </c>
       <c r="M11" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C12" s="6">
         <v>784</v>
@@ -4426,12 +4572,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>108</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C13" s="6">
         <v>938</v>
@@ -4455,12 +4601,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>109</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C14" s="6">
         <v>822</v>
@@ -4484,12 +4630,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C15" s="6">
         <v>798</v>
@@ -4513,12 +4659,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>111</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C16" s="6">
         <v>760</v>
@@ -4542,12 +4688,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C17" s="6">
         <v>885</v>
@@ -4571,12 +4717,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>113</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C18" s="6">
         <v>873</v>
@@ -4600,87 +4746,87 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="C19" s="6">
+        <v>912</v>
+      </c>
+      <c r="D19" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="E19" s="7">
+        <v>9</v>
+      </c>
+      <c r="F19" s="5">
+        <v>97</v>
+      </c>
+      <c r="G19" s="3">
+        <v>97</v>
+      </c>
+      <c r="H19" s="1">
+        <v>43</v>
+      </c>
+      <c r="I19" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C21" s="6">
+        <v>920</v>
+      </c>
+      <c r="D21" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E21" s="7">
+        <v>10</v>
+      </c>
+      <c r="F21" s="5">
+        <v>99</v>
+      </c>
+      <c r="G21" s="3">
+        <v>93</v>
+      </c>
+      <c r="H21" s="1">
+        <v>44</v>
+      </c>
+      <c r="I21" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C20" s="6">
-        <v>920</v>
-      </c>
-      <c r="D20" s="4">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E20" s="7">
-        <v>10</v>
-      </c>
-      <c r="F20" s="5">
-        <v>99</v>
-      </c>
-      <c r="G20" s="3">
-        <v>93</v>
-      </c>
-      <c r="H20" s="1">
-        <v>44</v>
-      </c>
-      <c r="I20" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C21" s="6">
+      <c r="B22" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C22" s="6">
         <v>1290</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D22" s="4">
         <v>3.5</v>
-      </c>
-      <c r="E21" s="7">
-        <v>12</v>
-      </c>
-      <c r="F21" s="5">
-        <v>94</v>
-      </c>
-      <c r="G21" s="3">
-        <v>115</v>
-      </c>
-      <c r="H21" s="1">
-        <v>43</v>
-      </c>
-      <c r="I21" s="1">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C22" s="6">
-        <v>1344</v>
-      </c>
-      <c r="D22" s="4">
-        <v>3.2</v>
       </c>
       <c r="E22" s="7">
         <v>12</v>
@@ -4689,71 +4835,158 @@
         <v>94</v>
       </c>
       <c r="G22" s="3">
+        <v>115</v>
+      </c>
+      <c r="H22" s="1">
+        <v>43</v>
+      </c>
+      <c r="I22" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C23" s="6">
+        <v>1344</v>
+      </c>
+      <c r="D23" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="E23" s="7">
+        <v>12</v>
+      </c>
+      <c r="F23" s="5">
+        <v>94</v>
+      </c>
+      <c r="G23" s="3">
         <v>114</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H23" s="1">
         <v>42</v>
       </c>
-      <c r="I22" s="1">
+      <c r="I23" s="1">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="C23" s="6">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C24" s="6">
         <v>1036</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D24" s="4">
         <v>2.25</v>
-      </c>
-      <c r="E23" s="7">
-        <v>11</v>
-      </c>
-      <c r="F23" s="5">
-        <v>96</v>
-      </c>
-      <c r="G23" s="3">
-        <v>99</v>
-      </c>
-      <c r="H23" s="1">
-        <v>41</v>
-      </c>
-      <c r="I23" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="C24" s="6">
-        <v>998</v>
-      </c>
-      <c r="D24" s="4">
-        <v>2.5</v>
       </c>
       <c r="E24" s="7">
         <v>11</v>
       </c>
       <c r="F24" s="5">
+        <v>96</v>
+      </c>
+      <c r="G24" s="3">
+        <v>99</v>
+      </c>
+      <c r="H24" s="1">
+        <v>41</v>
+      </c>
+      <c r="I24" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C25" s="6">
+        <v>998</v>
+      </c>
+      <c r="D25" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="E25" s="7">
+        <v>11</v>
+      </c>
+      <c r="F25" s="5">
         <v>95</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G25" s="3">
         <v>115</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H25" s="1">
         <v>40</v>
       </c>
-      <c r="I24" s="1">
+      <c r="I25" s="1">
         <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C26" s="6">
+        <v>1468</v>
+      </c>
+      <c r="D26" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="E26" s="7">
+        <v>12</v>
+      </c>
+      <c r="F26" s="5">
+        <v>92</v>
+      </c>
+      <c r="G26" s="3">
+        <v>123</v>
+      </c>
+      <c r="H26" s="1">
+        <v>41</v>
+      </c>
+      <c r="I26" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C27" s="6">
+        <v>1274</v>
+      </c>
+      <c r="D27" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="E27" s="7">
+        <v>11</v>
+      </c>
+      <c r="F27" s="5">
+        <v>94</v>
+      </c>
+      <c r="G27" s="3">
+        <v>111</v>
+      </c>
+      <c r="H27" s="1">
+        <v>42</v>
+      </c>
+      <c r="I27" s="1">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -4770,12 +5003,12 @@
       <selection pane="bottomLeft" activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4804,9 +5037,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="6">
@@ -4835,9 +5068,9 @@
         <v>277.5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="6">
@@ -4866,9 +5099,9 @@
         <v>282.5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="6">
@@ -4897,9 +5130,9 @@
         <v>280</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="6">
@@ -4928,9 +5161,9 @@
         <v>276.66666666666669</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6">
@@ -4959,9 +5192,9 @@
         <v>272.5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="6">
@@ -4990,9 +5223,9 @@
         <v>275</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="6">
@@ -5021,9 +5254,9 @@
         <v>492.08333333333337</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="6">
@@ -5052,9 +5285,9 @@
         <v>340.83333333333337</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="6">
@@ -5083,9 +5316,9 @@
         <v>332.5</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="6">
@@ -5114,9 +5347,9 @@
         <v>406.2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="6">
@@ -5145,9 +5378,9 @@
         <v>427.8</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="6">
@@ -5176,9 +5409,9 @@
         <v>423.12</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="6">
@@ -5207,9 +5440,9 @@
         <v>412.2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="6">
@@ -5238,9 +5471,9 @@
         <v>395.56000000000006</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="6">
@@ -5269,9 +5502,9 @@
         <v>414.96</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="6">
@@ -5300,9 +5533,9 @@
         <v>428.03999999999996</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="6">
@@ -5331,9 +5564,9 @@
         <v>417.23999999999995</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="6">
@@ -5362,9 +5595,9 @@
         <v>435.12</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="6">
@@ -5393,9 +5626,9 @@
         <v>436.32</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="6">
@@ -5424,9 +5657,9 @@
         <v>458.03999999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="6">
@@ -5455,9 +5688,9 @@
         <v>406.32</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="6">
@@ -5486,9 +5719,9 @@
         <v>441.47999999999996</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="6">
@@ -5517,9 +5750,9 @@
         <v>418.8</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="6">
@@ -5548,9 +5781,9 @@
         <v>423.59999999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="6">
@@ -5579,9 +5812,9 @@
         <v>454.92</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="6">
@@ -5610,9 +5843,9 @@
         <v>489.96</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="6">
@@ -5641,9 +5874,9 @@
         <v>504.59999999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="6">
@@ -5672,9 +5905,9 @@
         <v>375.47999999999996</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="6">
@@ -5703,9 +5936,9 @@
         <v>375.7</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="6">
@@ -5734,9 +5967,9 @@
         <v>382.85</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="6">
@@ -5765,9 +5998,9 @@
         <v>376.09000000000003</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="6">
@@ -5796,9 +6029,9 @@
         <v>359.32</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="6">
@@ -5827,9 +6060,9 @@
         <v>355.16</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="6">
@@ -5858,9 +6091,9 @@
         <v>378.95000000000005</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="6">
@@ -5889,9 +6122,9 @@
         <v>360.03000000000003</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="6">
@@ -5920,9 +6153,9 @@
         <v>420.84</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="6">
@@ -5951,9 +6184,9 @@
         <v>438.07500000000005</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="6">
@@ -5982,9 +6215,9 @@
         <v>379.92</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="6">
@@ -6013,9 +6246,9 @@
         <v>444.34000000000003</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="6">
@@ -6044,9 +6277,9 @@
         <v>382.2</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="6">
@@ -6075,9 +6308,9 @@
         <v>427.18000000000006</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="6">
@@ -6106,9 +6339,9 @@
         <v>393.5</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="6">
@@ -6137,9 +6370,9 @@
         <v>368.125</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="6">
@@ -6168,9 +6401,9 @@
         <v>425.125</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="6">
@@ -6199,9 +6432,9 @@
         <v>421</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="6">
@@ -6230,9 +6463,9 @@
         <v>398.75</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="6">
@@ -6261,9 +6494,9 @@
         <v>340.25</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="6">
@@ -6292,9 +6525,9 @@
         <v>423.625</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="6">
@@ -6323,9 +6556,9 @@
         <v>470.875</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="6">
@@ -6354,9 +6587,9 @@
         <v>431</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="6">
@@ -6385,9 +6618,9 @@
         <v>327.5</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="6">
@@ -6416,9 +6649,9 @@
         <v>471.5</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="6">
@@ -6447,9 +6680,9 @@
         <v>506.875</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" s="6">
@@ -6478,9 +6711,9 @@
         <v>462.625</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="6">
@@ -6509,9 +6742,9 @@
         <v>457.5</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" s="6">
@@ -6540,9 +6773,9 @@
         <v>447.5</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" s="6">
@@ -6571,9 +6804,9 @@
         <v>253.89000000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" s="6">
@@ -6602,9 +6835,9 @@
         <v>259.38</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="6">
@@ -6633,9 +6866,9 @@
         <v>269.45999999999998</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="6">
@@ -6664,9 +6897,9 @@
         <v>250.29000000000002</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="6">
@@ -6695,9 +6928,9 @@
         <v>249.48</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="6">
@@ -6726,9 +6959,9 @@
         <v>283.14000000000004</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="6">
@@ -6757,9 +6990,9 @@
         <v>274.68</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="6">
@@ -6788,9 +7021,9 @@
         <v>278.37</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="6">
@@ -6819,9 +7052,9 @@
         <v>270.18</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" s="6">
@@ -6863,12 +7096,12 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -6894,9 +7127,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="6">
@@ -6922,9 +7155,9 @@
         <v>170.1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="6">
@@ -6950,9 +7183,9 @@
         <v>156.78</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="6">
@@ -6978,9 +7211,9 @@
         <v>196.2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="6">
@@ -7006,9 +7239,9 @@
         <v>190.01999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6">
@@ -7034,9 +7267,9 @@
         <v>178.5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="6">
@@ -7062,9 +7295,9 @@
         <v>180.29999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="6">
@@ -7090,9 +7323,9 @@
         <v>182.76000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="6">
@@ -7118,9 +7351,9 @@
         <v>184.43999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="6">
@@ -7146,14 +7379,14 @@
         <v>166.26000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F12" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="6">
@@ -7179,9 +7412,9 @@
         <v>240.8</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="6">
@@ -7207,9 +7440,9 @@
         <v>242.4</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="6">
@@ -7235,9 +7468,9 @@
         <v>304</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="6">
@@ -7263,9 +7496,9 @@
         <v>245.76</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="6">
@@ -7291,9 +7524,9 @@
         <v>251.36</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="6">
@@ -7319,9 +7552,9 @@
         <v>233.44000000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="6">
@@ -7347,9 +7580,9 @@
         <v>232.64000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="6">
@@ -7375,9 +7608,9 @@
         <v>268.48</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="6">
@@ -7403,9 +7636,9 @@
         <v>294.8</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="6">
@@ -7444,12 +7677,12 @@
       <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -7475,9 +7708,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="6">
@@ -7503,9 +7736,9 @@
         <v>134.255</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="6">
@@ -7531,9 +7764,9 @@
         <v>144.26500000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="6">
@@ -7559,9 +7792,9 @@
         <v>146.46500000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="6">
@@ -7587,9 +7820,9 @@
         <v>164.64</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6">
@@ -7615,9 +7848,9 @@
         <v>165.83999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="6">
@@ -7643,9 +7876,9 @@
         <v>167.7</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="6">
@@ -7671,9 +7904,9 @@
         <v>228.89999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="6">
@@ -7699,9 +7932,9 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="6">
@@ -7727,9 +7960,9 @@
         <v>87.324999999999989</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="6">
@@ -7755,9 +7988,9 @@
         <v>84.14</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="6">
@@ -7783,9 +8016,9 @@
         <v>142.5</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="6">
@@ -7811,9 +8044,9 @@
         <v>285.59999999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="6">
@@ -7839,9 +8072,9 @@
         <v>213.85</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="6">
@@ -7867,9 +8100,9 @@
         <v>224.27999999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="6">
@@ -7895,9 +8128,9 @@
         <v>320.32</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="6">
@@ -7923,9 +8156,9 @@
         <v>286.40000000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="6">
@@ -7951,9 +8184,9 @@
         <v>307.36</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="6">
@@ -7979,9 +8212,9 @@
         <v>307.36</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="6">
@@ -8007,9 +8240,9 @@
         <v>308.16000000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="6">
@@ -8035,9 +8268,9 @@
         <v>296.24</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="6">
@@ -8063,9 +8296,9 @@
         <v>308.16000000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="6">
@@ -8091,9 +8324,9 @@
         <v>308.16000000000003</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="6">
@@ -8119,9 +8352,9 @@
         <v>320.32</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="6">
@@ -8147,9 +8380,9 @@
         <v>308.16000000000003</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="6">
@@ -8175,9 +8408,9 @@
         <v>308.16000000000003</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="6">
@@ -8216,14 +8449,14 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -8240,21 +8473,21 @@
         <v>34</v>
       </c>
       <c r="F1" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="6">
@@ -8279,9 +8512,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="6">
@@ -8306,9 +8539,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="6">
@@ -8333,9 +8566,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="6">
@@ -8360,9 +8593,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="6">
@@ -8387,9 +8620,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="6">
@@ -8414,9 +8647,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="6">
@@ -8441,9 +8674,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="6">
@@ -8468,9 +8701,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="6">
@@ -8495,9 +8728,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="6">
@@ -8522,9 +8755,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="6">
@@ -8549,9 +8782,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="6">
@@ -8576,9 +8809,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="6">
@@ -8603,9 +8836,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="6">
@@ -8630,9 +8863,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="6">
@@ -8657,9 +8890,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="6">
@@ -8684,9 +8917,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="6">
@@ -8711,9 +8944,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="6">
@@ -8738,9 +8971,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="6">
@@ -8765,9 +8998,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="6">
@@ -8792,9 +9025,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="6">
@@ -8819,9 +9052,9 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="6">
@@ -8846,9 +9079,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="6">
@@ -8886,14 +9119,14 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -8901,13 +9134,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>225</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>227</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>34</v>
@@ -8916,15 +9149,15 @@
         <v>4</v>
       </c>
       <c r="H1" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>230</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="4">
@@ -8953,9 +9186,9 @@
         <v>299</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="4">
@@ -8984,9 +9217,9 @@
         <v>341.11111111111109</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="4">
@@ -9015,9 +9248,9 @@
         <v>493.33333333333337</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="4">
@@ -9046,9 +9279,9 @@
         <v>624</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="4">
@@ -9077,9 +9310,9 @@
         <v>780</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="4">
@@ -9108,9 +9341,9 @@
         <v>983.33333333333337</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="4">
@@ -9139,9 +9372,9 @@
         <v>1455</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="4">

</xml_diff>

<commit_message>
- Added new sword - Added Asher's gambeson with patches
</commit_message>
<xml_diff>
--- a/Items+Troops Spreadsheets/HYW Item Balance.xlsx
+++ b/Items+Troops Spreadsheets/HYW Item Balance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoann\OneDrive\Ambiente de Trabalho\Deeds_Modsys\Items+Troops Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38ACB4AD-B942-4BB5-A67B-92D32D566B5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DD02AB-DBA9-4468-9539-E17D003D2722}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="3" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
   </bookViews>
   <sheets>
     <sheet name="Maces" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="340">
   <si>
     <t>ID</t>
   </si>
@@ -1059,6 +1059,9 @@
   </si>
   <si>
     <t>w_onehanded_falchion_b</t>
+  </si>
+  <si>
+    <t>w_twohanded_sword_messer_b</t>
   </si>
 </sst>
 </file>
@@ -1142,7 +1145,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1165,22 +1168,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1211,7 +1203,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1968,7 +1959,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>315</v>
       </c>
       <c r="B2" s="6">
@@ -1988,7 +1979,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>316</v>
       </c>
       <c r="B3" s="6">
@@ -2008,7 +1999,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>317</v>
       </c>
       <c r="B4" s="6">
@@ -2028,7 +2019,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>318</v>
       </c>
       <c r="B5" s="6">
@@ -2048,7 +2039,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>319</v>
       </c>
       <c r="B6" s="6">
@@ -2068,7 +2059,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="16" t="s">
         <v>320</v>
       </c>
       <c r="B7" s="6">
@@ -2088,7 +2079,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>321</v>
       </c>
       <c r="B9" s="6">
@@ -2108,7 +2099,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
         <v>322</v>
       </c>
       <c r="B10" s="6">
@@ -2128,7 +2119,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="16" t="s">
         <v>323</v>
       </c>
       <c r="B11" s="6">
@@ -2148,7 +2139,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="16" t="s">
         <v>324</v>
       </c>
       <c r="B12" s="6">
@@ -2168,7 +2159,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="16" t="s">
         <v>325</v>
       </c>
       <c r="B13" s="6">
@@ -2925,9 +2916,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76258844-B7FB-4720-B431-7E6F0F318E31}">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K36" sqref="K36"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3302,24 +3293,24 @@
         <v>0</v>
       </c>
       <c r="F12" s="5">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G12" s="3">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H12" s="1">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I12" s="1">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J12">
         <f t="shared" si="0"/>
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="K12">
         <f t="shared" si="1"/>
-        <v>488.03999999999996</v>
+        <v>495.87999999999994</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -3339,24 +3330,24 @@
         <v>0</v>
       </c>
       <c r="F13" s="5">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G13" s="3">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="H13" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I13" s="1">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="J13">
         <f t="shared" si="0"/>
-        <v>254</v>
+        <v>264</v>
       </c>
       <c r="K13">
         <f t="shared" si="1"/>
-        <v>571.5</v>
+        <v>594</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -4226,15 +4217,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03FAF929-B978-461F-BC5C-F0B53573D36C}">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="1" max="1" width="28.5546875" customWidth="1"/>
     <col min="2" max="2" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4266,7 +4258,6 @@
       <c r="I1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="16"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -4817,175 +4808,204 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>114</v>
+        <v>339</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C22" s="6">
-        <v>1290</v>
+        <v>1166</v>
       </c>
       <c r="D22" s="4">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="E22" s="7">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F22" s="5">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G22" s="3">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="H22" s="1">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I22" s="1">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C23" s="6">
-        <v>1344</v>
+        <v>1290</v>
       </c>
       <c r="D23" s="4">
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="E23" s="7">
         <v>12</v>
       </c>
       <c r="F23" s="5">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G23" s="3">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="H23" s="1">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I23" s="1">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C24" s="6">
-        <v>1036</v>
+        <v>1344</v>
       </c>
       <c r="D24" s="4">
-        <v>2.25</v>
+        <v>3.2</v>
       </c>
       <c r="E24" s="7">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F24" s="5">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G24" s="3">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="H24" s="1">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I24" s="1">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>327</v>
+        <v>116</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C25" s="6">
-        <v>998</v>
+        <v>1036</v>
       </c>
       <c r="D25" s="4">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="E25" s="7">
         <v>11</v>
       </c>
       <c r="F25" s="5">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G25" s="3">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="H25" s="1">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I25" s="1">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>329</v>
+        <v>184</v>
       </c>
       <c r="C26" s="6">
-        <v>1468</v>
+        <v>998</v>
       </c>
       <c r="D26" s="4">
-        <v>2.7</v>
+        <v>2.5</v>
       </c>
       <c r="E26" s="7">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F26" s="5">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G26" s="3">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="H26" s="1">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I26" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C27" s="6">
+        <v>1468</v>
+      </c>
+      <c r="D27" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="E27" s="7">
+        <v>12</v>
+      </c>
+      <c r="F27" s="5">
+        <v>92</v>
+      </c>
+      <c r="G27" s="3">
+        <v>123</v>
+      </c>
+      <c r="H27" s="1">
+        <v>41</v>
+      </c>
+      <c r="I27" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C28" s="6">
         <v>1274</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D28" s="4">
         <v>2.4</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E28" s="7">
         <v>11</v>
       </c>
-      <c r="F27" s="5">
+      <c r="F28" s="5">
         <v>94</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G28" s="3">
         <v>111</v>
       </c>
-      <c r="H27" s="1">
+      <c r="H28" s="1">
         <v>42</v>
       </c>
-      <c r="I27" s="1">
+      <c r="I28" s="1">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Added iJustWant2bPure's updated sounds - Updated English plate and added German shield variants - Minor code tweaks to agent spawning
</commit_message>
<xml_diff>
--- a/Items+Troops Spreadsheets/HYW Item Balance.xlsx
+++ b/Items+Troops Spreadsheets/HYW Item Balance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoann\OneDrive\Ambiente de Trabalho\Deeds_Modsys\Items+Troops Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DD02AB-DBA9-4468-9539-E17D003D2722}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63060D38-42F6-4432-A38D-AB5DF3BD4912}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="3" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="10" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
   </bookViews>
   <sheets>
     <sheet name="Maces" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Bows &amp; Crossbows" sheetId="6" r:id="rId8"/>
     <sheet name="Horses" sheetId="7" r:id="rId9"/>
     <sheet name="Arrows &amp; Bolts" sheetId="10" r:id="rId10"/>
+    <sheet name="Shields" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="351">
   <si>
     <t>ID</t>
   </si>
@@ -1062,6 +1063,39 @@
   </si>
   <si>
     <t>w_twohanded_sword_messer_b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width </t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Native</t>
+  </si>
+  <si>
+    <t>Native Pavise</t>
+  </si>
+  <si>
+    <t>Pavise</t>
+  </si>
+  <si>
+    <t>Heater Shield</t>
+  </si>
+  <si>
+    <t>LL Heater Shield</t>
+  </si>
+  <si>
+    <t>Metal Heraldic Shield</t>
+  </si>
+  <si>
+    <t>Bouche Shield</t>
+  </si>
+  <si>
+    <t>Heraldic Banner</t>
+  </si>
+  <si>
+    <t>Buckler</t>
   </si>
 </sst>
 </file>
@@ -1077,7 +1111,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1144,8 +1178,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1168,11 +1214,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1204,11 +1263,116 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="11">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1226,6 +1390,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9F5046EE-3462-4861-8BA7-BDFE936F9817}" name="Tableau1" displayName="Tableau1" ref="A1:H9" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="9" tableBorderDxfId="10">
+  <autoFilter ref="A1:H9" xr:uid="{C03180B4-6AED-435F-B389-4A4563BC2CC7}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{C9803FB6-EDE5-4D36-AE31-771E624ABD45}" name="Native" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{5FC1EA44-BFAD-4BBC-B86E-2A3CF8B5EE66}" name="Price" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{01474069-2C07-4B0D-BCD4-BCBEA8815443}" name="Weight" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{90286B08-5EC7-4290-B829-6A962FFA020D}" name="Hitpoints" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{BEB87F5A-2E44-49CC-B818-CB41CAE1540E}" name="Armor" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{1FC9649F-49E2-4557-9365-90302BBA23F5}" name="Speed" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{9DBEE228-7BC6-4A16-9AEA-276D82F520AF}" name="Width " dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{F49F7FEF-63B8-416A-B721-00BC45756836}" name="Height" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1930,7 +2111,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2180,6 +2361,252 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6EE9141-0B58-4213-922A-6EE4F5E15BD3}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
+        <v>342</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>340</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>343</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="19">
+        <v>4.5</v>
+      </c>
+      <c r="D2" s="20">
+        <v>660</v>
+      </c>
+      <c r="E2" s="21">
+        <v>32</v>
+      </c>
+      <c r="F2" s="22">
+        <v>82</v>
+      </c>
+      <c r="G2" s="19">
+        <v>55</v>
+      </c>
+      <c r="H2" s="23">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
+        <v>344</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="19">
+        <v>3.5</v>
+      </c>
+      <c r="D3" s="20">
+        <v>380</v>
+      </c>
+      <c r="E3" s="21">
+        <v>30</v>
+      </c>
+      <c r="F3" s="22">
+        <v>86</v>
+      </c>
+      <c r="G3" s="19">
+        <v>45</v>
+      </c>
+      <c r="H3" s="23">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>345</v>
+      </c>
+      <c r="B4" s="18"/>
+      <c r="C4" s="19">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D4" s="20">
+        <v>350</v>
+      </c>
+      <c r="E4" s="21">
+        <v>25</v>
+      </c>
+      <c r="F4" s="22">
+        <v>92</v>
+      </c>
+      <c r="G4" s="19">
+        <v>50</v>
+      </c>
+      <c r="H4" s="23">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>346</v>
+      </c>
+      <c r="B5" s="18"/>
+      <c r="C5" s="19">
+        <v>1.6</v>
+      </c>
+      <c r="D5" s="20">
+        <v>400</v>
+      </c>
+      <c r="E5" s="21">
+        <v>22</v>
+      </c>
+      <c r="F5" s="22">
+        <v>94</v>
+      </c>
+      <c r="G5" s="19">
+        <v>48</v>
+      </c>
+      <c r="H5" s="23">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
+        <v>347</v>
+      </c>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19">
+        <v>2.4</v>
+      </c>
+      <c r="D6" s="20">
+        <v>350</v>
+      </c>
+      <c r="E6" s="21">
+        <v>28</v>
+      </c>
+      <c r="F6" s="22">
+        <v>91</v>
+      </c>
+      <c r="G6" s="19">
+        <v>50</v>
+      </c>
+      <c r="H6" s="23">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>348</v>
+      </c>
+      <c r="B7" s="18"/>
+      <c r="C7" s="19">
+        <v>2</v>
+      </c>
+      <c r="D7" s="20">
+        <v>260</v>
+      </c>
+      <c r="E7" s="21">
+        <v>26</v>
+      </c>
+      <c r="F7" s="22">
+        <v>90</v>
+      </c>
+      <c r="G7" s="19">
+        <v>40</v>
+      </c>
+      <c r="H7" s="23">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="B8" s="18"/>
+      <c r="C8" s="19">
+        <v>3</v>
+      </c>
+      <c r="D8" s="20">
+        <v>999</v>
+      </c>
+      <c r="E8" s="21">
+        <v>4</v>
+      </c>
+      <c r="F8" s="22">
+        <v>88</v>
+      </c>
+      <c r="G8" s="19">
+        <v>1</v>
+      </c>
+      <c r="H8" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>350</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D9" s="20">
+        <v>115</v>
+      </c>
+      <c r="E9" s="21">
+        <v>40</v>
+      </c>
+      <c r="F9" s="22">
+        <v>100</v>
+      </c>
+      <c r="G9" s="19">
+        <v>34</v>
+      </c>
+      <c r="H9" s="23">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -4219,7 +4646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03FAF929-B978-461F-BC5C-F0B53573D36C}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>

</xml_diff>

<commit_message>
- Updated shield stats
</commit_message>
<xml_diff>
--- a/Items+Troops Spreadsheets/HYW Item Balance.xlsx
+++ b/Items+Troops Spreadsheets/HYW Item Balance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoann\OneDrive\Ambiente de Trabalho\Deeds_Modsys\Items+Troops Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63060D38-42F6-4432-A38D-AB5DF3BD4912}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7243CE62-4B1B-475B-B07C-802425B909D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="10" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
+    <workbookView xWindow="12576" yWindow="5424" windowWidth="17280" windowHeight="8964" firstSheet="5" activeTab="10" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
   </bookViews>
   <sheets>
     <sheet name="Maces" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="352">
   <si>
     <t>ID</t>
   </si>
@@ -1096,6 +1096,9 @@
   </si>
   <si>
     <t>Buckler</t>
+  </si>
+  <si>
+    <t>Colonne1</t>
   </si>
 </sst>
 </file>
@@ -1275,24 +1278,9 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="12">
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1" tint="0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <fill>
@@ -1360,16 +1348,34 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
           <color indexed="64"/>
-        </top>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1393,9 +1399,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9F5046EE-3462-4861-8BA7-BDFE936F9817}" name="Tableau1" displayName="Tableau1" ref="A1:H9" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="9" tableBorderDxfId="10">
-  <autoFilter ref="A1:H9" xr:uid="{C03180B4-6AED-435F-B389-4A4563BC2CC7}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9F5046EE-3462-4861-8BA7-BDFE936F9817}" name="Tableau1" displayName="Tableau1" ref="A1:I9" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
+  <autoFilter ref="A1:I9" xr:uid="{C03180B4-6AED-435F-B389-4A4563BC2CC7}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{C9803FB6-EDE5-4D36-AE31-771E624ABD45}" name="Native" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{5FC1EA44-BFAD-4BBC-B86E-2A3CF8B5EE66}" name="Price" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{01474069-2C07-4B0D-BCD4-BCBEA8815443}" name="Weight" dataDxfId="6"/>
@@ -1404,6 +1410,9 @@
     <tableColumn id="6" xr3:uid="{1FC9649F-49E2-4557-9365-90302BBA23F5}" name="Speed" dataDxfId="3"/>
     <tableColumn id="7" xr3:uid="{9DBEE228-7BC6-4A16-9AEA-276D82F520AF}" name="Width " dataDxfId="2"/>
     <tableColumn id="8" xr3:uid="{F49F7FEF-63B8-416A-B721-00BC45756836}" name="Height" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{2B135CC7-F1ED-468C-AA68-F96B873B45CB}" name="Colonne1" dataDxfId="0">
+      <calculatedColumnFormula>((Tableau1[[#This Row],[Hitpoints]]*Tableau1[[#This Row],[Armor]]*2)+(Tableau1[[#This Row],[Width ]]*Tableau1[[#This Row],[Height]]*2)-(Tableau1[[#This Row],[Speed]]*Tableau1[[#This Row],[Weight]]))/100</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2366,10 +2375,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6EE9141-0B58-4213-922A-6EE4F5E15BD3}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2384,7 +2393,7 @@
     <col min="8" max="8" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>342</v>
       </c>
@@ -2409,12 +2418,17 @@
       <c r="H1" s="24" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="24" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>343</v>
       </c>
-      <c r="B2" s="18"/>
+      <c r="B2" s="18">
+        <v>550</v>
+      </c>
       <c r="C2" s="19">
         <v>4.5</v>
       </c>
@@ -2433,12 +2447,18 @@
       <c r="H2" s="23">
         <v>120</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2">
+        <f>((Tableau1[[#This Row],[Hitpoints]]*Tableau1[[#This Row],[Armor]]*2)+(Tableau1[[#This Row],[Width ]]*Tableau1[[#This Row],[Height]]*2)-(Tableau1[[#This Row],[Speed]]*Tableau1[[#This Row],[Weight]]))/100</f>
+        <v>550.71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>344</v>
       </c>
-      <c r="B3" s="18"/>
+      <c r="B3" s="18">
+        <v>420</v>
+      </c>
       <c r="C3" s="19">
         <v>3.5</v>
       </c>
@@ -2457,12 +2477,18 @@
       <c r="H3" s="23">
         <v>85</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <f>((Tableau1[[#This Row],[Hitpoints]]*Tableau1[[#This Row],[Armor]])+(Tableau1[[#This Row],[Width ]]*Tableau1[[#This Row],[Height]]*2)-(Tableau1[[#This Row],[Speed]]*Tableau1[[#This Row],[Weight]]))/100</f>
+        <v>187.49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>345</v>
       </c>
-      <c r="B4" s="18"/>
+      <c r="B4" s="18">
+        <v>340</v>
+      </c>
       <c r="C4" s="19">
         <v>2.2000000000000002</v>
       </c>
@@ -2481,12 +2507,18 @@
       <c r="H4" s="23">
         <v>70</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <f>((Tableau1[[#This Row],[Hitpoints]]*Tableau1[[#This Row],[Armor]]*2)+(Tableau1[[#This Row],[Width ]]*Tableau1[[#This Row],[Height]]*2)-(Tableau1[[#This Row],[Speed]]*Tableau1[[#This Row],[Weight]]))/100</f>
+        <v>242.976</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>346</v>
       </c>
-      <c r="B5" s="18"/>
+      <c r="B5" s="18">
+        <v>220</v>
+      </c>
       <c r="C5" s="19">
         <v>1.6</v>
       </c>
@@ -2505,12 +2537,18 @@
       <c r="H5" s="23">
         <v>85</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <f>((Tableau1[[#This Row],[Hitpoints]]*Tableau1[[#This Row],[Armor]]*2)+(Tableau1[[#This Row],[Width ]]*Tableau1[[#This Row],[Height]]*2)-(Tableau1[[#This Row],[Speed]]*Tableau1[[#This Row],[Weight]]))/100</f>
+        <v>256.096</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>347</v>
       </c>
-      <c r="B6" s="18"/>
+      <c r="B6" s="18">
+        <v>380</v>
+      </c>
       <c r="C6" s="19">
         <v>2.4</v>
       </c>
@@ -2529,12 +2567,18 @@
       <c r="H6" s="23">
         <v>70</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6">
+        <f>((Tableau1[[#This Row],[Hitpoints]]*Tableau1[[#This Row],[Armor]]*2)+(Tableau1[[#This Row],[Width ]]*Tableau1[[#This Row],[Height]]*2)-(Tableau1[[#This Row],[Speed]]*Tableau1[[#This Row],[Weight]]))/100</f>
+        <v>263.81599999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>348</v>
       </c>
-      <c r="B7" s="18"/>
+      <c r="B7" s="18">
+        <v>400</v>
+      </c>
       <c r="C7" s="19">
         <v>2</v>
       </c>
@@ -2553,12 +2597,18 @@
       <c r="H7" s="23">
         <v>65</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7">
+        <f>((Tableau1[[#This Row],[Hitpoints]]*Tableau1[[#This Row],[Armor]]*2)+(Tableau1[[#This Row],[Width ]]*Tableau1[[#This Row],[Height]]*2)-(Tableau1[[#This Row],[Speed]]*Tableau1[[#This Row],[Weight]]))/100</f>
+        <v>185.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>349</v>
       </c>
-      <c r="B8" s="18"/>
+      <c r="B8" s="18">
+        <v>1500</v>
+      </c>
       <c r="C8" s="19">
         <v>3</v>
       </c>
@@ -2577,12 +2627,18 @@
       <c r="H8" s="23">
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <f>((Tableau1[[#This Row],[Hitpoints]]*Tableau1[[#This Row],[Armor]]*2)+(Tableau1[[#This Row],[Width ]]*Tableau1[[#This Row],[Height]]*2)-(Tableau1[[#This Row],[Speed]]*Tableau1[[#This Row],[Weight]]))/100</f>
+        <v>79.28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>350</v>
       </c>
-      <c r="B9" s="18"/>
+      <c r="B9" s="18">
+        <v>180</v>
+      </c>
       <c r="C9" s="19">
         <v>1.1000000000000001</v>
       </c>
@@ -2600,6 +2656,10 @@
       </c>
       <c r="H9" s="23">
         <v>34</v>
+      </c>
+      <c r="I9">
+        <f>((Tableau1[[#This Row],[Hitpoints]]*Tableau1[[#This Row],[Armor]]*2)+(Tableau1[[#This Row],[Width ]]*Tableau1[[#This Row],[Height]]*2)-(Tableau1[[#This Row],[Speed]]*Tableau1[[#This Row],[Weight]]))/100</f>
+        <v>114.02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Added new pollaxes
</commit_message>
<xml_diff>
--- a/Items+Troops Spreadsheets/HYW Item Balance.xlsx
+++ b/Items+Troops Spreadsheets/HYW Item Balance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoann\OneDrive\Ambiente de Trabalho\Deeds_Modsys\Items+Troops Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7243CE62-4B1B-475B-B07C-802425B909D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBA71C5-FF2B-4C91-8783-A67CBB16902F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12576" yWindow="5424" windowWidth="17280" windowHeight="8964" firstSheet="5" activeTab="10" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="7" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
   </bookViews>
   <sheets>
     <sheet name="Maces" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,11 @@
     <sheet name="Pikes &amp; Halberds" sheetId="5" r:id="rId5"/>
     <sheet name="Forks, Fauchards &amp; Glaives" sheetId="8" r:id="rId6"/>
     <sheet name="Spears &amp; Lances" sheetId="9" r:id="rId7"/>
-    <sheet name="Bows &amp; Crossbows" sheetId="6" r:id="rId8"/>
-    <sheet name="Horses" sheetId="7" r:id="rId9"/>
-    <sheet name="Arrows &amp; Bolts" sheetId="10" r:id="rId10"/>
-    <sheet name="Shields" sheetId="11" r:id="rId11"/>
+    <sheet name="Pollaxes" sheetId="12" r:id="rId8"/>
+    <sheet name="Bows &amp; Crossbows" sheetId="6" r:id="rId9"/>
+    <sheet name="Horses" sheetId="7" r:id="rId10"/>
+    <sheet name="Arrows &amp; Bolts" sheetId="10" r:id="rId11"/>
+    <sheet name="Shields" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="376">
   <si>
     <t>ID</t>
   </si>
@@ -1099,13 +1100,85 @@
   </si>
   <si>
     <t>Colonne1</t>
+  </si>
+  <si>
+    <t>w_pollaxe_blunt_1_french</t>
+  </si>
+  <si>
+    <t>w_pollaxe_blunt_2_french</t>
+  </si>
+  <si>
+    <t>w_pollaxe_blunt_3</t>
+  </si>
+  <si>
+    <t>w_pollaxe_blunt_4_english</t>
+  </si>
+  <si>
+    <t>w_pollaxe_blunt_5</t>
+  </si>
+  <si>
+    <t>w_pollaxe_blunt_6_italian</t>
+  </si>
+  <si>
+    <t>w_pollaxe_blunt_7</t>
+  </si>
+  <si>
+    <t>w_pollaxe_blunt_8</t>
+  </si>
+  <si>
+    <t>w_pollaxe_blunt_9</t>
+  </si>
+  <si>
+    <t>w_pollaxe_blunt_10</t>
+  </si>
+  <si>
+    <t>w_pollaxe_blunt_11</t>
+  </si>
+  <si>
+    <t>w_pollaxe_blunt_12</t>
+  </si>
+  <si>
+    <t>w_pollaxe_cut_1_burgundian</t>
+  </si>
+  <si>
+    <t>w_pollaxe_cut_2_french</t>
+  </si>
+  <si>
+    <t>w_pollaxe_cut_3</t>
+  </si>
+  <si>
+    <t>w_pollaxe_cut_4_english</t>
+  </si>
+  <si>
+    <t>w_pollaxe_cut_5</t>
+  </si>
+  <si>
+    <t>w_pollaxe_cut_6</t>
+  </si>
+  <si>
+    <t>w_pollaxe_cut_7</t>
+  </si>
+  <si>
+    <t>w_pollaxe_cut_8_burgundian</t>
+  </si>
+  <si>
+    <t>w_pollaxe_cut_9</t>
+  </si>
+  <si>
+    <t>Alternative</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>bl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1113,8 +1186,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1193,8 +1272,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C7E7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1230,11 +1321,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1274,6 +1395,16 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2116,6 +2247,303 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DAD396-9A3B-4E45-8468-1404C7D6E830}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="4">
+        <v>100</v>
+      </c>
+      <c r="D2" s="7">
+        <v>100</v>
+      </c>
+      <c r="E2" s="5">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>36</v>
+      </c>
+      <c r="H2" s="1">
+        <v>42</v>
+      </c>
+      <c r="I2" s="1">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <f>SUM(C2:I2)</f>
+        <v>299</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="4">
+        <v>90</v>
+      </c>
+      <c r="D3" s="7">
+        <v>110</v>
+      </c>
+      <c r="E3" s="5">
+        <v>12</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>40</v>
+      </c>
+      <c r="H3" s="1">
+        <v>42</v>
+      </c>
+      <c r="I3" s="1">
+        <v>12</v>
+      </c>
+      <c r="J3">
+        <f>SUM(C3:I3)/0.9</f>
+        <v>341.11111111111109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="4">
+        <v>80</v>
+      </c>
+      <c r="D4" s="7">
+        <v>90</v>
+      </c>
+      <c r="E4" s="5">
+        <v>14</v>
+      </c>
+      <c r="F4" s="3">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>50</v>
+      </c>
+      <c r="H4" s="1">
+        <v>44</v>
+      </c>
+      <c r="I4" s="1">
+        <v>16</v>
+      </c>
+      <c r="J4">
+        <f>SUM(C4:I4)/0.6</f>
+        <v>493.33333333333337</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="4">
+        <v>70</v>
+      </c>
+      <c r="D5" s="7">
+        <v>120</v>
+      </c>
+      <c r="E5" s="5">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>44</v>
+      </c>
+      <c r="H5" s="1">
+        <v>42</v>
+      </c>
+      <c r="I5" s="1">
+        <v>20</v>
+      </c>
+      <c r="J5">
+        <f>SUM(C5:I5)/0.5</f>
+        <v>624</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="4">
+        <v>60</v>
+      </c>
+      <c r="D6" s="7">
+        <v>120</v>
+      </c>
+      <c r="E6" s="5">
+        <v>25</v>
+      </c>
+      <c r="F6" s="3">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1">
+        <v>40</v>
+      </c>
+      <c r="H6" s="1">
+        <v>40</v>
+      </c>
+      <c r="I6" s="1">
+        <v>24</v>
+      </c>
+      <c r="J6">
+        <f>SUM(C6:I6)/0.4</f>
+        <v>780</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="4">
+        <v>40</v>
+      </c>
+      <c r="D7" s="7">
+        <v>120</v>
+      </c>
+      <c r="E7" s="5">
+        <v>30</v>
+      </c>
+      <c r="F7" s="3">
+        <v>3</v>
+      </c>
+      <c r="G7" s="1">
+        <v>38</v>
+      </c>
+      <c r="H7" s="1">
+        <v>38</v>
+      </c>
+      <c r="I7" s="1">
+        <v>26</v>
+      </c>
+      <c r="J7">
+        <f>SUM(C7:I7)/0.3</f>
+        <v>983.33333333333337</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="4">
+        <v>40</v>
+      </c>
+      <c r="D8" s="7">
+        <v>120</v>
+      </c>
+      <c r="E8" s="5">
+        <v>22</v>
+      </c>
+      <c r="F8" s="3">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1">
+        <v>42</v>
+      </c>
+      <c r="H8" s="1">
+        <v>40</v>
+      </c>
+      <c r="I8" s="1">
+        <v>24</v>
+      </c>
+      <c r="J8">
+        <f>SUM(C8:I8)/0.2</f>
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="4">
+        <v>40</v>
+      </c>
+      <c r="D9" s="7">
+        <v>130</v>
+      </c>
+      <c r="E9" s="5">
+        <v>25</v>
+      </c>
+      <c r="F9" s="3">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1">
+        <v>42</v>
+      </c>
+      <c r="H9" s="1">
+        <v>40</v>
+      </c>
+      <c r="I9" s="1">
+        <v>28</v>
+      </c>
+      <c r="J9">
+        <f>SUM(C9:I9)/0.2</f>
+        <v>1540</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3C8FEF-B598-4AEC-9E3E-97CE35ABD837}">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -2373,11 +2801,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6EE9141-0B58-4213-922A-6EE4F5E15BD3}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -4707,8 +5135,8 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5507,7 +5935,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C79" sqref="C79"/>
+      <selection pane="bottomLeft" activeCell="J65" sqref="J65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7600,7 +8028,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8181,7 +8609,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8949,6 +9377,691 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C18765D9-5E60-43F7-8EAE-7692D37C4247}">
+  <dimension ref="A1:J23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B2" s="27">
+        <v>1047</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D2" s="7">
+        <v>12</v>
+      </c>
+      <c r="E2" s="5">
+        <v>90</v>
+      </c>
+      <c r="F2" s="3">
+        <v>148</v>
+      </c>
+      <c r="G2" s="1">
+        <v>33</v>
+      </c>
+      <c r="H2" s="1">
+        <v>33</v>
+      </c>
+      <c r="I2" s="28">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B3" s="26">
+        <v>1142</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D3" s="7">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5">
+        <v>90</v>
+      </c>
+      <c r="F3" s="3">
+        <v>148</v>
+      </c>
+      <c r="G3" s="1">
+        <v>36</v>
+      </c>
+      <c r="H3" s="1">
+        <v>33</v>
+      </c>
+      <c r="I3" s="28">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B4" s="26">
+        <v>1070</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D4" s="7">
+        <v>12</v>
+      </c>
+      <c r="E4" s="5">
+        <v>91</v>
+      </c>
+      <c r="F4" s="3">
+        <v>141</v>
+      </c>
+      <c r="G4" s="1">
+        <v>34</v>
+      </c>
+      <c r="H4" s="1">
+        <v>34</v>
+      </c>
+      <c r="I4" s="28">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B5" s="26">
+        <v>990</v>
+      </c>
+      <c r="C5" s="4">
+        <v>2</v>
+      </c>
+      <c r="D5" s="7">
+        <v>12</v>
+      </c>
+      <c r="E5" s="5">
+        <v>93</v>
+      </c>
+      <c r="F5" s="3">
+        <v>124</v>
+      </c>
+      <c r="G5" s="1">
+        <v>35</v>
+      </c>
+      <c r="H5" s="1">
+        <v>34</v>
+      </c>
+      <c r="I5" s="28">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B6" s="26">
+        <v>1343</v>
+      </c>
+      <c r="C6" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="D6" s="7">
+        <v>12</v>
+      </c>
+      <c r="E6" s="5">
+        <v>88</v>
+      </c>
+      <c r="F6" s="3">
+        <v>159</v>
+      </c>
+      <c r="G6" s="1">
+        <v>38</v>
+      </c>
+      <c r="H6" s="1">
+        <v>35</v>
+      </c>
+      <c r="I6" s="28">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B7" s="26">
+        <v>1052</v>
+      </c>
+      <c r="C7" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D7" s="7">
+        <v>12</v>
+      </c>
+      <c r="E7" s="5">
+        <v>91</v>
+      </c>
+      <c r="F7" s="3">
+        <v>143</v>
+      </c>
+      <c r="G7" s="1">
+        <v>32</v>
+      </c>
+      <c r="H7" s="1">
+        <v>35</v>
+      </c>
+      <c r="I7" s="28">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B8" s="26">
+        <v>1125</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D8" s="7">
+        <v>12</v>
+      </c>
+      <c r="E8" s="5">
+        <v>91</v>
+      </c>
+      <c r="F8" s="3">
+        <v>144</v>
+      </c>
+      <c r="G8" s="1">
+        <v>35</v>
+      </c>
+      <c r="H8" s="1">
+        <v>34</v>
+      </c>
+      <c r="I8" s="28">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B9" s="26">
+        <v>1333</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="D9" s="7">
+        <v>12</v>
+      </c>
+      <c r="E9" s="5">
+        <v>86</v>
+      </c>
+      <c r="F9" s="3">
+        <v>157</v>
+      </c>
+      <c r="G9" s="1">
+        <v>38</v>
+      </c>
+      <c r="H9" s="1">
+        <v>36</v>
+      </c>
+      <c r="I9" s="28">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B10" s="26">
+        <v>1253</v>
+      </c>
+      <c r="C10" s="4">
+        <v>2.6</v>
+      </c>
+      <c r="D10" s="7">
+        <v>12</v>
+      </c>
+      <c r="E10" s="5">
+        <v>84</v>
+      </c>
+      <c r="F10" s="3">
+        <v>164</v>
+      </c>
+      <c r="G10" s="1">
+        <v>35</v>
+      </c>
+      <c r="H10" s="1">
+        <v>36</v>
+      </c>
+      <c r="I10" s="28">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B11" s="26">
+        <v>1138</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="D11" s="7">
+        <v>12</v>
+      </c>
+      <c r="E11" s="5">
+        <v>88</v>
+      </c>
+      <c r="F11" s="3">
+        <v>155</v>
+      </c>
+      <c r="G11" s="1">
+        <v>34</v>
+      </c>
+      <c r="H11" s="1">
+        <v>34</v>
+      </c>
+      <c r="I11" s="28">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B12" s="26">
+        <v>1227</v>
+      </c>
+      <c r="C12" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="D12" s="7">
+        <v>12</v>
+      </c>
+      <c r="E12" s="5">
+        <v>88</v>
+      </c>
+      <c r="F12" s="3">
+        <v>154</v>
+      </c>
+      <c r="G12" s="1">
+        <v>38</v>
+      </c>
+      <c r="H12" s="1">
+        <v>33</v>
+      </c>
+      <c r="I12" s="28">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B13" s="26">
+        <v>1313</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="D13" s="7">
+        <v>12</v>
+      </c>
+      <c r="E13" s="5">
+        <v>88</v>
+      </c>
+      <c r="F13" s="3">
+        <v>151</v>
+      </c>
+      <c r="G13" s="1">
+        <v>37</v>
+      </c>
+      <c r="H13" s="1">
+        <v>37</v>
+      </c>
+      <c r="I13" s="28">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B15" s="25">
+        <v>1332</v>
+      </c>
+      <c r="C15" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D15" s="7">
+        <v>12</v>
+      </c>
+      <c r="E15" s="5">
+        <v>91</v>
+      </c>
+      <c r="F15" s="3">
+        <v>142</v>
+      </c>
+      <c r="G15" s="1">
+        <v>42</v>
+      </c>
+      <c r="H15" s="1">
+        <v>34</v>
+      </c>
+      <c r="I15" s="28">
+        <v>34</v>
+      </c>
+      <c r="J15" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B16" s="26">
+        <v>1288</v>
+      </c>
+      <c r="C16" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="D16" s="7">
+        <v>12</v>
+      </c>
+      <c r="E16" s="5">
+        <v>90</v>
+      </c>
+      <c r="F16" s="3">
+        <v>145</v>
+      </c>
+      <c r="G16" s="1">
+        <v>38</v>
+      </c>
+      <c r="H16" s="1">
+        <v>36</v>
+      </c>
+      <c r="I16" s="28">
+        <v>35</v>
+      </c>
+      <c r="J16" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B17" s="26">
+        <v>1207</v>
+      </c>
+      <c r="C17" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D17" s="7">
+        <v>12</v>
+      </c>
+      <c r="E17" s="5">
+        <v>93</v>
+      </c>
+      <c r="F17" s="3">
+        <v>129</v>
+      </c>
+      <c r="G17" s="1">
+        <v>41</v>
+      </c>
+      <c r="H17" s="1">
+        <v>34</v>
+      </c>
+      <c r="I17" s="28">
+        <v>35</v>
+      </c>
+      <c r="J17" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="B18" s="26">
+        <v>1648</v>
+      </c>
+      <c r="C18" s="4">
+        <v>2.6</v>
+      </c>
+      <c r="D18" s="7">
+        <v>12</v>
+      </c>
+      <c r="E18" s="5">
+        <v>82</v>
+      </c>
+      <c r="F18" s="3">
+        <v>173</v>
+      </c>
+      <c r="G18" s="1">
+        <v>46</v>
+      </c>
+      <c r="H18" s="1">
+        <v>35</v>
+      </c>
+      <c r="I18" s="28">
+        <v>36</v>
+      </c>
+      <c r="J18" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B19" s="26">
+        <v>1403</v>
+      </c>
+      <c r="C19" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="D19" s="7">
+        <v>12</v>
+      </c>
+      <c r="E19" s="5">
+        <v>86</v>
+      </c>
+      <c r="F19" s="3">
+        <v>157</v>
+      </c>
+      <c r="G19" s="1">
+        <v>40</v>
+      </c>
+      <c r="H19" s="1">
+        <v>36</v>
+      </c>
+      <c r="I19" s="28">
+        <v>36</v>
+      </c>
+      <c r="J19" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B20" s="26">
+        <v>1594</v>
+      </c>
+      <c r="C20" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="D20" s="7">
+        <v>12</v>
+      </c>
+      <c r="E20" s="5">
+        <v>84</v>
+      </c>
+      <c r="F20" s="3">
+        <v>166</v>
+      </c>
+      <c r="G20" s="1">
+        <v>44</v>
+      </c>
+      <c r="H20" s="1">
+        <v>36</v>
+      </c>
+      <c r="I20" s="28">
+        <v>38</v>
+      </c>
+      <c r="J20" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="B21" s="26">
+        <v>1558</v>
+      </c>
+      <c r="C21" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="D21" s="7">
+        <v>12</v>
+      </c>
+      <c r="E21" s="5">
+        <v>84</v>
+      </c>
+      <c r="F21" s="3">
+        <v>166</v>
+      </c>
+      <c r="G21" s="1">
+        <v>43</v>
+      </c>
+      <c r="H21" s="1">
+        <v>36</v>
+      </c>
+      <c r="I21" s="28">
+        <v>38</v>
+      </c>
+      <c r="J21" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B22" s="26">
+        <v>1657</v>
+      </c>
+      <c r="C22" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="D22" s="7">
+        <v>12</v>
+      </c>
+      <c r="E22" s="5">
+        <v>82</v>
+      </c>
+      <c r="F22" s="3">
+        <v>172</v>
+      </c>
+      <c r="G22" s="1">
+        <v>44</v>
+      </c>
+      <c r="H22" s="1">
+        <v>37</v>
+      </c>
+      <c r="I22" s="28">
+        <v>38</v>
+      </c>
+      <c r="J22" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B23" s="26">
+        <v>1620</v>
+      </c>
+      <c r="C23" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="D23" s="7">
+        <v>12</v>
+      </c>
+      <c r="E23" s="5">
+        <v>84</v>
+      </c>
+      <c r="F23" s="3">
+        <v>165</v>
+      </c>
+      <c r="G23" s="1">
+        <v>45</v>
+      </c>
+      <c r="H23" s="1">
+        <v>36</v>
+      </c>
+      <c r="I23" s="28">
+        <v>37</v>
+      </c>
+      <c r="J23" t="s">
+        <v>375</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96551E4B-D0DF-400F-B6DB-43F70FA502C4}">
   <dimension ref="A1:I29"/>
   <sheetViews>
@@ -9616,301 +10729,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DAD396-9A3B-4E45-8468-1404C7D6E830}">
-  <dimension ref="A1:J9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="4">
-        <v>100</v>
-      </c>
-      <c r="D2" s="7">
-        <v>100</v>
-      </c>
-      <c r="E2" s="5">
-        <v>10</v>
-      </c>
-      <c r="F2" s="3">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1">
-        <v>36</v>
-      </c>
-      <c r="H2" s="1">
-        <v>42</v>
-      </c>
-      <c r="I2" s="1">
-        <v>10</v>
-      </c>
-      <c r="J2">
-        <f>SUM(C2:I2)</f>
-        <v>299</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="4">
-        <v>90</v>
-      </c>
-      <c r="D3" s="7">
-        <v>110</v>
-      </c>
-      <c r="E3" s="5">
-        <v>12</v>
-      </c>
-      <c r="F3" s="3">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1">
-        <v>40</v>
-      </c>
-      <c r="H3" s="1">
-        <v>42</v>
-      </c>
-      <c r="I3" s="1">
-        <v>12</v>
-      </c>
-      <c r="J3">
-        <f>SUM(C3:I3)/0.9</f>
-        <v>341.11111111111109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="4">
-        <v>80</v>
-      </c>
-      <c r="D4" s="7">
-        <v>90</v>
-      </c>
-      <c r="E4" s="5">
-        <v>14</v>
-      </c>
-      <c r="F4" s="3">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1">
-        <v>50</v>
-      </c>
-      <c r="H4" s="1">
-        <v>44</v>
-      </c>
-      <c r="I4" s="1">
-        <v>16</v>
-      </c>
-      <c r="J4">
-        <f>SUM(C4:I4)/0.6</f>
-        <v>493.33333333333337</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="4">
-        <v>70</v>
-      </c>
-      <c r="D5" s="7">
-        <v>120</v>
-      </c>
-      <c r="E5" s="5">
-        <v>14</v>
-      </c>
-      <c r="F5" s="3">
-        <v>2</v>
-      </c>
-      <c r="G5" s="1">
-        <v>44</v>
-      </c>
-      <c r="H5" s="1">
-        <v>42</v>
-      </c>
-      <c r="I5" s="1">
-        <v>20</v>
-      </c>
-      <c r="J5">
-        <f>SUM(C5:I5)/0.5</f>
-        <v>624</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="4">
-        <v>60</v>
-      </c>
-      <c r="D6" s="7">
-        <v>120</v>
-      </c>
-      <c r="E6" s="5">
-        <v>25</v>
-      </c>
-      <c r="F6" s="3">
-        <v>3</v>
-      </c>
-      <c r="G6" s="1">
-        <v>40</v>
-      </c>
-      <c r="H6" s="1">
-        <v>40</v>
-      </c>
-      <c r="I6" s="1">
-        <v>24</v>
-      </c>
-      <c r="J6">
-        <f>SUM(C6:I6)/0.4</f>
-        <v>780</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="4">
-        <v>40</v>
-      </c>
-      <c r="D7" s="7">
-        <v>120</v>
-      </c>
-      <c r="E7" s="5">
-        <v>30</v>
-      </c>
-      <c r="F7" s="3">
-        <v>3</v>
-      </c>
-      <c r="G7" s="1">
-        <v>38</v>
-      </c>
-      <c r="H7" s="1">
-        <v>38</v>
-      </c>
-      <c r="I7" s="1">
-        <v>26</v>
-      </c>
-      <c r="J7">
-        <f>SUM(C7:I7)/0.3</f>
-        <v>983.33333333333337</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="4">
-        <v>40</v>
-      </c>
-      <c r="D8" s="7">
-        <v>120</v>
-      </c>
-      <c r="E8" s="5">
-        <v>22</v>
-      </c>
-      <c r="F8" s="3">
-        <v>3</v>
-      </c>
-      <c r="G8" s="1">
-        <v>42</v>
-      </c>
-      <c r="H8" s="1">
-        <v>40</v>
-      </c>
-      <c r="I8" s="1">
-        <v>24</v>
-      </c>
-      <c r="J8">
-        <f>SUM(C8:I8)/0.2</f>
-        <v>1455</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="4">
-        <v>40</v>
-      </c>
-      <c r="D9" s="7">
-        <v>130</v>
-      </c>
-      <c r="E9" s="5">
-        <v>25</v>
-      </c>
-      <c r="F9" s="3">
-        <v>3</v>
-      </c>
-      <c r="G9" s="1">
-        <v>42</v>
-      </c>
-      <c r="H9" s="1">
-        <v>40</v>
-      </c>
-      <c r="I9" s="1">
-        <v>28</v>
-      </c>
-      <c r="J9">
-        <f>SUM(C9:I9)/0.2</f>
-        <v>1540</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
- Updated Axes and Bardiches - Reduced costs of purchasing weapons for the mercenary camp (needs testing)
</commit_message>
<xml_diff>
--- a/Items+Troops Spreadsheets/HYW Item Balance.xlsx
+++ b/Items+Troops Spreadsheets/HYW Item Balance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoann\OneDrive\Ambiente de Trabalho\Deeds_Modsys\Items+Troops Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBA71C5-FF2B-4C91-8783-A67CBB16902F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9124E127-B05B-4D3D-8542-8079C2A74CA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="7" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
   </bookViews>
   <sheets>
     <sheet name="Maces" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="381">
   <si>
     <t>ID</t>
   </si>
@@ -154,36 +154,6 @@
     <t>w_archer_hatchet</t>
   </si>
   <si>
-    <t>w_onehanded_war_axe</t>
-  </si>
-  <si>
-    <t>w_onehanded_war_axe_2</t>
-  </si>
-  <si>
-    <t>w_onehanded_war_axe_3</t>
-  </si>
-  <si>
-    <t>w_onehanded_war_axe_4</t>
-  </si>
-  <si>
-    <t>w_horseman_axe_1</t>
-  </si>
-  <si>
-    <t>w_horseman_axe_2</t>
-  </si>
-  <si>
-    <t>w_horseman_axe_3</t>
-  </si>
-  <si>
-    <t>w_german_knight_axe</t>
-  </si>
-  <si>
-    <t>w_german_knight_axe_2</t>
-  </si>
-  <si>
-    <t>w_knight_battle_axe</t>
-  </si>
-  <si>
     <t>w_twohanded_war_axe</t>
   </si>
   <si>
@@ -1172,6 +1142,51 @@
   </si>
   <si>
     <t>bl</t>
+  </si>
+  <si>
+    <t>w_onehanded_war_axe_01</t>
+  </si>
+  <si>
+    <t>w_onehanded_war_axe_02</t>
+  </si>
+  <si>
+    <t>w_onehanded_war_axe_03</t>
+  </si>
+  <si>
+    <t>w_onehanded_war_axe_04</t>
+  </si>
+  <si>
+    <t>w_onehanded_horseman_axe_01</t>
+  </si>
+  <si>
+    <t>w_onehanded_horseman_axe_02</t>
+  </si>
+  <si>
+    <t>w_onehanded_horseman_axe_03</t>
+  </si>
+  <si>
+    <t>w_onehanded_knight_axe_german_01</t>
+  </si>
+  <si>
+    <t>w_onehanded_knight_axe_german_02</t>
+  </si>
+  <si>
+    <t>w_twohanded_knight_battle_axe_01</t>
+  </si>
+  <si>
+    <t>w_onehanded_knight_axe_01</t>
+  </si>
+  <si>
+    <t>Knight Axe</t>
+  </si>
+  <si>
+    <t>w_onehanded_knight_axe_02</t>
+  </si>
+  <si>
+    <t>w_twohanded_knight_battle_axe_02</t>
+  </si>
+  <si>
+    <t>w_twohanded_knight_battle_axe_03</t>
   </si>
 </sst>
 </file>
@@ -2269,13 +2284,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>34</v>
@@ -2284,15 +2299,15 @@
         <v>4</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="4">
@@ -2323,7 +2338,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="4">
@@ -2354,7 +2369,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="4">
@@ -2385,7 +2400,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="4">
@@ -2416,7 +2431,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="4">
@@ -2447,7 +2462,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="4">
@@ -2478,7 +2493,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="4">
@@ -2509,7 +2524,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="4">
@@ -2570,15 +2585,15 @@
         <v>5</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="B2" s="6">
         <v>72</v>
@@ -2598,7 +2613,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="B3" s="6">
         <v>104</v>
@@ -2618,7 +2633,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="B4" s="6">
         <v>162</v>
@@ -2638,7 +2653,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="B5" s="6">
         <v>98</v>
@@ -2658,7 +2673,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="B6" s="6">
         <v>146</v>
@@ -2678,7 +2693,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="B7" s="6">
         <v>86</v>
@@ -2698,7 +2713,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="B9" s="6">
         <v>64</v>
@@ -2718,7 +2733,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="B10" s="6">
         <v>92</v>
@@ -2738,7 +2753,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="B11" s="6">
         <v>125</v>
@@ -2758,7 +2773,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="B12" s="6">
         <v>100</v>
@@ -2778,7 +2793,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="B13" s="6">
         <v>118</v>
@@ -2823,7 +2838,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="B1" s="24" t="s">
         <v>2</v>
@@ -2832,27 +2847,27 @@
         <v>3</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="F1" s="24" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="H1" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="I1" s="24" t="s">
         <v>341</v>
-      </c>
-      <c r="I1" s="24" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="B2" s="18">
         <v>550</v>
@@ -2882,7 +2897,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="B3" s="18">
         <v>420</v>
@@ -2912,7 +2927,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="B4" s="18">
         <v>340</v>
@@ -2942,7 +2957,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="B5" s="18">
         <v>220</v>
@@ -2972,7 +2987,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="B6" s="18">
         <v>380</v>
@@ -3002,7 +3017,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="B7" s="18">
         <v>400</v>
@@ -3032,7 +3047,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="B8" s="18">
         <v>1500</v>
@@ -3062,7 +3077,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="B9" s="18">
         <v>180</v>
@@ -3100,15 +3115,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64CAC7F2-FAD3-4FE8-9D42-216993956934}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" width="35.21875" customWidth="1"/>
     <col min="2" max="2" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3146,7 +3161,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C2" s="15">
         <v>71</v>
@@ -3162,7 +3177,7 @@
         <v>46</v>
       </c>
       <c r="H2" s="14">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="I2" s="14">
         <v>0</v>
@@ -3170,10 +3185,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>36</v>
+        <v>366</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C3" s="15">
         <v>221</v>
@@ -3197,10 +3212,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>37</v>
+        <v>367</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C4" s="15">
         <v>87</v>
@@ -3224,10 +3239,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>38</v>
+        <v>368</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C5" s="15">
         <v>142</v>
@@ -3251,10 +3266,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>39</v>
+        <v>369</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C6" s="15">
         <v>190</v>
@@ -3289,10 +3304,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>40</v>
+        <v>370</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C8" s="15">
         <v>202</v>
@@ -3316,10 +3331,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>41</v>
+        <v>371</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C9" s="15">
         <v>176</v>
@@ -3343,10 +3358,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>42</v>
+        <v>372</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C10" s="15">
         <v>234</v>
@@ -3369,84 +3384,68 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="15">
-        <v>354</v>
-      </c>
-      <c r="D11" s="10">
-        <v>3</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="11"/>
-      <c r="F11" s="12">
-        <v>94</v>
-      </c>
-      <c r="G11" s="13">
-        <v>94</v>
-      </c>
-      <c r="H11" s="14">
-        <v>35</v>
-      </c>
-      <c r="I11" s="14">
-        <v>19</v>
-      </c>
+      <c r="F11" s="12"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>44</v>
+        <v>373</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C12" s="15">
-        <v>246</v>
+        <v>354</v>
       </c>
       <c r="D12" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="12">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G12" s="13">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="H12" s="14">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I12" s="14">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>45</v>
+        <v>374</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C13" s="15">
-        <v>371</v>
+        <v>246</v>
       </c>
       <c r="D13" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E13" s="11"/>
       <c r="F13" s="12">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G13" s="13">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="H13" s="14">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I13" s="14">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -3462,199 +3461,183 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>46</v>
+        <v>376</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>64</v>
+        <v>377</v>
       </c>
       <c r="C15" s="15">
-        <v>236</v>
+        <v>337</v>
       </c>
       <c r="D15" s="10">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="12">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G15" s="13">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="H15" s="14">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="I15" s="14">
-        <v>0</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>47</v>
+        <v>378</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>64</v>
+        <v>377</v>
       </c>
       <c r="C16" s="15">
-        <v>287</v>
+        <v>314</v>
       </c>
       <c r="D16" s="10">
-        <v>4</v>
+        <v>3.2</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="12">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G16" s="13">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="H16" s="14">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="I16" s="14">
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" s="15">
-        <v>321</v>
-      </c>
-      <c r="D17" s="10">
-        <v>4</v>
-      </c>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="10"/>
       <c r="E17" s="11"/>
-      <c r="F17" s="12">
-        <v>94</v>
-      </c>
-      <c r="G17" s="13">
-        <v>99</v>
-      </c>
-      <c r="H17" s="14">
-        <v>44</v>
-      </c>
-      <c r="I17" s="14">
-        <v>0</v>
-      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>49</v>
+        <v>375</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C18" s="15">
-        <v>304</v>
+        <v>371</v>
       </c>
       <c r="D18" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E18" s="11"/>
       <c r="F18" s="12">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="G18" s="13">
-        <v>156</v>
+        <v>97</v>
       </c>
       <c r="H18" s="14">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I18" s="14">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="10"/>
+      <c r="A19" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="15">
+        <v>428</v>
+      </c>
+      <c r="D19" s="10">
+        <v>3.4</v>
+      </c>
       <c r="E19" s="11"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
+      <c r="F19" s="12">
+        <v>92</v>
+      </c>
+      <c r="G19" s="13">
+        <v>106</v>
+      </c>
+      <c r="H19" s="14">
+        <v>38</v>
+      </c>
+      <c r="I19" s="14">
+        <v>33</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>50</v>
+        <v>380</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C20" s="15">
-        <v>539</v>
+        <v>399</v>
       </c>
       <c r="D20" s="10">
-        <v>5.75</v>
+        <v>3.3</v>
       </c>
       <c r="E20" s="11"/>
       <c r="F20" s="12">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="G20" s="13">
-        <v>140</v>
+        <v>97</v>
       </c>
       <c r="H20" s="14">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="I20" s="14">
-        <v>0</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21" s="15">
-        <v>628</v>
-      </c>
-      <c r="D21" s="10">
-        <v>6</v>
-      </c>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="10"/>
       <c r="E21" s="11"/>
-      <c r="F21" s="12">
-        <v>85</v>
-      </c>
-      <c r="G21" s="13">
-        <v>155</v>
-      </c>
-      <c r="H21" s="14">
-        <v>52</v>
-      </c>
-      <c r="I21" s="14">
-        <v>0</v>
-      </c>
+      <c r="F21" s="12"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C22" s="15">
-        <v>334</v>
+        <v>236</v>
       </c>
       <c r="D22" s="10">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="E22" s="11"/>
       <c r="F22" s="12">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="G22" s="13">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="H22" s="14">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I22" s="14">
         <v>0</v>
@@ -3662,26 +3645,26 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C23" s="15">
-        <v>306</v>
+        <v>287</v>
       </c>
       <c r="D23" s="10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E23" s="11"/>
       <c r="F23" s="12">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G23" s="13">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H23" s="14">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I23" s="14">
         <v>0</v>
@@ -3689,26 +3672,26 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="C24" s="15">
-        <v>368</v>
+        <v>321</v>
       </c>
       <c r="D24" s="10">
-        <v>5.25</v>
+        <v>4</v>
       </c>
       <c r="E24" s="11"/>
       <c r="F24" s="12">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="G24" s="13">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="H24" s="14">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I24" s="14">
         <v>0</v>
@@ -3716,80 +3699,64 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="C25" s="15">
-        <v>399</v>
+        <v>304</v>
       </c>
       <c r="D25" s="10">
-        <v>5.25</v>
+        <v>4</v>
       </c>
       <c r="E25" s="11"/>
       <c r="F25" s="12">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G25" s="13">
-        <v>110</v>
+        <v>156</v>
       </c>
       <c r="H25" s="14">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="I25" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="15">
-        <v>291</v>
-      </c>
-      <c r="D26" s="10">
-        <v>5</v>
-      </c>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="10"/>
       <c r="E26" s="11"/>
-      <c r="F26" s="12">
-        <v>91</v>
-      </c>
-      <c r="G26" s="13">
-        <v>106</v>
-      </c>
-      <c r="H26" s="14">
-        <v>43</v>
-      </c>
-      <c r="I26" s="14">
-        <v>0</v>
-      </c>
+      <c r="F26" s="12"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C27" s="15">
-        <v>498</v>
+        <v>539</v>
       </c>
       <c r="D27" s="10">
-        <v>5.5</v>
+        <v>5.75</v>
       </c>
       <c r="E27" s="11"/>
       <c r="F27" s="12">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G27" s="13">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="H27" s="14">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="I27" s="14">
         <v>0</v>
@@ -3797,28 +3764,217 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C28" s="15">
-        <v>464</v>
+        <v>628</v>
       </c>
       <c r="D28" s="10">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="E28" s="11"/>
       <c r="F28" s="12">
+        <v>85</v>
+      </c>
+      <c r="G28" s="13">
+        <v>155</v>
+      </c>
+      <c r="H28" s="14">
+        <v>52</v>
+      </c>
+      <c r="I28" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="15">
+        <v>334</v>
+      </c>
+      <c r="D29" s="10">
+        <v>5</v>
+      </c>
+      <c r="E29" s="11"/>
+      <c r="F29" s="12">
         <v>89</v>
       </c>
-      <c r="G28" s="13">
+      <c r="G29" s="13">
+        <v>107</v>
+      </c>
+      <c r="H29" s="14">
+        <v>45</v>
+      </c>
+      <c r="I29" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="15">
+        <v>306</v>
+      </c>
+      <c r="D30" s="10">
+        <v>5</v>
+      </c>
+      <c r="E30" s="11"/>
+      <c r="F30" s="12">
+        <v>91</v>
+      </c>
+      <c r="G30" s="13">
+        <v>103</v>
+      </c>
+      <c r="H30" s="14">
+        <v>44</v>
+      </c>
+      <c r="I30" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="15">
+        <v>368</v>
+      </c>
+      <c r="D31" s="10">
+        <v>5.25</v>
+      </c>
+      <c r="E31" s="11"/>
+      <c r="F31" s="12">
+        <v>90</v>
+      </c>
+      <c r="G31" s="13">
+        <v>106</v>
+      </c>
+      <c r="H31" s="14">
+        <v>46</v>
+      </c>
+      <c r="I31" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="15">
+        <v>399</v>
+      </c>
+      <c r="D32" s="10">
+        <v>5.25</v>
+      </c>
+      <c r="E32" s="11"/>
+      <c r="F32" s="12">
+        <v>89</v>
+      </c>
+      <c r="G32" s="13">
+        <v>110</v>
+      </c>
+      <c r="H32" s="14">
+        <v>47</v>
+      </c>
+      <c r="I32" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="15">
+        <v>291</v>
+      </c>
+      <c r="D33" s="10">
+        <v>5</v>
+      </c>
+      <c r="E33" s="11"/>
+      <c r="F33" s="12">
+        <v>91</v>
+      </c>
+      <c r="G33" s="13">
+        <v>106</v>
+      </c>
+      <c r="H33" s="14">
+        <v>43</v>
+      </c>
+      <c r="I33" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="15">
+        <v>498</v>
+      </c>
+      <c r="D34" s="10">
+        <v>5.5</v>
+      </c>
+      <c r="E34" s="11"/>
+      <c r="F34" s="12">
+        <v>88</v>
+      </c>
+      <c r="G34" s="13">
+        <v>105</v>
+      </c>
+      <c r="H34" s="14">
+        <v>49</v>
+      </c>
+      <c r="I34" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="15">
+        <v>464</v>
+      </c>
+      <c r="D35" s="10">
+        <v>5.5</v>
+      </c>
+      <c r="E35" s="11"/>
+      <c r="F35" s="12">
+        <v>89</v>
+      </c>
+      <c r="G35" s="13">
         <v>101</v>
       </c>
-      <c r="H28" s="14">
+      <c r="H35" s="14">
         <v>48</v>
       </c>
-      <c r="I28" s="14">
+      <c r="I35" s="14">
         <v>0</v>
       </c>
     </row>
@@ -3873,10 +4029,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="C2" s="6">
         <v>73</v>
@@ -3902,10 +4058,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="C3" s="6">
         <v>122</v>
@@ -3931,10 +4087,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C4" s="6">
         <v>136</v>
@@ -3971,10 +4127,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C6" s="6">
         <v>325</v>
@@ -4008,10 +4164,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C7" s="6">
         <v>488</v>
@@ -4045,10 +4201,10 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C8" s="6">
         <v>572</v>
@@ -4082,10 +4238,10 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C9" s="6">
         <v>488</v>
@@ -4119,10 +4275,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C10" s="6">
         <v>572</v>
@@ -4156,10 +4312,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="C11" s="6">
         <v>400</v>
@@ -4193,10 +4349,10 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C12" s="6">
         <v>488</v>
@@ -4230,10 +4386,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C13" s="6">
         <v>572</v>
@@ -4267,10 +4423,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="C14" s="6">
         <v>506</v>
@@ -4304,10 +4460,10 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="C15" s="6">
         <v>402</v>
@@ -4341,10 +4497,10 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="C16" s="6">
         <v>406</v>
@@ -4389,10 +4545,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C18" s="6">
         <v>415</v>
@@ -4426,10 +4582,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="C19" s="6">
         <v>487</v>
@@ -4463,10 +4619,10 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="C20" s="6">
         <v>582</v>
@@ -4500,10 +4656,10 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C21" s="6">
         <v>508</v>
@@ -4537,10 +4693,10 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="C22" s="6">
         <v>514</v>
@@ -4574,10 +4730,10 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C23" s="6">
         <v>582</v>
@@ -4611,10 +4767,10 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="C24" s="6">
         <v>577</v>
@@ -4648,10 +4804,10 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C25" s="6">
         <v>670</v>
@@ -4685,10 +4841,10 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C26" s="6">
         <v>491</v>
@@ -4722,10 +4878,10 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C27" s="6">
         <v>491</v>
@@ -4757,10 +4913,10 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C28" s="6">
         <v>406</v>
@@ -4794,10 +4950,10 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="C29" s="6">
         <v>497</v>
@@ -4831,10 +4987,10 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C30" s="6">
         <v>505</v>
@@ -4868,10 +5024,10 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C31" s="6">
         <v>570</v>
@@ -4905,10 +5061,10 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="C32" s="6">
         <v>406</v>
@@ -4942,10 +5098,10 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="C33" s="6">
         <v>499</v>
@@ -4979,10 +5135,10 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C34" s="6">
         <v>577</v>
@@ -5016,10 +5172,10 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="C36" s="6">
         <v>312</v>
@@ -5053,10 +5209,10 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="C37" s="6">
         <v>555</v>
@@ -5090,10 +5246,10 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="C38" s="6">
         <v>644</v>
@@ -5176,10 +5332,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="C2" s="6">
         <v>294</v>
@@ -5205,10 +5361,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="C3" s="6">
         <v>526</v>
@@ -5234,10 +5390,10 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="C4" s="6">
         <v>548</v>
@@ -5263,10 +5419,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C5" s="6">
         <v>676</v>
@@ -5292,10 +5448,10 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C6" s="6">
         <v>724</v>
@@ -5321,10 +5477,10 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C7" s="6">
         <v>638</v>
@@ -5361,10 +5517,10 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="C9" s="6">
         <v>698</v>
@@ -5390,10 +5546,10 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C10" s="6">
         <v>892</v>
@@ -5419,10 +5575,10 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C11" s="6">
         <v>831</v>
@@ -5446,15 +5602,15 @@
         <v>30</v>
       </c>
       <c r="M11" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C12" s="6">
         <v>784</v>
@@ -5480,10 +5636,10 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="C13" s="6">
         <v>938</v>
@@ -5509,10 +5665,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="C14" s="6">
         <v>822</v>
@@ -5538,10 +5694,10 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C15" s="6">
         <v>798</v>
@@ -5567,10 +5723,10 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C16" s="6">
         <v>760</v>
@@ -5596,10 +5752,10 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="C17" s="6">
         <v>885</v>
@@ -5625,10 +5781,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C18" s="6">
         <v>873</v>
@@ -5654,10 +5810,10 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="C19" s="6">
         <v>912</v>
@@ -5694,10 +5850,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C21" s="6">
         <v>920</v>
@@ -5723,10 +5879,10 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C22" s="6">
         <v>1166</v>
@@ -5752,10 +5908,10 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="C23" s="6">
         <v>1290</v>
@@ -5781,10 +5937,10 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="C24" s="6">
         <v>1344</v>
@@ -5810,10 +5966,10 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="C25" s="6">
         <v>1036</v>
@@ -5839,10 +5995,10 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="C26" s="6">
         <v>998</v>
@@ -5868,10 +6024,10 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="C27" s="6">
         <v>1468</v>
@@ -5897,10 +6053,10 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="C28" s="6">
         <v>1274</v>
@@ -5974,7 +6130,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="6">
@@ -6005,7 +6161,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="6">
@@ -6036,7 +6192,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="6">
@@ -6067,7 +6223,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="6">
@@ -6098,7 +6254,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6">
@@ -6129,7 +6285,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="6">
@@ -6160,7 +6316,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="6">
@@ -6191,7 +6347,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="6">
@@ -6222,7 +6378,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="6">
@@ -6253,7 +6409,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="6">
@@ -6284,7 +6440,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="6">
@@ -6315,7 +6471,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="6">
@@ -6346,7 +6502,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="6">
@@ -6377,7 +6533,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="6">
@@ -6408,7 +6564,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="6">
@@ -6439,7 +6595,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="6">
@@ -6470,7 +6626,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="6">
@@ -6501,7 +6657,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="6">
@@ -6532,7 +6688,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="6">
@@ -6563,7 +6719,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="6">
@@ -6594,7 +6750,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="6">
@@ -6625,7 +6781,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="6">
@@ -6656,7 +6812,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="6">
@@ -6687,7 +6843,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="6">
@@ -6718,7 +6874,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="6">
@@ -6749,7 +6905,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="6">
@@ -6780,7 +6936,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="6">
@@ -6811,7 +6967,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="6">
@@ -6842,7 +6998,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="6">
@@ -6873,7 +7029,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="6">
@@ -6904,7 +7060,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="6">
@@ -6935,7 +7091,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="6">
@@ -6966,7 +7122,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="6">
@@ -6997,7 +7153,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="6">
@@ -7028,7 +7184,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="6">
@@ -7059,7 +7215,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="6">
@@ -7090,7 +7246,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="6">
@@ -7121,7 +7277,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="6">
@@ -7152,7 +7308,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="6">
@@ -7183,7 +7339,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="6">
@@ -7214,7 +7370,7 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="6">
@@ -7245,7 +7401,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="6">
@@ -7276,7 +7432,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="6">
@@ -7307,7 +7463,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="6">
@@ -7338,7 +7494,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="6">
@@ -7369,7 +7525,7 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="6">
@@ -7400,7 +7556,7 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="6">
@@ -7431,7 +7587,7 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="6">
@@ -7462,7 +7618,7 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="6">
@@ -7493,7 +7649,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="6">
@@ -7524,7 +7680,7 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="6">
@@ -7555,7 +7711,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="6">
@@ -7586,7 +7742,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="6">
@@ -7617,7 +7773,7 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" s="6">
@@ -7648,7 +7804,7 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="6">
@@ -7679,7 +7835,7 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" s="6">
@@ -7710,7 +7866,7 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" s="6">
@@ -7741,7 +7897,7 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" s="6">
@@ -7772,7 +7928,7 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="6">
@@ -7803,7 +7959,7 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="6">
@@ -7834,7 +7990,7 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="6">
@@ -7865,7 +8021,7 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="6">
@@ -7896,7 +8052,7 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="6">
@@ -7927,7 +8083,7 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="6">
@@ -7958,7 +8114,7 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="6">
@@ -7989,7 +8145,7 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" s="6">
@@ -8064,7 +8220,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="6">
@@ -8092,7 +8248,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="6">
@@ -8120,7 +8276,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="6">
@@ -8148,7 +8304,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="6">
@@ -8176,7 +8332,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6">
@@ -8204,7 +8360,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="6">
@@ -8232,7 +8388,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="6">
@@ -8260,7 +8416,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="6">
@@ -8288,7 +8444,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="6">
@@ -8316,12 +8472,12 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F12" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="6">
@@ -8349,7 +8505,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="6">
@@ -8377,7 +8533,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="6">
@@ -8405,7 +8561,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="6">
@@ -8433,7 +8589,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="6">
@@ -8461,7 +8617,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="6">
@@ -8489,7 +8645,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="6">
@@ -8517,7 +8673,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="6">
@@ -8545,7 +8701,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="6">
@@ -8573,7 +8729,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="6">
@@ -8645,7 +8801,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="6">
@@ -8673,7 +8829,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="6">
@@ -8701,7 +8857,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="6">
@@ -8729,7 +8885,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="6">
@@ -8757,7 +8913,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6">
@@ -8785,7 +8941,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="6">
@@ -8813,7 +8969,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="6">
@@ -8841,7 +8997,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="6">
@@ -8869,7 +9025,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="6">
@@ -8897,7 +9053,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="6">
@@ -8925,7 +9081,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="6">
@@ -8953,7 +9109,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="6">
@@ -8981,7 +9137,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="6">
@@ -9009,7 +9165,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="6">
@@ -9037,7 +9193,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="6">
@@ -9065,7 +9221,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="6">
@@ -9093,7 +9249,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="6">
@@ -9121,7 +9277,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="6">
@@ -9149,7 +9305,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="6">
@@ -9177,7 +9333,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="6">
@@ -9205,7 +9361,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="6">
@@ -9233,7 +9389,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="6">
@@ -9261,7 +9417,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="6">
@@ -9289,7 +9445,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="6">
@@ -9317,7 +9473,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="6">
@@ -9345,7 +9501,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="6">
@@ -9380,7 +9536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C18765D9-5E60-43F7-8EAE-7692D37C4247}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -9415,12 +9571,12 @@
         <v>7</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="B2" s="27">
         <v>1047</v>
@@ -9449,7 +9605,7 @@
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="B3" s="26">
         <v>1142</v>
@@ -9478,7 +9634,7 @@
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="B4" s="26">
         <v>1070</v>
@@ -9507,7 +9663,7 @@
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="B5" s="26">
         <v>990</v>
@@ -9536,7 +9692,7 @@
     </row>
     <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="B6" s="26">
         <v>1343</v>
@@ -9565,7 +9721,7 @@
     </row>
     <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="B7" s="26">
         <v>1052</v>
@@ -9594,7 +9750,7 @@
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="B8" s="26">
         <v>1125</v>
@@ -9623,7 +9779,7 @@
     </row>
     <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="B9" s="26">
         <v>1333</v>
@@ -9652,7 +9808,7 @@
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="B10" s="26">
         <v>1253</v>
@@ -9681,7 +9837,7 @@
     </row>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="B11" s="26">
         <v>1138</v>
@@ -9710,7 +9866,7 @@
     </row>
     <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="B12" s="26">
         <v>1227</v>
@@ -9739,7 +9895,7 @@
     </row>
     <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="B13" s="26">
         <v>1313</v>
@@ -9769,7 +9925,7 @@
     <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="B15" s="25">
         <v>1332</v>
@@ -9796,12 +9952,12 @@
         <v>34</v>
       </c>
       <c r="J15" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="B16" s="26">
         <v>1288</v>
@@ -9828,12 +9984,12 @@
         <v>35</v>
       </c>
       <c r="J16" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="B17" s="26">
         <v>1207</v>
@@ -9860,12 +10016,12 @@
         <v>35</v>
       </c>
       <c r="J17" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="B18" s="26">
         <v>1648</v>
@@ -9892,12 +10048,12 @@
         <v>36</v>
       </c>
       <c r="J18" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="B19" s="26">
         <v>1403</v>
@@ -9924,12 +10080,12 @@
         <v>36</v>
       </c>
       <c r="J19" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="B20" s="26">
         <v>1594</v>
@@ -9956,12 +10112,12 @@
         <v>38</v>
       </c>
       <c r="J20" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="B21" s="26">
         <v>1558</v>
@@ -9988,12 +10144,12 @@
         <v>38</v>
       </c>
       <c r="J21" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="B22" s="26">
         <v>1657</v>
@@ -10020,12 +10176,12 @@
         <v>38</v>
       </c>
       <c r="J22" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="B23" s="26">
         <v>1620</v>
@@ -10052,7 +10208,7 @@
         <v>37</v>
       </c>
       <c r="J23" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -10093,21 +10249,21 @@
         <v>34</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="6">
@@ -10134,7 +10290,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="6">
@@ -10161,7 +10317,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="6">
@@ -10188,7 +10344,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="6">
@@ -10215,7 +10371,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="6">
@@ -10242,7 +10398,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="6">
@@ -10269,7 +10425,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="6">
@@ -10296,7 +10452,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="6">
@@ -10323,7 +10479,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="6">
@@ -10350,7 +10506,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="6">
@@ -10377,7 +10533,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="6">
@@ -10404,7 +10560,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="6">
@@ -10431,7 +10587,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="6">
@@ -10458,7 +10614,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="6">
@@ -10485,7 +10641,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="6">
@@ -10512,7 +10668,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="6">
@@ -10539,7 +10695,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="6">
@@ -10566,7 +10722,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="6">
@@ -10593,7 +10749,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="6">
@@ -10620,7 +10776,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="6">
@@ -10647,7 +10803,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="6">
@@ -10674,7 +10830,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="6">
@@ -10701,7 +10857,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="6">

</xml_diff>

<commit_message>
- Added and reworked blunt weapons
</commit_message>
<xml_diff>
--- a/Items+Troops Spreadsheets/HYW Item Balance.xlsx
+++ b/Items+Troops Spreadsheets/HYW Item Balance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoann\OneDrive\Ambiente de Trabalho\Deeds_Modsys\Items+Troops Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9124E127-B05B-4D3D-8542-8079C2A74CA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81365770-3EE0-416E-99D6-67779B0C8B93}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
   </bookViews>
   <sheets>
     <sheet name="Maces" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="388">
   <si>
     <t>ID</t>
   </si>
@@ -1187,6 +1187,27 @@
   </si>
   <si>
     <t>w_twohanded_knight_battle_axe_03</t>
+  </si>
+  <si>
+    <t>w_mace_german</t>
+  </si>
+  <si>
+    <t>German Mace</t>
+  </si>
+  <si>
+    <t>w_knight_warhammer_3</t>
+  </si>
+  <si>
+    <t>w_knight_flanged_mace</t>
+  </si>
+  <si>
+    <t>Knight Flanged Mace</t>
+  </si>
+  <si>
+    <t>w_kriegshammer</t>
+  </si>
+  <si>
+    <t>Kriegshammer</t>
   </si>
 </sst>
 </file>
@@ -1861,11 +1882,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E78F97E-9C1C-481B-BAF8-93CCEE571C45}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1958,41 +1979,25 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="9">
-        <v>293</v>
-      </c>
-      <c r="D4" s="10">
-        <v>2</v>
-      </c>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
       <c r="E4" s="11"/>
-      <c r="F4" s="12">
-        <v>95</v>
-      </c>
-      <c r="G4" s="13">
-        <v>70</v>
-      </c>
-      <c r="H4" s="14">
-        <v>30</v>
-      </c>
-      <c r="I4" s="14">
-        <v>0</v>
-      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="9">
-        <v>317</v>
+        <v>293</v>
       </c>
       <c r="D5" s="10">
         <v>2</v>
@@ -2005,7 +2010,7 @@
         <v>70</v>
       </c>
       <c r="H5" s="14">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I5" s="14">
         <v>0</v>
@@ -2013,109 +2018,91 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C6" s="9">
-        <v>372</v>
+        <v>317</v>
       </c>
       <c r="D6" s="10">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="12">
         <v>95</v>
       </c>
       <c r="G6" s="13">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="H6" s="14">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I6" s="14">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="9">
-        <v>334</v>
-      </c>
-      <c r="D7" s="10">
-        <v>2</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="10"/>
       <c r="E7" s="11"/>
-      <c r="F7" s="12">
-        <v>95</v>
-      </c>
-      <c r="G7" s="13">
-        <v>63</v>
-      </c>
-      <c r="H7" s="14">
-        <v>32</v>
-      </c>
-      <c r="I7" s="14">
-        <v>0</v>
-      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C8" s="9">
-        <v>422</v>
+        <v>372</v>
       </c>
       <c r="D8" s="10">
-        <v>9</v>
-      </c>
-      <c r="E8" s="11">
-        <v>14</v>
-      </c>
+        <v>2.5</v>
+      </c>
+      <c r="E8" s="11"/>
       <c r="F8" s="12">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="G8" s="13">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H8" s="14">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="I8" s="14">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9" s="9">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D9" s="10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="12">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G9" s="13">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H9" s="14">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="I9" s="14">
         <v>0</v>
@@ -2123,137 +2110,358 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>16</v>
+        <v>383</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10" s="9">
-        <v>262</v>
+        <v>365</v>
       </c>
       <c r="D10" s="10">
-        <v>3.25</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="12">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G10" s="13">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H10" s="14">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="I10" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="9">
-        <v>83</v>
-      </c>
-      <c r="D11" s="10">
-        <v>3.25</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="11"/>
-      <c r="F11" s="12">
-        <v>96</v>
-      </c>
-      <c r="G11" s="13">
-        <v>75</v>
-      </c>
-      <c r="H11" s="14">
-        <v>21</v>
-      </c>
-      <c r="I11" s="14">
-        <v>0</v>
-      </c>
+      <c r="F11" s="12"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C12" s="9">
-        <v>98</v>
+        <v>422</v>
       </c>
       <c r="D12" s="10">
-        <v>2.5</v>
-      </c>
-      <c r="E12" s="11"/>
+        <v>9</v>
+      </c>
+      <c r="E12" s="11">
+        <v>14</v>
+      </c>
       <c r="F12" s="12">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="G12" s="13">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="H12" s="14">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="I12" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="9">
-        <v>152</v>
-      </c>
-      <c r="D13" s="10">
-        <v>2.75</v>
-      </c>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="10"/>
       <c r="E13" s="11"/>
-      <c r="F13" s="12">
-        <v>98</v>
-      </c>
-      <c r="G13" s="13">
-        <v>71</v>
-      </c>
-      <c r="H13" s="14">
-        <v>23</v>
-      </c>
-      <c r="I13" s="14">
-        <v>0</v>
-      </c>
+      <c r="F13" s="12"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C14" s="9">
-        <v>212</v>
+        <v>336</v>
       </c>
       <c r="D14" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="12">
+        <v>96</v>
+      </c>
+      <c r="G14" s="13">
+        <v>69</v>
+      </c>
+      <c r="H14" s="14">
+        <v>28</v>
+      </c>
+      <c r="I14" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="C15" s="9">
+        <v>344</v>
+      </c>
+      <c r="D15" s="10">
+        <v>4.2</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="12">
+        <v>95</v>
+      </c>
+      <c r="G15" s="13">
+        <v>72</v>
+      </c>
+      <c r="H15" s="14">
+        <v>29</v>
+      </c>
+      <c r="I15" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="9">
+        <v>262</v>
+      </c>
+      <c r="D17" s="10">
+        <v>3.25</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="12">
         <v>97</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G17" s="13">
+        <v>72</v>
+      </c>
+      <c r="H17" s="14">
+        <v>26</v>
+      </c>
+      <c r="I17" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="C18" s="9">
+        <v>278</v>
+      </c>
+      <c r="D18" s="10">
+        <v>3.4</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="12">
+        <v>97</v>
+      </c>
+      <c r="G18" s="13">
+        <v>72</v>
+      </c>
+      <c r="H18" s="14">
+        <v>27</v>
+      </c>
+      <c r="I18" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="9">
+        <v>83</v>
+      </c>
+      <c r="D20" s="10">
+        <v>3.25</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="12">
+        <v>96</v>
+      </c>
+      <c r="G20" s="13">
+        <v>75</v>
+      </c>
+      <c r="H20" s="14">
+        <v>21</v>
+      </c>
+      <c r="I20" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="9">
+        <v>98</v>
+      </c>
+      <c r="D21" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="12">
+        <v>98</v>
+      </c>
+      <c r="G21" s="13">
+        <v>70</v>
+      </c>
+      <c r="H21" s="14">
+        <v>21</v>
+      </c>
+      <c r="I21" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="9">
+        <v>152</v>
+      </c>
+      <c r="D22" s="10">
+        <v>2.75</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="12">
+        <v>98</v>
+      </c>
+      <c r="G22" s="13">
         <v>71</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H22" s="14">
+        <v>23</v>
+      </c>
+      <c r="I22" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="9">
+        <v>212</v>
+      </c>
+      <c r="D23" s="10">
+        <v>3</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="12">
+        <v>97</v>
+      </c>
+      <c r="G23" s="13">
+        <v>71</v>
+      </c>
+      <c r="H23" s="14">
         <v>24</v>
       </c>
-      <c r="I14" s="14">
-        <v>0</v>
+      <c r="I23" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="C25" s="9">
+        <v>512</v>
+      </c>
+      <c r="D25" s="10">
+        <v>4.5</v>
+      </c>
+      <c r="E25" s="11">
+        <v>12</v>
+      </c>
+      <c r="F25" s="12">
+        <v>82</v>
+      </c>
+      <c r="G25" s="13">
+        <v>83</v>
+      </c>
+      <c r="H25" s="14">
+        <v>42</v>
+      </c>
+      <c r="I25" s="14">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -3117,7 +3325,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64CAC7F2-FAD3-4FE8-9D42-216993956934}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
- Fix for unavailable banner and offset banner back colour - Fix for pikemen looping through their weapons - Added/replaced Glaives
</commit_message>
<xml_diff>
--- a/Items+Troops Spreadsheets/HYW Item Balance.xlsx
+++ b/Items+Troops Spreadsheets/HYW Item Balance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoann\OneDrive\Ambiente de Trabalho\Deeds_Modsys\Items+Troops Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81365770-3EE0-416E-99D6-67779B0C8B93}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0545DF73-4D79-4BB3-9CF4-F4128EF9BF0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="6" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
   </bookViews>
   <sheets>
     <sheet name="Maces" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="Swords &amp; Daggers" sheetId="3" r:id="rId3"/>
     <sheet name="Bastard &amp; Twohanded Swords" sheetId="4" r:id="rId4"/>
     <sheet name="Pikes &amp; Halberds" sheetId="5" r:id="rId5"/>
-    <sheet name="Forks, Fauchards &amp; Glaives" sheetId="8" r:id="rId6"/>
-    <sheet name="Spears &amp; Lances" sheetId="9" r:id="rId7"/>
-    <sheet name="Pollaxes" sheetId="12" r:id="rId8"/>
-    <sheet name="Bows &amp; Crossbows" sheetId="6" r:id="rId9"/>
-    <sheet name="Horses" sheetId="7" r:id="rId10"/>
-    <sheet name="Arrows &amp; Bolts" sheetId="10" r:id="rId11"/>
-    <sheet name="Shields" sheetId="11" r:id="rId12"/>
+    <sheet name="Forks &amp; Fauchards" sheetId="8" r:id="rId6"/>
+    <sheet name="Glaives &amp; Couteau" sheetId="13" r:id="rId7"/>
+    <sheet name="Spears &amp; Lances" sheetId="9" r:id="rId8"/>
+    <sheet name="Pollaxes" sheetId="12" r:id="rId9"/>
+    <sheet name="Bows &amp; Crossbows" sheetId="6" r:id="rId10"/>
+    <sheet name="Horses" sheetId="7" r:id="rId11"/>
+    <sheet name="Arrows &amp; Bolts" sheetId="10" r:id="rId12"/>
+    <sheet name="Shields" sheetId="11" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="386">
   <si>
     <t>ID</t>
   </si>
@@ -769,15 +770,6 @@
     <t>w_glaive_6</t>
   </si>
   <si>
-    <t>w_glaive_7</t>
-  </si>
-  <si>
-    <t>w_glaive_8</t>
-  </si>
-  <si>
-    <t>w_glaive_burgundy</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -1208,6 +1200,9 @@
   </si>
   <si>
     <t>Kriegshammer</t>
+  </si>
+  <si>
+    <t>w_couteau_de_breche</t>
   </si>
 </sst>
 </file>
@@ -1229,7 +1224,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1320,6 +1315,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -1391,7 +1392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1441,6 +1442,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1884,7 +1887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E78F97E-9C1C-481B-BAF8-93CCEE571C45}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
@@ -2110,7 +2113,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>31</v>
@@ -2215,10 +2218,10 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C15" s="9">
         <v>344</v>
@@ -2280,10 +2283,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C18" s="9">
         <v>278</v>
@@ -2437,10 +2440,10 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C25" s="9">
         <v>512</v>
@@ -2470,6 +2473,676 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96551E4B-D0DF-400F-B6DB-43F70FA502C4}">
+  <dimension ref="A1:I29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="6">
+        <v>42</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
+        <v>95</v>
+      </c>
+      <c r="G2" s="3">
+        <v>40</v>
+      </c>
+      <c r="H2" s="1">
+        <v>90</v>
+      </c>
+      <c r="I2" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="6">
+        <v>50</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>94</v>
+      </c>
+      <c r="G3" s="3">
+        <v>42</v>
+      </c>
+      <c r="H3" s="1">
+        <v>90</v>
+      </c>
+      <c r="I3" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="6">
+        <v>58</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5">
+        <v>93</v>
+      </c>
+      <c r="G4" s="3">
+        <v>44</v>
+      </c>
+      <c r="H4" s="1">
+        <v>91</v>
+      </c>
+      <c r="I4" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="6">
+        <v>66</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
+        <v>92</v>
+      </c>
+      <c r="G5" s="3">
+        <v>45</v>
+      </c>
+      <c r="H5" s="1">
+        <v>92</v>
+      </c>
+      <c r="I5" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="6">
+        <v>90</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5">
+        <v>90</v>
+      </c>
+      <c r="G7" s="3">
+        <v>45</v>
+      </c>
+      <c r="H7" s="1">
+        <v>92</v>
+      </c>
+      <c r="I7" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="6">
+        <v>102</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="5">
+        <v>89</v>
+      </c>
+      <c r="G8" s="3">
+        <v>48</v>
+      </c>
+      <c r="H8" s="1">
+        <v>92</v>
+      </c>
+      <c r="I8" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="6">
+        <v>124</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="E9" s="7">
+        <v>2</v>
+      </c>
+      <c r="F9" s="5">
+        <v>88</v>
+      </c>
+      <c r="G9" s="3">
+        <v>51</v>
+      </c>
+      <c r="H9" s="1">
+        <v>93</v>
+      </c>
+      <c r="I9" s="4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="6">
+        <v>136</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="7">
+        <v>2</v>
+      </c>
+      <c r="F10" s="5">
+        <v>87</v>
+      </c>
+      <c r="G10" s="3">
+        <v>54</v>
+      </c>
+      <c r="H10" s="1">
+        <v>94</v>
+      </c>
+      <c r="I10" s="4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="6">
+        <v>140</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="E12" s="7">
+        <v>3</v>
+      </c>
+      <c r="F12" s="5">
+        <v>85</v>
+      </c>
+      <c r="G12" s="3">
+        <v>71</v>
+      </c>
+      <c r="H12" s="1">
+        <v>95</v>
+      </c>
+      <c r="I12" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="6">
+        <v>154</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="E13" s="7">
+        <v>3</v>
+      </c>
+      <c r="F13" s="5">
+        <v>84</v>
+      </c>
+      <c r="G13" s="3">
+        <v>76</v>
+      </c>
+      <c r="H13" s="1">
+        <v>95</v>
+      </c>
+      <c r="I13" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="6">
+        <v>168</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="E14" s="7">
+        <v>3</v>
+      </c>
+      <c r="F14" s="5">
+        <v>83</v>
+      </c>
+      <c r="G14" s="3">
+        <v>82</v>
+      </c>
+      <c r="H14" s="1">
+        <v>96</v>
+      </c>
+      <c r="I14" s="4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="6">
+        <v>184</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="E15" s="7">
+        <v>3</v>
+      </c>
+      <c r="F15" s="5">
+        <v>82</v>
+      </c>
+      <c r="G15" s="3">
+        <v>89</v>
+      </c>
+      <c r="H15" s="1">
+        <v>97</v>
+      </c>
+      <c r="I15" s="4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="6">
+        <v>220</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="E17" s="7">
+        <v>4</v>
+      </c>
+      <c r="F17" s="5">
+        <v>80</v>
+      </c>
+      <c r="G17" s="3">
+        <v>96</v>
+      </c>
+      <c r="H17" s="1">
+        <v>98</v>
+      </c>
+      <c r="I17" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="6">
+        <v>235</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="E18" s="7">
+        <v>4</v>
+      </c>
+      <c r="F18" s="5">
+        <v>79</v>
+      </c>
+      <c r="G18" s="3">
+        <v>104</v>
+      </c>
+      <c r="H18" s="1">
+        <v>98</v>
+      </c>
+      <c r="I18" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="6">
+        <v>250</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="E19" s="7">
+        <v>5</v>
+      </c>
+      <c r="F19" s="5">
+        <v>78</v>
+      </c>
+      <c r="G19" s="3">
+        <v>115</v>
+      </c>
+      <c r="H19" s="1">
+        <v>99</v>
+      </c>
+      <c r="I19" s="4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="6">
+        <v>265</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="E20" s="7">
+        <v>5</v>
+      </c>
+      <c r="F20" s="5">
+        <v>77</v>
+      </c>
+      <c r="G20" s="3">
+        <v>121</v>
+      </c>
+      <c r="H20" s="1">
+        <v>99</v>
+      </c>
+      <c r="I20" s="4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="6">
+        <v>88</v>
+      </c>
+      <c r="D22" s="4">
+        <v>2.25</v>
+      </c>
+      <c r="E22" s="7">
+        <v>0</v>
+      </c>
+      <c r="F22" s="5">
+        <v>80</v>
+      </c>
+      <c r="G22" s="3">
+        <v>81</v>
+      </c>
+      <c r="H22" s="1">
+        <v>98</v>
+      </c>
+      <c r="I22" s="4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="6">
+        <v>132</v>
+      </c>
+      <c r="D23" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="E23" s="7">
+        <v>8</v>
+      </c>
+      <c r="F23" s="5">
+        <v>76</v>
+      </c>
+      <c r="G23" s="3">
+        <v>92</v>
+      </c>
+      <c r="H23" s="1">
+        <v>98</v>
+      </c>
+      <c r="I23" s="4">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="6">
+        <v>218</v>
+      </c>
+      <c r="D24" s="4">
+        <v>3</v>
+      </c>
+      <c r="E24" s="7">
+        <v>9</v>
+      </c>
+      <c r="F24" s="5">
+        <v>72</v>
+      </c>
+      <c r="G24" s="3">
+        <v>112</v>
+      </c>
+      <c r="H24" s="1">
+        <v>99</v>
+      </c>
+      <c r="I24" s="4">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="6">
+        <v>349</v>
+      </c>
+      <c r="D25" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="E25" s="7">
+        <v>10</v>
+      </c>
+      <c r="F25" s="5">
+        <v>68</v>
+      </c>
+      <c r="G25" s="3">
+        <v>125</v>
+      </c>
+      <c r="H25" s="1">
+        <v>99</v>
+      </c>
+      <c r="I25" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="6">
+        <v>683</v>
+      </c>
+      <c r="D26" s="4">
+        <v>3.75</v>
+      </c>
+      <c r="E26" s="7">
+        <v>11</v>
+      </c>
+      <c r="F26" s="5">
+        <v>62</v>
+      </c>
+      <c r="G26" s="3">
+        <v>128</v>
+      </c>
+      <c r="H26" s="1">
+        <v>98</v>
+      </c>
+      <c r="I26" s="4">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="6">
+        <v>1850</v>
+      </c>
+      <c r="D28" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="E28" s="7">
+        <v>0</v>
+      </c>
+      <c r="F28" s="5">
+        <v>58</v>
+      </c>
+      <c r="G28" s="3">
+        <v>160</v>
+      </c>
+      <c r="H28" s="1">
+        <v>95</v>
+      </c>
+      <c r="I28" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="6">
+        <v>2250</v>
+      </c>
+      <c r="D29" s="4">
+        <v>3.8</v>
+      </c>
+      <c r="E29" s="7">
+        <v>0</v>
+      </c>
+      <c r="F29" s="5">
+        <v>60</v>
+      </c>
+      <c r="G29" s="3">
+        <v>180</v>
+      </c>
+      <c r="H29" s="1">
+        <v>98</v>
+      </c>
+      <c r="I29" s="4">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DAD396-9A3B-4E45-8468-1404C7D6E830}">
   <dimension ref="A1:J9"/>
   <sheetViews>
@@ -2766,7 +3439,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3C8FEF-B598-4AEC-9E3E-97CE35ABD837}">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -2796,12 +3469,12 @@
         <v>178</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B2" s="6">
         <v>72</v>
@@ -2821,7 +3494,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B3" s="6">
         <v>104</v>
@@ -2841,7 +3514,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B4" s="6">
         <v>162</v>
@@ -2861,7 +3534,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B5" s="6">
         <v>98</v>
@@ -2881,7 +3554,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B6" s="6">
         <v>146</v>
@@ -2901,7 +3574,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B7" s="6">
         <v>86</v>
@@ -2921,7 +3594,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B9" s="6">
         <v>64</v>
@@ -2941,7 +3614,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B10" s="6">
         <v>92</v>
@@ -2961,7 +3634,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B11" s="6">
         <v>125</v>
@@ -2981,7 +3654,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B12" s="6">
         <v>100</v>
@@ -3001,7 +3674,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B13" s="6">
         <v>118</v>
@@ -3024,7 +3697,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6EE9141-0B58-4213-922A-6EE4F5E15BD3}">
   <dimension ref="A1:I9"/>
   <sheetViews>
@@ -3046,7 +3719,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B1" s="24" t="s">
         <v>2</v>
@@ -3064,18 +3737,18 @@
         <v>4</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="I1" s="24" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B2" s="18">
         <v>550</v>
@@ -3105,7 +3778,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B3" s="18">
         <v>420</v>
@@ -3135,7 +3808,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B4" s="18">
         <v>340</v>
@@ -3165,7 +3838,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B5" s="18">
         <v>220</v>
@@ -3195,7 +3868,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B6" s="18">
         <v>380</v>
@@ -3225,7 +3898,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B7" s="18">
         <v>400</v>
@@ -3255,7 +3928,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B8" s="18">
         <v>1500</v>
@@ -3285,7 +3958,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B9" s="18">
         <v>180</v>
@@ -3393,7 +4066,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>49</v>
@@ -3420,7 +4093,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>49</v>
@@ -3447,7 +4120,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>49</v>
@@ -3474,7 +4147,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>49</v>
@@ -3512,7 +4185,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>51</v>
@@ -3539,7 +4212,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>51</v>
@@ -3566,7 +4239,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>51</v>
@@ -3604,7 +4277,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>52</v>
@@ -3631,7 +4304,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>52</v>
@@ -3669,10 +4342,10 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C15" s="15">
         <v>337</v>
@@ -3696,10 +4369,10 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C16" s="15">
         <v>314</v>
@@ -3734,7 +4407,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>53</v>
@@ -3761,7 +4434,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>53</v>
@@ -3788,7 +4461,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>53</v>
@@ -5380,10 +6053,10 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C36" s="6">
         <v>312</v>
@@ -5417,10 +6090,10 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C37" s="6">
         <v>555</v>
@@ -5454,10 +6127,10 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C38" s="6">
         <v>644</v>
@@ -6018,10 +6691,10 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C19" s="6">
         <v>912</v>
@@ -6058,7 +6731,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>170</v>
@@ -6087,7 +6760,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>170</v>
@@ -6203,7 +6876,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>174</v>
@@ -6232,10 +6905,10 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C27" s="6">
         <v>1468</v>
@@ -6261,10 +6934,10 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C28" s="6">
         <v>1274</v>
@@ -7361,7 +8034,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="6">
@@ -7392,7 +8065,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="6">
@@ -7423,7 +8096,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="6">
@@ -7454,7 +8127,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="6">
@@ -7485,7 +8158,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="6">
@@ -7516,7 +8189,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="6">
@@ -7547,7 +8220,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="6">
@@ -7578,7 +8251,7 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="6">
@@ -7609,7 +8282,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="6">
@@ -7640,7 +8313,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="6">
@@ -7671,7 +8344,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="6">
@@ -7702,7 +8375,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="6">
@@ -7764,7 +8437,7 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="6">
@@ -7795,7 +8468,7 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="6">
@@ -7826,7 +8499,7 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="6">
@@ -7857,7 +8530,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="6">
@@ -7888,7 +8561,7 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="6">
@@ -7919,7 +8592,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="6">
@@ -7950,7 +8623,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="6">
@@ -7981,7 +8654,7 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" s="6">
@@ -8012,7 +8685,7 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="6">
@@ -8043,7 +8716,7 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" s="6">
@@ -8074,7 +8747,7 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" s="6">
@@ -8105,7 +8778,7 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" s="6">
@@ -8136,7 +8809,7 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="6">
@@ -8167,7 +8840,7 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="6">
@@ -8198,7 +8871,7 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="6">
@@ -8229,7 +8902,7 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="6">
@@ -8260,7 +8933,7 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="6">
@@ -8291,7 +8964,7 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="6">
@@ -8322,7 +8995,7 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="6">
@@ -8353,7 +9026,7 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" s="6">
@@ -8389,10 +9062,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE67CB9-8D30-45BB-9729-53435DBF7C02}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8680,286 +9353,34 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F12" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>235</v>
+        <v>285</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="6">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="D13" s="4">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="E13" s="7">
         <v>9</v>
       </c>
       <c r="F13" s="5">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G13" s="3">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="H13" s="1">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="I13">
-        <f t="shared" ref="I13:I20" si="0">SUM(D13:H13)*0.8</f>
-        <v>240.8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="6">
-        <v>242</v>
-      </c>
-      <c r="D14" s="4">
-        <v>3</v>
-      </c>
-      <c r="E14" s="7">
-        <v>9</v>
-      </c>
-      <c r="F14" s="5">
-        <v>83</v>
-      </c>
-      <c r="G14" s="3">
-        <v>175</v>
-      </c>
-      <c r="H14" s="1">
-        <v>33</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="0"/>
-        <v>242.4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="6">
-        <v>304</v>
-      </c>
-      <c r="D15" s="4">
-        <v>4</v>
-      </c>
-      <c r="E15" s="7">
-        <v>9</v>
-      </c>
-      <c r="F15" s="5">
-        <v>78</v>
-      </c>
-      <c r="G15" s="3">
-        <v>255</v>
-      </c>
-      <c r="H15" s="1">
-        <v>34</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="0"/>
-        <v>304</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="6">
-        <v>246</v>
-      </c>
-      <c r="D16" s="4">
-        <v>3.2</v>
-      </c>
-      <c r="E16" s="7">
-        <v>9</v>
-      </c>
-      <c r="F16" s="5">
-        <v>82</v>
-      </c>
-      <c r="G16" s="3">
-        <v>179</v>
-      </c>
-      <c r="H16" s="1">
-        <v>34</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="0"/>
-        <v>245.76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="6">
-        <v>251</v>
-      </c>
-      <c r="D17" s="4">
-        <v>3.2</v>
-      </c>
-      <c r="E17" s="7">
-        <v>9</v>
-      </c>
-      <c r="F17" s="5">
-        <v>82</v>
-      </c>
-      <c r="G17" s="3">
-        <v>185</v>
-      </c>
-      <c r="H17" s="1">
-        <v>35</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="0"/>
-        <v>251.36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="6">
-        <v>233</v>
-      </c>
-      <c r="D18" s="4">
-        <v>2.8</v>
-      </c>
-      <c r="E18" s="7">
-        <v>9</v>
-      </c>
-      <c r="F18" s="5">
-        <v>84</v>
-      </c>
-      <c r="G18" s="3">
-        <v>160</v>
-      </c>
-      <c r="H18" s="1">
-        <v>36</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="0"/>
-        <v>233.44000000000003</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="6">
-        <v>233</v>
-      </c>
-      <c r="D19" s="4">
-        <v>2.8</v>
-      </c>
-      <c r="E19" s="7">
-        <v>9</v>
-      </c>
-      <c r="F19" s="5">
-        <v>84</v>
-      </c>
-      <c r="G19" s="3">
-        <v>164</v>
-      </c>
-      <c r="H19" s="1">
-        <v>31</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="0"/>
-        <v>232.64000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="6">
-        <v>268</v>
-      </c>
-      <c r="D20" s="4">
-        <v>3.6</v>
-      </c>
-      <c r="E20" s="7">
-        <v>9</v>
-      </c>
-      <c r="F20" s="5">
-        <v>80</v>
-      </c>
-      <c r="G20" s="3">
-        <v>208</v>
-      </c>
-      <c r="H20" s="1">
-        <v>35</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="0"/>
-        <v>268.48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="6">
-        <v>295</v>
-      </c>
-      <c r="D21" s="4">
-        <v>2.8</v>
-      </c>
-      <c r="E21" s="7">
-        <v>9</v>
-      </c>
-      <c r="F21" s="5">
-        <v>84</v>
-      </c>
-      <c r="G21" s="3">
-        <v>160</v>
-      </c>
-      <c r="H21" s="1">
-        <v>39</v>
-      </c>
-      <c r="I21">
-        <f>SUM(D21:H21)</f>
-        <v>294.8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="6">
-        <v>231</v>
-      </c>
-      <c r="D23" s="4">
-        <v>3.1</v>
-      </c>
-      <c r="E23" s="7">
-        <v>9</v>
-      </c>
-      <c r="F23" s="5">
-        <v>85</v>
-      </c>
-      <c r="G23" s="3">
-        <v>155</v>
-      </c>
-      <c r="H23" s="1">
-        <v>36</v>
-      </c>
-      <c r="I23">
-        <f>SUM(D23:H23)*0.8</f>
+        <f>SUM(D13:H13)*0.8</f>
         <v>230.48000000000002</v>
       </c>
     </row>
@@ -8969,6 +9390,282 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{042C4405-AEC3-4A36-A3E7-7EA75E4B87DD}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="6">
+        <v>265</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1.9</v>
+      </c>
+      <c r="E2" s="7">
+        <v>9</v>
+      </c>
+      <c r="F2" s="5">
+        <v>92</v>
+      </c>
+      <c r="G2" s="3">
+        <v>160</v>
+      </c>
+      <c r="H2" s="1">
+        <v>37</v>
+      </c>
+      <c r="I2" s="1">
+        <v>32</v>
+      </c>
+      <c r="J2">
+        <f>SUM(D2:I2)*0.8</f>
+        <v>265.52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="6">
+        <v>312</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="E3" s="7">
+        <v>9</v>
+      </c>
+      <c r="F3" s="5">
+        <v>84</v>
+      </c>
+      <c r="G3" s="3">
+        <v>228</v>
+      </c>
+      <c r="H3" s="1">
+        <v>36</v>
+      </c>
+      <c r="I3" s="1">
+        <v>31</v>
+      </c>
+      <c r="J3">
+        <f>SUM(D3:I3)*0.8</f>
+        <v>312.40000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="6">
+        <v>255</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="7">
+        <v>9</v>
+      </c>
+      <c r="F4" s="5">
+        <v>91</v>
+      </c>
+      <c r="G4" s="3">
+        <v>164</v>
+      </c>
+      <c r="H4" s="1">
+        <v>31</v>
+      </c>
+      <c r="I4" s="1">
+        <v>22</v>
+      </c>
+      <c r="J4">
+        <f>SUM(D4:I4)*0.8</f>
+        <v>255.20000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="6">
+        <v>275</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E5" s="7">
+        <v>9</v>
+      </c>
+      <c r="F5" s="5">
+        <v>90</v>
+      </c>
+      <c r="G5" s="3">
+        <v>175</v>
+      </c>
+      <c r="H5" s="1">
+        <v>33</v>
+      </c>
+      <c r="I5" s="1">
+        <v>35</v>
+      </c>
+      <c r="J5">
+        <f>SUM(D5:I5)*0.8</f>
+        <v>275.36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="6">
+        <v>300</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="E6" s="7">
+        <v>9</v>
+      </c>
+      <c r="F6" s="5">
+        <v>86</v>
+      </c>
+      <c r="G6" s="3">
+        <v>212</v>
+      </c>
+      <c r="H6" s="1">
+        <v>32</v>
+      </c>
+      <c r="I6" s="1">
+        <v>34</v>
+      </c>
+      <c r="J6">
+        <f>SUM(D6:I6)*0.8</f>
+        <v>300.32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="6">
+        <v>269</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E7" s="7">
+        <v>9</v>
+      </c>
+      <c r="F7" s="5">
+        <v>92</v>
+      </c>
+      <c r="G7" s="3">
+        <v>164</v>
+      </c>
+      <c r="H7" s="1">
+        <v>35</v>
+      </c>
+      <c r="I7" s="1">
+        <v>35</v>
+      </c>
+      <c r="J7">
+        <f>SUM(D7:I7)*0.8</f>
+        <v>269.84000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="30"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="6">
+        <v>276</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E9" s="7">
+        <v>9</v>
+      </c>
+      <c r="F9" s="5">
+        <v>90</v>
+      </c>
+      <c r="G9" s="3">
+        <v>173</v>
+      </c>
+      <c r="H9" s="1">
+        <v>36</v>
+      </c>
+      <c r="I9" s="1">
+        <v>35</v>
+      </c>
+      <c r="J9">
+        <f>SUM(D9:I9)*0.8</f>
+        <v>276.16000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{270FCD42-7C0A-42FB-9872-27F0BB063FAE}">
   <dimension ref="A1:I32"/>
   <sheetViews>
@@ -9009,7 +9706,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="6">
@@ -9037,7 +9734,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="6">
@@ -9065,7 +9762,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="6">
@@ -9093,7 +9790,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="6">
@@ -9121,7 +9818,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6">
@@ -9149,7 +9846,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="6">
@@ -9177,7 +9874,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="6">
@@ -9205,7 +9902,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="6">
@@ -9233,7 +9930,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="6">
@@ -9261,7 +9958,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="6">
@@ -9289,7 +9986,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="6">
@@ -9317,7 +10014,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="6">
@@ -9345,7 +10042,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="6">
@@ -9373,7 +10070,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="6">
@@ -9401,7 +10098,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="6">
@@ -9429,7 +10126,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="6">
@@ -9457,7 +10154,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="6">
@@ -9485,7 +10182,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="6">
@@ -9513,7 +10210,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="6">
@@ -9541,7 +10238,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="6">
@@ -9569,7 +10266,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="6">
@@ -9597,7 +10294,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="6">
@@ -9625,7 +10322,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="6">
@@ -9653,7 +10350,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="6">
@@ -9681,7 +10378,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="6">
@@ -9709,7 +10406,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="6">
@@ -9740,12 +10437,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C18765D9-5E60-43F7-8EAE-7692D37C4247}">
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9779,12 +10476,12 @@
         <v>7</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B2" s="27">
         <v>1047</v>
@@ -9813,7 +10510,7 @@
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B3" s="26">
         <v>1142</v>
@@ -9842,7 +10539,7 @@
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B4" s="26">
         <v>1070</v>
@@ -9871,7 +10568,7 @@
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B5" s="26">
         <v>990</v>
@@ -9900,7 +10597,7 @@
     </row>
     <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B6" s="26">
         <v>1343</v>
@@ -9929,7 +10626,7 @@
     </row>
     <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B7" s="26">
         <v>1052</v>
@@ -9958,7 +10655,7 @@
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B8" s="26">
         <v>1125</v>
@@ -9987,7 +10684,7 @@
     </row>
     <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B9" s="26">
         <v>1333</v>
@@ -10016,7 +10713,7 @@
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B10" s="26">
         <v>1253</v>
@@ -10045,7 +10742,7 @@
     </row>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B11" s="26">
         <v>1138</v>
@@ -10074,7 +10771,7 @@
     </row>
     <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B12" s="26">
         <v>1227</v>
@@ -10103,7 +10800,7 @@
     </row>
     <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B13" s="26">
         <v>1313</v>
@@ -10133,7 +10830,7 @@
     <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B15" s="25">
         <v>1332</v>
@@ -10160,12 +10857,12 @@
         <v>34</v>
       </c>
       <c r="J15" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B16" s="26">
         <v>1288</v>
@@ -10192,12 +10889,12 @@
         <v>35</v>
       </c>
       <c r="J16" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B17" s="26">
         <v>1207</v>
@@ -10224,12 +10921,12 @@
         <v>35</v>
       </c>
       <c r="J17" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B18" s="26">
         <v>1648</v>
@@ -10256,12 +10953,12 @@
         <v>36</v>
       </c>
       <c r="J18" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B19" s="26">
         <v>1403</v>
@@ -10288,12 +10985,12 @@
         <v>36</v>
       </c>
       <c r="J19" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="B20" s="26">
         <v>1594</v>
@@ -10320,12 +11017,12 @@
         <v>38</v>
       </c>
       <c r="J20" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B21" s="26">
         <v>1558</v>
@@ -10352,12 +11049,12 @@
         <v>38</v>
       </c>
       <c r="J21" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B22" s="26">
         <v>1657</v>
@@ -10384,12 +11081,12 @@
         <v>38</v>
       </c>
       <c r="J22" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B23" s="26">
         <v>1620</v>
@@ -10416,681 +11113,11 @@
         <v>37</v>
       </c>
       <c r="J23" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96551E4B-D0DF-400F-B6DB-43F70FA502C4}">
-  <dimension ref="A1:I29"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="20.5546875" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="6">
-        <v>42</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="E2" s="7">
-        <v>0</v>
-      </c>
-      <c r="F2" s="5">
-        <v>95</v>
-      </c>
-      <c r="G2" s="3">
-        <v>40</v>
-      </c>
-      <c r="H2" s="1">
-        <v>90</v>
-      </c>
-      <c r="I2" s="4">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="6">
-        <v>50</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="E3" s="7">
-        <v>0</v>
-      </c>
-      <c r="F3" s="5">
-        <v>94</v>
-      </c>
-      <c r="G3" s="3">
-        <v>42</v>
-      </c>
-      <c r="H3" s="1">
-        <v>90</v>
-      </c>
-      <c r="I3" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="6">
-        <v>58</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="E4" s="7">
-        <v>1</v>
-      </c>
-      <c r="F4" s="5">
-        <v>93</v>
-      </c>
-      <c r="G4" s="3">
-        <v>44</v>
-      </c>
-      <c r="H4" s="1">
-        <v>91</v>
-      </c>
-      <c r="I4" s="4">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="6">
-        <v>66</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="E5" s="7">
-        <v>1</v>
-      </c>
-      <c r="F5" s="5">
-        <v>92</v>
-      </c>
-      <c r="G5" s="3">
-        <v>45</v>
-      </c>
-      <c r="H5" s="1">
-        <v>92</v>
-      </c>
-      <c r="I5" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="6">
-        <v>90</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="E7" s="7">
-        <v>1</v>
-      </c>
-      <c r="F7" s="5">
-        <v>90</v>
-      </c>
-      <c r="G7" s="3">
-        <v>45</v>
-      </c>
-      <c r="H7" s="1">
-        <v>92</v>
-      </c>
-      <c r="I7" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="6">
-        <v>102</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="E8" s="7">
-        <v>1</v>
-      </c>
-      <c r="F8" s="5">
-        <v>89</v>
-      </c>
-      <c r="G8" s="3">
-        <v>48</v>
-      </c>
-      <c r="H8" s="1">
-        <v>92</v>
-      </c>
-      <c r="I8" s="4">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="6">
-        <v>124</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="E9" s="7">
-        <v>2</v>
-      </c>
-      <c r="F9" s="5">
-        <v>88</v>
-      </c>
-      <c r="G9" s="3">
-        <v>51</v>
-      </c>
-      <c r="H9" s="1">
-        <v>93</v>
-      </c>
-      <c r="I9" s="4">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="6">
-        <v>136</v>
-      </c>
-      <c r="D10" s="4">
-        <v>1</v>
-      </c>
-      <c r="E10" s="7">
-        <v>2</v>
-      </c>
-      <c r="F10" s="5">
-        <v>87</v>
-      </c>
-      <c r="G10" s="3">
-        <v>54</v>
-      </c>
-      <c r="H10" s="1">
-        <v>94</v>
-      </c>
-      <c r="I10" s="4">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="6">
-        <v>140</v>
-      </c>
-      <c r="D12" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="E12" s="7">
-        <v>3</v>
-      </c>
-      <c r="F12" s="5">
-        <v>85</v>
-      </c>
-      <c r="G12" s="3">
-        <v>71</v>
-      </c>
-      <c r="H12" s="1">
-        <v>95</v>
-      </c>
-      <c r="I12" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="6">
-        <v>154</v>
-      </c>
-      <c r="D13" s="4">
-        <v>1.3</v>
-      </c>
-      <c r="E13" s="7">
-        <v>3</v>
-      </c>
-      <c r="F13" s="5">
-        <v>84</v>
-      </c>
-      <c r="G13" s="3">
-        <v>76</v>
-      </c>
-      <c r="H13" s="1">
-        <v>95</v>
-      </c>
-      <c r="I13" s="4">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="6">
-        <v>168</v>
-      </c>
-      <c r="D14" s="4">
-        <v>1.3</v>
-      </c>
-      <c r="E14" s="7">
-        <v>3</v>
-      </c>
-      <c r="F14" s="5">
-        <v>83</v>
-      </c>
-      <c r="G14" s="3">
-        <v>82</v>
-      </c>
-      <c r="H14" s="1">
-        <v>96</v>
-      </c>
-      <c r="I14" s="4">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="6">
-        <v>184</v>
-      </c>
-      <c r="D15" s="4">
-        <v>1.4</v>
-      </c>
-      <c r="E15" s="7">
-        <v>3</v>
-      </c>
-      <c r="F15" s="5">
-        <v>82</v>
-      </c>
-      <c r="G15" s="3">
-        <v>89</v>
-      </c>
-      <c r="H15" s="1">
-        <v>97</v>
-      </c>
-      <c r="I15" s="4">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="6">
-        <v>220</v>
-      </c>
-      <c r="D17" s="4">
-        <v>1.4</v>
-      </c>
-      <c r="E17" s="7">
-        <v>4</v>
-      </c>
-      <c r="F17" s="5">
-        <v>80</v>
-      </c>
-      <c r="G17" s="3">
-        <v>96</v>
-      </c>
-      <c r="H17" s="1">
-        <v>98</v>
-      </c>
-      <c r="I17" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="6">
-        <v>235</v>
-      </c>
-      <c r="D18" s="4">
-        <v>1.4</v>
-      </c>
-      <c r="E18" s="7">
-        <v>4</v>
-      </c>
-      <c r="F18" s="5">
-        <v>79</v>
-      </c>
-      <c r="G18" s="3">
-        <v>104</v>
-      </c>
-      <c r="H18" s="1">
-        <v>98</v>
-      </c>
-      <c r="I18" s="4">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="6">
-        <v>250</v>
-      </c>
-      <c r="D19" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="E19" s="7">
-        <v>5</v>
-      </c>
-      <c r="F19" s="5">
-        <v>78</v>
-      </c>
-      <c r="G19" s="3">
-        <v>115</v>
-      </c>
-      <c r="H19" s="1">
-        <v>99</v>
-      </c>
-      <c r="I19" s="4">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="6">
-        <v>265</v>
-      </c>
-      <c r="D20" s="4">
-        <v>1.6</v>
-      </c>
-      <c r="E20" s="7">
-        <v>5</v>
-      </c>
-      <c r="F20" s="5">
-        <v>77</v>
-      </c>
-      <c r="G20" s="3">
-        <v>121</v>
-      </c>
-      <c r="H20" s="1">
-        <v>99</v>
-      </c>
-      <c r="I20" s="4">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="6">
-        <v>88</v>
-      </c>
-      <c r="D22" s="4">
-        <v>2.25</v>
-      </c>
-      <c r="E22" s="7">
-        <v>0</v>
-      </c>
-      <c r="F22" s="5">
-        <v>80</v>
-      </c>
-      <c r="G22" s="3">
-        <v>81</v>
-      </c>
-      <c r="H22" s="1">
-        <v>98</v>
-      </c>
-      <c r="I22" s="4">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="6">
-        <v>132</v>
-      </c>
-      <c r="D23" s="4">
-        <v>2.5</v>
-      </c>
-      <c r="E23" s="7">
-        <v>8</v>
-      </c>
-      <c r="F23" s="5">
-        <v>76</v>
-      </c>
-      <c r="G23" s="3">
-        <v>92</v>
-      </c>
-      <c r="H23" s="1">
-        <v>98</v>
-      </c>
-      <c r="I23" s="4">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="6">
-        <v>218</v>
-      </c>
-      <c r="D24" s="4">
-        <v>3</v>
-      </c>
-      <c r="E24" s="7">
-        <v>9</v>
-      </c>
-      <c r="F24" s="5">
-        <v>72</v>
-      </c>
-      <c r="G24" s="3">
-        <v>112</v>
-      </c>
-      <c r="H24" s="1">
-        <v>99</v>
-      </c>
-      <c r="I24" s="4">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="6">
-        <v>349</v>
-      </c>
-      <c r="D25" s="4">
-        <v>3.5</v>
-      </c>
-      <c r="E25" s="7">
-        <v>10</v>
-      </c>
-      <c r="F25" s="5">
-        <v>68</v>
-      </c>
-      <c r="G25" s="3">
-        <v>125</v>
-      </c>
-      <c r="H25" s="1">
-        <v>99</v>
-      </c>
-      <c r="I25" s="4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="6">
-        <v>683</v>
-      </c>
-      <c r="D26" s="4">
-        <v>3.75</v>
-      </c>
-      <c r="E26" s="7">
-        <v>11</v>
-      </c>
-      <c r="F26" s="5">
-        <v>62</v>
-      </c>
-      <c r="G26" s="3">
-        <v>128</v>
-      </c>
-      <c r="H26" s="1">
-        <v>98</v>
-      </c>
-      <c r="I26" s="4">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="6">
-        <v>1850</v>
-      </c>
-      <c r="D28" s="4">
-        <v>4.5</v>
-      </c>
-      <c r="E28" s="7">
-        <v>0</v>
-      </c>
-      <c r="F28" s="5">
-        <v>58</v>
-      </c>
-      <c r="G28" s="3">
-        <v>160</v>
-      </c>
-      <c r="H28" s="1">
-        <v>95</v>
-      </c>
-      <c r="I28" s="4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="6">
-        <v>2250</v>
-      </c>
-      <c r="D29" s="4">
-        <v>3.8</v>
-      </c>
-      <c r="E29" s="7">
-        <v>0</v>
-      </c>
-      <c r="F29" s="5">
-        <v>60</v>
-      </c>
-      <c r="G29" s="3">
-        <v>180</v>
-      </c>
-      <c r="H29" s="1">
-        <v>98</v>
-      </c>
-      <c r="I29" s="4">
-        <v>120</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
- Added Halberds - Added German Kettle Hats - Replaced mail aventails - Fight near looted villages scene test - Added brick props
</commit_message>
<xml_diff>
--- a/Items+Troops Spreadsheets/HYW Item Balance.xlsx
+++ b/Items+Troops Spreadsheets/HYW Item Balance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoann\OneDrive\Ambiente de Trabalho\Deeds_Modsys\Items+Troops Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0545DF73-4D79-4BB3-9CF4-F4128EF9BF0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E800A93D-8B3C-4F24-971A-3771105D7E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="6" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
+    <workbookView xWindow="12696" yWindow="5352" windowWidth="17280" windowHeight="8964" firstSheet="4" activeTab="5" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
   </bookViews>
   <sheets>
     <sheet name="Maces" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,15 @@
     <sheet name="Swords &amp; Daggers" sheetId="3" r:id="rId3"/>
     <sheet name="Bastard &amp; Twohanded Swords" sheetId="4" r:id="rId4"/>
     <sheet name="Pikes &amp; Halberds" sheetId="5" r:id="rId5"/>
-    <sheet name="Forks &amp; Fauchards" sheetId="8" r:id="rId6"/>
-    <sheet name="Glaives &amp; Couteau" sheetId="13" r:id="rId7"/>
-    <sheet name="Spears &amp; Lances" sheetId="9" r:id="rId8"/>
-    <sheet name="Pollaxes" sheetId="12" r:id="rId9"/>
-    <sheet name="Bows &amp; Crossbows" sheetId="6" r:id="rId10"/>
-    <sheet name="Horses" sheetId="7" r:id="rId11"/>
-    <sheet name="Arrows &amp; Bolts" sheetId="10" r:id="rId12"/>
-    <sheet name="Shields" sheetId="11" r:id="rId13"/>
+    <sheet name="Halberds" sheetId="14" r:id="rId6"/>
+    <sheet name="Forks &amp; Fauchards" sheetId="8" r:id="rId7"/>
+    <sheet name="Glaives &amp; Couteau" sheetId="13" r:id="rId8"/>
+    <sheet name="Spears &amp; Lances" sheetId="9" r:id="rId9"/>
+    <sheet name="Pollaxes" sheetId="12" r:id="rId10"/>
+    <sheet name="Bows &amp; Crossbows" sheetId="6" r:id="rId11"/>
+    <sheet name="Horses" sheetId="7" r:id="rId12"/>
+    <sheet name="Arrows &amp; Bolts" sheetId="10" r:id="rId13"/>
+    <sheet name="Shields" sheetId="11" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="387">
   <si>
     <t>ID</t>
   </si>
@@ -1203,6 +1204,9 @@
   </si>
   <si>
     <t>w_couteau_de_breche</t>
+  </si>
+  <si>
+    <t>Halberd</t>
   </si>
 </sst>
 </file>
@@ -2473,6 +2477,691 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C18765D9-5E60-43F7-8EAE-7692D37C4247}">
+  <dimension ref="A1:J23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B2" s="27">
+        <v>1047</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D2" s="7">
+        <v>12</v>
+      </c>
+      <c r="E2" s="5">
+        <v>90</v>
+      </c>
+      <c r="F2" s="3">
+        <v>148</v>
+      </c>
+      <c r="G2" s="1">
+        <v>33</v>
+      </c>
+      <c r="H2" s="1">
+        <v>33</v>
+      </c>
+      <c r="I2" s="28">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B3" s="26">
+        <v>1142</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D3" s="7">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5">
+        <v>90</v>
+      </c>
+      <c r="F3" s="3">
+        <v>148</v>
+      </c>
+      <c r="G3" s="1">
+        <v>36</v>
+      </c>
+      <c r="H3" s="1">
+        <v>33</v>
+      </c>
+      <c r="I3" s="28">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B4" s="26">
+        <v>1070</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D4" s="7">
+        <v>12</v>
+      </c>
+      <c r="E4" s="5">
+        <v>91</v>
+      </c>
+      <c r="F4" s="3">
+        <v>141</v>
+      </c>
+      <c r="G4" s="1">
+        <v>34</v>
+      </c>
+      <c r="H4" s="1">
+        <v>34</v>
+      </c>
+      <c r="I4" s="28">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B5" s="26">
+        <v>990</v>
+      </c>
+      <c r="C5" s="4">
+        <v>2</v>
+      </c>
+      <c r="D5" s="7">
+        <v>12</v>
+      </c>
+      <c r="E5" s="5">
+        <v>93</v>
+      </c>
+      <c r="F5" s="3">
+        <v>124</v>
+      </c>
+      <c r="G5" s="1">
+        <v>35</v>
+      </c>
+      <c r="H5" s="1">
+        <v>34</v>
+      </c>
+      <c r="I5" s="28">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="B6" s="26">
+        <v>1343</v>
+      </c>
+      <c r="C6" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="D6" s="7">
+        <v>12</v>
+      </c>
+      <c r="E6" s="5">
+        <v>88</v>
+      </c>
+      <c r="F6" s="3">
+        <v>159</v>
+      </c>
+      <c r="G6" s="1">
+        <v>38</v>
+      </c>
+      <c r="H6" s="1">
+        <v>35</v>
+      </c>
+      <c r="I6" s="28">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B7" s="26">
+        <v>1052</v>
+      </c>
+      <c r="C7" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D7" s="7">
+        <v>12</v>
+      </c>
+      <c r="E7" s="5">
+        <v>91</v>
+      </c>
+      <c r="F7" s="3">
+        <v>143</v>
+      </c>
+      <c r="G7" s="1">
+        <v>32</v>
+      </c>
+      <c r="H7" s="1">
+        <v>35</v>
+      </c>
+      <c r="I7" s="28">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B8" s="26">
+        <v>1125</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D8" s="7">
+        <v>12</v>
+      </c>
+      <c r="E8" s="5">
+        <v>91</v>
+      </c>
+      <c r="F8" s="3">
+        <v>144</v>
+      </c>
+      <c r="G8" s="1">
+        <v>35</v>
+      </c>
+      <c r="H8" s="1">
+        <v>34</v>
+      </c>
+      <c r="I8" s="28">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B9" s="26">
+        <v>1333</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="D9" s="7">
+        <v>12</v>
+      </c>
+      <c r="E9" s="5">
+        <v>86</v>
+      </c>
+      <c r="F9" s="3">
+        <v>157</v>
+      </c>
+      <c r="G9" s="1">
+        <v>38</v>
+      </c>
+      <c r="H9" s="1">
+        <v>36</v>
+      </c>
+      <c r="I9" s="28">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B10" s="26">
+        <v>1253</v>
+      </c>
+      <c r="C10" s="4">
+        <v>2.6</v>
+      </c>
+      <c r="D10" s="7">
+        <v>12</v>
+      </c>
+      <c r="E10" s="5">
+        <v>84</v>
+      </c>
+      <c r="F10" s="3">
+        <v>164</v>
+      </c>
+      <c r="G10" s="1">
+        <v>35</v>
+      </c>
+      <c r="H10" s="1">
+        <v>36</v>
+      </c>
+      <c r="I10" s="28">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B11" s="26">
+        <v>1138</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="D11" s="7">
+        <v>12</v>
+      </c>
+      <c r="E11" s="5">
+        <v>88</v>
+      </c>
+      <c r="F11" s="3">
+        <v>155</v>
+      </c>
+      <c r="G11" s="1">
+        <v>34</v>
+      </c>
+      <c r="H11" s="1">
+        <v>34</v>
+      </c>
+      <c r="I11" s="28">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B12" s="26">
+        <v>1227</v>
+      </c>
+      <c r="C12" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="D12" s="7">
+        <v>12</v>
+      </c>
+      <c r="E12" s="5">
+        <v>88</v>
+      </c>
+      <c r="F12" s="3">
+        <v>154</v>
+      </c>
+      <c r="G12" s="1">
+        <v>38</v>
+      </c>
+      <c r="H12" s="1">
+        <v>33</v>
+      </c>
+      <c r="I12" s="28">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B13" s="26">
+        <v>1313</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="D13" s="7">
+        <v>12</v>
+      </c>
+      <c r="E13" s="5">
+        <v>88</v>
+      </c>
+      <c r="F13" s="3">
+        <v>151</v>
+      </c>
+      <c r="G13" s="1">
+        <v>37</v>
+      </c>
+      <c r="H13" s="1">
+        <v>37</v>
+      </c>
+      <c r="I13" s="28">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B15" s="25">
+        <v>1332</v>
+      </c>
+      <c r="C15" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D15" s="7">
+        <v>12</v>
+      </c>
+      <c r="E15" s="5">
+        <v>91</v>
+      </c>
+      <c r="F15" s="3">
+        <v>142</v>
+      </c>
+      <c r="G15" s="1">
+        <v>42</v>
+      </c>
+      <c r="H15" s="1">
+        <v>34</v>
+      </c>
+      <c r="I15" s="28">
+        <v>34</v>
+      </c>
+      <c r="J15" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B16" s="26">
+        <v>1288</v>
+      </c>
+      <c r="C16" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="D16" s="7">
+        <v>12</v>
+      </c>
+      <c r="E16" s="5">
+        <v>90</v>
+      </c>
+      <c r="F16" s="3">
+        <v>145</v>
+      </c>
+      <c r="G16" s="1">
+        <v>38</v>
+      </c>
+      <c r="H16" s="1">
+        <v>36</v>
+      </c>
+      <c r="I16" s="28">
+        <v>35</v>
+      </c>
+      <c r="J16" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B17" s="26">
+        <v>1207</v>
+      </c>
+      <c r="C17" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D17" s="7">
+        <v>12</v>
+      </c>
+      <c r="E17" s="5">
+        <v>93</v>
+      </c>
+      <c r="F17" s="3">
+        <v>129</v>
+      </c>
+      <c r="G17" s="1">
+        <v>41</v>
+      </c>
+      <c r="H17" s="1">
+        <v>34</v>
+      </c>
+      <c r="I17" s="28">
+        <v>35</v>
+      </c>
+      <c r="J17" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B18" s="26">
+        <v>1648</v>
+      </c>
+      <c r="C18" s="4">
+        <v>2.6</v>
+      </c>
+      <c r="D18" s="7">
+        <v>12</v>
+      </c>
+      <c r="E18" s="5">
+        <v>82</v>
+      </c>
+      <c r="F18" s="3">
+        <v>173</v>
+      </c>
+      <c r="G18" s="1">
+        <v>46</v>
+      </c>
+      <c r="H18" s="1">
+        <v>35</v>
+      </c>
+      <c r="I18" s="28">
+        <v>36</v>
+      </c>
+      <c r="J18" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B19" s="26">
+        <v>1403</v>
+      </c>
+      <c r="C19" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="D19" s="7">
+        <v>12</v>
+      </c>
+      <c r="E19" s="5">
+        <v>86</v>
+      </c>
+      <c r="F19" s="3">
+        <v>157</v>
+      </c>
+      <c r="G19" s="1">
+        <v>40</v>
+      </c>
+      <c r="H19" s="1">
+        <v>36</v>
+      </c>
+      <c r="I19" s="28">
+        <v>36</v>
+      </c>
+      <c r="J19" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B20" s="26">
+        <v>1594</v>
+      </c>
+      <c r="C20" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="D20" s="7">
+        <v>12</v>
+      </c>
+      <c r="E20" s="5">
+        <v>84</v>
+      </c>
+      <c r="F20" s="3">
+        <v>166</v>
+      </c>
+      <c r="G20" s="1">
+        <v>44</v>
+      </c>
+      <c r="H20" s="1">
+        <v>36</v>
+      </c>
+      <c r="I20" s="28">
+        <v>38</v>
+      </c>
+      <c r="J20" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B21" s="26">
+        <v>1558</v>
+      </c>
+      <c r="C21" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="D21" s="7">
+        <v>12</v>
+      </c>
+      <c r="E21" s="5">
+        <v>84</v>
+      </c>
+      <c r="F21" s="3">
+        <v>166</v>
+      </c>
+      <c r="G21" s="1">
+        <v>43</v>
+      </c>
+      <c r="H21" s="1">
+        <v>36</v>
+      </c>
+      <c r="I21" s="28">
+        <v>38</v>
+      </c>
+      <c r="J21" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B22" s="26">
+        <v>1657</v>
+      </c>
+      <c r="C22" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="D22" s="7">
+        <v>12</v>
+      </c>
+      <c r="E22" s="5">
+        <v>82</v>
+      </c>
+      <c r="F22" s="3">
+        <v>172</v>
+      </c>
+      <c r="G22" s="1">
+        <v>44</v>
+      </c>
+      <c r="H22" s="1">
+        <v>37</v>
+      </c>
+      <c r="I22" s="28">
+        <v>38</v>
+      </c>
+      <c r="J22" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B23" s="26">
+        <v>1620</v>
+      </c>
+      <c r="C23" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="D23" s="7">
+        <v>12</v>
+      </c>
+      <c r="E23" s="5">
+        <v>84</v>
+      </c>
+      <c r="F23" s="3">
+        <v>165</v>
+      </c>
+      <c r="G23" s="1">
+        <v>45</v>
+      </c>
+      <c r="H23" s="1">
+        <v>36</v>
+      </c>
+      <c r="I23" s="28">
+        <v>37</v>
+      </c>
+      <c r="J23" t="s">
+        <v>362</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96551E4B-D0DF-400F-B6DB-43F70FA502C4}">
   <dimension ref="A1:I29"/>
   <sheetViews>
@@ -3142,7 +3831,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DAD396-9A3B-4E45-8468-1404C7D6E830}">
   <dimension ref="A1:J9"/>
   <sheetViews>
@@ -3439,7 +4128,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3C8FEF-B598-4AEC-9E3E-97CE35ABD837}">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -3697,7 +4386,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6EE9141-0B58-4213-922A-6EE4F5E15BD3}">
   <dimension ref="A1:I9"/>
   <sheetViews>
@@ -6972,7 +7661,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J65" sqref="J65"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9061,6 +9750,248 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC772471-31F7-4C6C-832D-6D1F31BC4A1E}">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C2" s="6">
+        <v>313</v>
+      </c>
+      <c r="D2" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="E2" s="7">
+        <v>9</v>
+      </c>
+      <c r="F2" s="5">
+        <v>79</v>
+      </c>
+      <c r="G2" s="3">
+        <v>183</v>
+      </c>
+      <c r="H2" s="1">
+        <v>39</v>
+      </c>
+      <c r="I2" s="1">
+        <v>35</v>
+      </c>
+      <c r="J2">
+        <f>SUM(D2:I2) * 0.9</f>
+        <v>313.29000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C3" s="6">
+        <v>308</v>
+      </c>
+      <c r="D3" s="4">
+        <v>3</v>
+      </c>
+      <c r="E3" s="7">
+        <v>9</v>
+      </c>
+      <c r="F3" s="5">
+        <v>80</v>
+      </c>
+      <c r="G3" s="3">
+        <v>181</v>
+      </c>
+      <c r="H3" s="1">
+        <v>37</v>
+      </c>
+      <c r="I3" s="1">
+        <v>33</v>
+      </c>
+      <c r="J3">
+        <f>SUM(D3:I3) * 0.9</f>
+        <v>308.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C4" s="6">
+        <v>309</v>
+      </c>
+      <c r="D4" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="E4" s="7">
+        <v>9</v>
+      </c>
+      <c r="F4" s="5">
+        <v>79</v>
+      </c>
+      <c r="G4" s="3">
+        <v>182</v>
+      </c>
+      <c r="H4" s="1">
+        <v>38</v>
+      </c>
+      <c r="I4" s="1">
+        <v>32</v>
+      </c>
+      <c r="J4">
+        <f>SUM(D4:I4) * 0.9</f>
+        <v>308.79000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C5" s="6">
+        <v>313</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="E5" s="7">
+        <v>9</v>
+      </c>
+      <c r="F5" s="5">
+        <v>79</v>
+      </c>
+      <c r="G5" s="3">
+        <v>183</v>
+      </c>
+      <c r="H5" s="1">
+        <v>39</v>
+      </c>
+      <c r="I5" s="1">
+        <v>35</v>
+      </c>
+      <c r="J5">
+        <f>SUM(D5:I5) *0.9</f>
+        <v>313.29000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C6" s="6">
+        <v>321</v>
+      </c>
+      <c r="D6" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="E6" s="7">
+        <v>9</v>
+      </c>
+      <c r="F6" s="5">
+        <v>76</v>
+      </c>
+      <c r="G6" s="3">
+        <v>193</v>
+      </c>
+      <c r="H6" s="1">
+        <v>40</v>
+      </c>
+      <c r="I6" s="1">
+        <v>36</v>
+      </c>
+      <c r="J6">
+        <f>SUM(D6:I6) *0.9</f>
+        <v>321.75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C7" s="6">
+        <v>315</v>
+      </c>
+      <c r="D7" s="4">
+        <v>3.3</v>
+      </c>
+      <c r="E7" s="7">
+        <v>9</v>
+      </c>
+      <c r="F7" s="5">
+        <v>78</v>
+      </c>
+      <c r="G7" s="3">
+        <v>186</v>
+      </c>
+      <c r="H7" s="1">
+        <v>37</v>
+      </c>
+      <c r="I7" s="1">
+        <v>37</v>
+      </c>
+      <c r="J7">
+        <f>SUM(D7:I7) *0.9</f>
+        <v>315.27000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE67CB9-8D30-45BB-9729-53435DBF7C02}">
   <dimension ref="A1:I13"/>
   <sheetViews>
@@ -9389,12 +10320,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{042C4405-AEC3-4A36-A3E7-7EA75E4B87DD}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9458,7 +10389,7 @@
         <v>32</v>
       </c>
       <c r="J2">
-        <f>SUM(D2:I2)*0.8</f>
+        <f t="shared" ref="J2:J7" si="0">SUM(D2:I2)*0.8</f>
         <v>265.52</v>
       </c>
     </row>
@@ -9489,7 +10420,7 @@
         <v>31</v>
       </c>
       <c r="J3">
-        <f>SUM(D3:I3)*0.8</f>
+        <f t="shared" si="0"/>
         <v>312.40000000000003</v>
       </c>
     </row>
@@ -9520,7 +10451,7 @@
         <v>22</v>
       </c>
       <c r="J4">
-        <f>SUM(D4:I4)*0.8</f>
+        <f t="shared" si="0"/>
         <v>255.20000000000002</v>
       </c>
     </row>
@@ -9551,7 +10482,7 @@
         <v>35</v>
       </c>
       <c r="J5">
-        <f>SUM(D5:I5)*0.8</f>
+        <f t="shared" si="0"/>
         <v>275.36</v>
       </c>
     </row>
@@ -9582,7 +10513,7 @@
         <v>34</v>
       </c>
       <c r="J6">
-        <f>SUM(D6:I6)*0.8</f>
+        <f t="shared" si="0"/>
         <v>300.32</v>
       </c>
     </row>
@@ -9613,7 +10544,7 @@
         <v>35</v>
       </c>
       <c r="J7">
-        <f>SUM(D7:I7)*0.8</f>
+        <f t="shared" si="0"/>
         <v>269.84000000000003</v>
       </c>
     </row>
@@ -9665,7 +10596,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{270FCD42-7C0A-42FB-9872-27F0BB063FAE}">
   <dimension ref="A1:I32"/>
   <sheetViews>
@@ -10435,689 +11366,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C18765D9-5E60-43F7-8EAE-7692D37C4247}">
-  <dimension ref="A1:J23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="B2" s="27">
-        <v>1047</v>
-      </c>
-      <c r="C2" s="4">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D2" s="7">
-        <v>12</v>
-      </c>
-      <c r="E2" s="5">
-        <v>90</v>
-      </c>
-      <c r="F2" s="3">
-        <v>148</v>
-      </c>
-      <c r="G2" s="1">
-        <v>33</v>
-      </c>
-      <c r="H2" s="1">
-        <v>33</v>
-      </c>
-      <c r="I2" s="28">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="B3" s="26">
-        <v>1142</v>
-      </c>
-      <c r="C3" s="4">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D3" s="7">
-        <v>12</v>
-      </c>
-      <c r="E3" s="5">
-        <v>90</v>
-      </c>
-      <c r="F3" s="3">
-        <v>148</v>
-      </c>
-      <c r="G3" s="1">
-        <v>36</v>
-      </c>
-      <c r="H3" s="1">
-        <v>33</v>
-      </c>
-      <c r="I3" s="28">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="B4" s="26">
-        <v>1070</v>
-      </c>
-      <c r="C4" s="4">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D4" s="7">
-        <v>12</v>
-      </c>
-      <c r="E4" s="5">
-        <v>91</v>
-      </c>
-      <c r="F4" s="3">
-        <v>141</v>
-      </c>
-      <c r="G4" s="1">
-        <v>34</v>
-      </c>
-      <c r="H4" s="1">
-        <v>34</v>
-      </c>
-      <c r="I4" s="28">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="B5" s="26">
-        <v>990</v>
-      </c>
-      <c r="C5" s="4">
-        <v>2</v>
-      </c>
-      <c r="D5" s="7">
-        <v>12</v>
-      </c>
-      <c r="E5" s="5">
-        <v>93</v>
-      </c>
-      <c r="F5" s="3">
-        <v>124</v>
-      </c>
-      <c r="G5" s="1">
-        <v>35</v>
-      </c>
-      <c r="H5" s="1">
-        <v>34</v>
-      </c>
-      <c r="I5" s="28">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="B6" s="26">
-        <v>1343</v>
-      </c>
-      <c r="C6" s="4">
-        <v>2.4</v>
-      </c>
-      <c r="D6" s="7">
-        <v>12</v>
-      </c>
-      <c r="E6" s="5">
-        <v>88</v>
-      </c>
-      <c r="F6" s="3">
-        <v>159</v>
-      </c>
-      <c r="G6" s="1">
-        <v>38</v>
-      </c>
-      <c r="H6" s="1">
-        <v>35</v>
-      </c>
-      <c r="I6" s="28">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="B7" s="26">
-        <v>1052</v>
-      </c>
-      <c r="C7" s="4">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D7" s="7">
-        <v>12</v>
-      </c>
-      <c r="E7" s="5">
-        <v>91</v>
-      </c>
-      <c r="F7" s="3">
-        <v>143</v>
-      </c>
-      <c r="G7" s="1">
-        <v>32</v>
-      </c>
-      <c r="H7" s="1">
-        <v>35</v>
-      </c>
-      <c r="I7" s="28">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="B8" s="26">
-        <v>1125</v>
-      </c>
-      <c r="C8" s="4">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D8" s="7">
-        <v>12</v>
-      </c>
-      <c r="E8" s="5">
-        <v>91</v>
-      </c>
-      <c r="F8" s="3">
-        <v>144</v>
-      </c>
-      <c r="G8" s="1">
-        <v>35</v>
-      </c>
-      <c r="H8" s="1">
-        <v>34</v>
-      </c>
-      <c r="I8" s="28">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="B9" s="26">
-        <v>1333</v>
-      </c>
-      <c r="C9" s="4">
-        <v>2.5</v>
-      </c>
-      <c r="D9" s="7">
-        <v>12</v>
-      </c>
-      <c r="E9" s="5">
-        <v>86</v>
-      </c>
-      <c r="F9" s="3">
-        <v>157</v>
-      </c>
-      <c r="G9" s="1">
-        <v>38</v>
-      </c>
-      <c r="H9" s="1">
-        <v>36</v>
-      </c>
-      <c r="I9" s="28">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="B10" s="26">
-        <v>1253</v>
-      </c>
-      <c r="C10" s="4">
-        <v>2.6</v>
-      </c>
-      <c r="D10" s="7">
-        <v>12</v>
-      </c>
-      <c r="E10" s="5">
-        <v>84</v>
-      </c>
-      <c r="F10" s="3">
-        <v>164</v>
-      </c>
-      <c r="G10" s="1">
-        <v>35</v>
-      </c>
-      <c r="H10" s="1">
-        <v>36</v>
-      </c>
-      <c r="I10" s="28">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="B11" s="26">
-        <v>1138</v>
-      </c>
-      <c r="C11" s="4">
-        <v>2.4</v>
-      </c>
-      <c r="D11" s="7">
-        <v>12</v>
-      </c>
-      <c r="E11" s="5">
-        <v>88</v>
-      </c>
-      <c r="F11" s="3">
-        <v>155</v>
-      </c>
-      <c r="G11" s="1">
-        <v>34</v>
-      </c>
-      <c r="H11" s="1">
-        <v>34</v>
-      </c>
-      <c r="I11" s="28">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="B12" s="26">
-        <v>1227</v>
-      </c>
-      <c r="C12" s="4">
-        <v>2.4</v>
-      </c>
-      <c r="D12" s="7">
-        <v>12</v>
-      </c>
-      <c r="E12" s="5">
-        <v>88</v>
-      </c>
-      <c r="F12" s="3">
-        <v>154</v>
-      </c>
-      <c r="G12" s="1">
-        <v>38</v>
-      </c>
-      <c r="H12" s="1">
-        <v>33</v>
-      </c>
-      <c r="I12" s="28">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="B13" s="26">
-        <v>1313</v>
-      </c>
-      <c r="C13" s="4">
-        <v>2.4</v>
-      </c>
-      <c r="D13" s="7">
-        <v>12</v>
-      </c>
-      <c r="E13" s="5">
-        <v>88</v>
-      </c>
-      <c r="F13" s="3">
-        <v>151</v>
-      </c>
-      <c r="G13" s="1">
-        <v>37</v>
-      </c>
-      <c r="H13" s="1">
-        <v>37</v>
-      </c>
-      <c r="I13" s="28">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="B15" s="25">
-        <v>1332</v>
-      </c>
-      <c r="C15" s="4">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D15" s="7">
-        <v>12</v>
-      </c>
-      <c r="E15" s="5">
-        <v>91</v>
-      </c>
-      <c r="F15" s="3">
-        <v>142</v>
-      </c>
-      <c r="G15" s="1">
-        <v>42</v>
-      </c>
-      <c r="H15" s="1">
-        <v>34</v>
-      </c>
-      <c r="I15" s="28">
-        <v>34</v>
-      </c>
-      <c r="J15" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="B16" s="26">
-        <v>1288</v>
-      </c>
-      <c r="C16" s="4">
-        <v>2.4</v>
-      </c>
-      <c r="D16" s="7">
-        <v>12</v>
-      </c>
-      <c r="E16" s="5">
-        <v>90</v>
-      </c>
-      <c r="F16" s="3">
-        <v>145</v>
-      </c>
-      <c r="G16" s="1">
-        <v>38</v>
-      </c>
-      <c r="H16" s="1">
-        <v>36</v>
-      </c>
-      <c r="I16" s="28">
-        <v>35</v>
-      </c>
-      <c r="J16" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="B17" s="26">
-        <v>1207</v>
-      </c>
-      <c r="C17" s="4">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D17" s="7">
-        <v>12</v>
-      </c>
-      <c r="E17" s="5">
-        <v>93</v>
-      </c>
-      <c r="F17" s="3">
-        <v>129</v>
-      </c>
-      <c r="G17" s="1">
-        <v>41</v>
-      </c>
-      <c r="H17" s="1">
-        <v>34</v>
-      </c>
-      <c r="I17" s="28">
-        <v>35</v>
-      </c>
-      <c r="J17" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="B18" s="26">
-        <v>1648</v>
-      </c>
-      <c r="C18" s="4">
-        <v>2.6</v>
-      </c>
-      <c r="D18" s="7">
-        <v>12</v>
-      </c>
-      <c r="E18" s="5">
-        <v>82</v>
-      </c>
-      <c r="F18" s="3">
-        <v>173</v>
-      </c>
-      <c r="G18" s="1">
-        <v>46</v>
-      </c>
-      <c r="H18" s="1">
-        <v>35</v>
-      </c>
-      <c r="I18" s="28">
-        <v>36</v>
-      </c>
-      <c r="J18" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="B19" s="26">
-        <v>1403</v>
-      </c>
-      <c r="C19" s="4">
-        <v>2.5</v>
-      </c>
-      <c r="D19" s="7">
-        <v>12</v>
-      </c>
-      <c r="E19" s="5">
-        <v>86</v>
-      </c>
-      <c r="F19" s="3">
-        <v>157</v>
-      </c>
-      <c r="G19" s="1">
-        <v>40</v>
-      </c>
-      <c r="H19" s="1">
-        <v>36</v>
-      </c>
-      <c r="I19" s="28">
-        <v>36</v>
-      </c>
-      <c r="J19" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="B20" s="26">
-        <v>1594</v>
-      </c>
-      <c r="C20" s="4">
-        <v>2.7</v>
-      </c>
-      <c r="D20" s="7">
-        <v>12</v>
-      </c>
-      <c r="E20" s="5">
-        <v>84</v>
-      </c>
-      <c r="F20" s="3">
-        <v>166</v>
-      </c>
-      <c r="G20" s="1">
-        <v>44</v>
-      </c>
-      <c r="H20" s="1">
-        <v>36</v>
-      </c>
-      <c r="I20" s="28">
-        <v>38</v>
-      </c>
-      <c r="J20" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="B21" s="26">
-        <v>1558</v>
-      </c>
-      <c r="C21" s="4">
-        <v>2.7</v>
-      </c>
-      <c r="D21" s="7">
-        <v>12</v>
-      </c>
-      <c r="E21" s="5">
-        <v>84</v>
-      </c>
-      <c r="F21" s="3">
-        <v>166</v>
-      </c>
-      <c r="G21" s="1">
-        <v>43</v>
-      </c>
-      <c r="H21" s="1">
-        <v>36</v>
-      </c>
-      <c r="I21" s="28">
-        <v>38</v>
-      </c>
-      <c r="J21" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="B22" s="26">
-        <v>1657</v>
-      </c>
-      <c r="C22" s="4">
-        <v>2.8</v>
-      </c>
-      <c r="D22" s="7">
-        <v>12</v>
-      </c>
-      <c r="E22" s="5">
-        <v>82</v>
-      </c>
-      <c r="F22" s="3">
-        <v>172</v>
-      </c>
-      <c r="G22" s="1">
-        <v>44</v>
-      </c>
-      <c r="H22" s="1">
-        <v>37</v>
-      </c>
-      <c r="I22" s="28">
-        <v>38</v>
-      </c>
-      <c r="J22" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="B23" s="26">
-        <v>1620</v>
-      </c>
-      <c r="C23" s="4">
-        <v>2.7</v>
-      </c>
-      <c r="D23" s="7">
-        <v>12</v>
-      </c>
-      <c r="E23" s="5">
-        <v>84</v>
-      </c>
-      <c r="F23" s="3">
-        <v>165</v>
-      </c>
-      <c r="G23" s="1">
-        <v>45</v>
-      </c>
-      <c r="H23" s="1">
-        <v>36</v>
-      </c>
-      <c r="I23" s="28">
-        <v>37</v>
-      </c>
-      <c r="J23" t="s">
-        <v>362</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
- Added iJustWant2bPure's latest scenes - Updated helmet stats - Updated some starting option stats
</commit_message>
<xml_diff>
--- a/Items+Troops Spreadsheets/HYW Item Balance.xlsx
+++ b/Items+Troops Spreadsheets/HYW Item Balance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoann\OneDrive\Ambiente de Trabalho\Deeds_Modsys\Items+Troops Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E800A93D-8B3C-4F24-971A-3771105D7E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4172D8-B951-4981-94D3-8902C9758949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12696" yWindow="5352" windowWidth="17280" windowHeight="8964" firstSheet="4" activeTab="5" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" firstSheet="9" activeTab="15" xr2:uid="{B36B220B-AFFD-40C9-B18F-2948A113413C}"/>
   </bookViews>
   <sheets>
     <sheet name="Maces" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,16 @@
     <sheet name="Bastard &amp; Twohanded Swords" sheetId="4" r:id="rId4"/>
     <sheet name="Pikes &amp; Halberds" sheetId="5" r:id="rId5"/>
     <sheet name="Halberds" sheetId="14" r:id="rId6"/>
-    <sheet name="Forks &amp; Fauchards" sheetId="8" r:id="rId7"/>
-    <sheet name="Glaives &amp; Couteau" sheetId="13" r:id="rId8"/>
-    <sheet name="Spears &amp; Lances" sheetId="9" r:id="rId9"/>
-    <sheet name="Pollaxes" sheetId="12" r:id="rId10"/>
-    <sheet name="Bows &amp; Crossbows" sheetId="6" r:id="rId11"/>
-    <sheet name="Horses" sheetId="7" r:id="rId12"/>
-    <sheet name="Arrows &amp; Bolts" sheetId="10" r:id="rId13"/>
-    <sheet name="Shields" sheetId="11" r:id="rId14"/>
+    <sheet name="Feuil1" sheetId="15" r:id="rId7"/>
+    <sheet name="Forks &amp; Fauchards" sheetId="8" r:id="rId8"/>
+    <sheet name="Glaives &amp; Couteau" sheetId="13" r:id="rId9"/>
+    <sheet name="Spears &amp; Lances" sheetId="9" r:id="rId10"/>
+    <sheet name="Pollaxes" sheetId="12" r:id="rId11"/>
+    <sheet name="Bows &amp; Crossbows" sheetId="6" r:id="rId12"/>
+    <sheet name="Horses" sheetId="7" r:id="rId13"/>
+    <sheet name="Arrows &amp; Bolts" sheetId="10" r:id="rId14"/>
+    <sheet name="Shields" sheetId="11" r:id="rId15"/>
+    <sheet name="Helmets" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="445">
   <si>
     <t>ID</t>
   </si>
@@ -1207,6 +1209,180 @@
   </si>
   <si>
     <t>Halberd</t>
+  </si>
+  <si>
+    <t>Head Armour</t>
+  </si>
+  <si>
+    <t>Body Armour</t>
+  </si>
+  <si>
+    <t>Hood</t>
+  </si>
+  <si>
+    <t>Liripipe Hood</t>
+  </si>
+  <si>
+    <t>Mail Collar</t>
+  </si>
+  <si>
+    <t>Mail Aventail</t>
+  </si>
+  <si>
+    <t>Mail Collar and Bevor</t>
+  </si>
+  <si>
+    <t>h_wicker_helmet</t>
+  </si>
+  <si>
+    <t>h_rope_helmet</t>
+  </si>
+  <si>
+    <t>h_shingle_helmet</t>
+  </si>
+  <si>
+    <t>h_skullcap</t>
+  </si>
+  <si>
+    <t>h_skullcap_hood</t>
+  </si>
+  <si>
+    <t>h_skullcap_mail_aventail</t>
+  </si>
+  <si>
+    <t>h_skullcap_liripipe_hood</t>
+  </si>
+  <si>
+    <t>h_cervelliere</t>
+  </si>
+  <si>
+    <t>h_cervelliere_hood</t>
+  </si>
+  <si>
+    <t>h_cervelliere_liripipe_hood</t>
+  </si>
+  <si>
+    <t>h_cervelliere_mail_aventail</t>
+  </si>
+  <si>
+    <t>h_cervelliere_roundel</t>
+  </si>
+  <si>
+    <t>h_cervelliere_roundel_hood</t>
+  </si>
+  <si>
+    <t>h_cervelliere_roundel_liripipe_hood</t>
+  </si>
+  <si>
+    <t>h_cervelliere_roundel_mail_aventail</t>
+  </si>
+  <si>
+    <t>h_makeshift_kettle</t>
+  </si>
+  <si>
+    <t>h_makeshift_kettle_hood</t>
+  </si>
+  <si>
+    <t>h_makeshift_kettle_liripipe</t>
+  </si>
+  <si>
+    <t>h_makeshift_kettle_mail_aventail</t>
+  </si>
+  <si>
+    <t>h_german_kettlehats</t>
+  </si>
+  <si>
+    <t>h_german_kettlehats_hood</t>
+  </si>
+  <si>
+    <t>h_german_kettlehats_liripipe_hood</t>
+  </si>
+  <si>
+    <t>h_german_kettlehats_mail_aventail</t>
+  </si>
+  <si>
+    <t>h_sallets</t>
+  </si>
+  <si>
+    <t>h_sallets_mail_aventail</t>
+  </si>
+  <si>
+    <t>h_sallets_mail_collar</t>
+  </si>
+  <si>
+    <t>h_sallets_mail_collar_bevor</t>
+  </si>
+  <si>
+    <t>h_sallets_transitional_visor</t>
+  </si>
+  <si>
+    <t>h_sallets_transitional_visor_mail_collar</t>
+  </si>
+  <si>
+    <t>h_sallets_transitional_visor_mail_aventail</t>
+  </si>
+  <si>
+    <t>h_sallets_transitional_visor_mail_collar_bevor</t>
+  </si>
+  <si>
+    <t>h_sallets_bascinet_visor</t>
+  </si>
+  <si>
+    <t>h_sallets_bascinet_visor_mail_collar</t>
+  </si>
+  <si>
+    <t>h_sallets_bascinet_visor_mail_aventail</t>
+  </si>
+  <si>
+    <t>h_sallets_bascinet_visor_mail_collar_bevor</t>
+  </si>
+  <si>
+    <t>h_bascinets</t>
+  </si>
+  <si>
+    <t>h_bascinets_visor</t>
+  </si>
+  <si>
+    <t>h_bascinets_visor_gilded</t>
+  </si>
+  <si>
+    <t>h_eyeslot_kettlehats</t>
+  </si>
+  <si>
+    <t>h_eyeslot_kettlehats_hood</t>
+  </si>
+  <si>
+    <t>h_eyeslot_kettlehats_liripipe_hood</t>
+  </si>
+  <si>
+    <t>h_eyeslot_kettlehats_mail_aventail</t>
+  </si>
+  <si>
+    <t>h_barbutas</t>
+  </si>
+  <si>
+    <t>h_barbutas_mail_collar</t>
+  </si>
+  <si>
+    <t>h_barbutas_mail_collar_bevor</t>
+  </si>
+  <si>
+    <t>h_barbuta_nooxy_3</t>
+  </si>
+  <si>
+    <t>h_zitta/wespe/pigface</t>
+  </si>
+  <si>
+    <t>h_great_bascinets</t>
+  </si>
+  <si>
+    <t>h_great_bascinets_visor</t>
+  </si>
+  <si>
+    <t>h_great_sallet</t>
+  </si>
+  <si>
+    <t>h_great_sallet_visor</t>
   </si>
 </sst>
 </file>
@@ -1228,7 +1404,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1325,6 +1501,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFED7F7F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -1396,7 +1590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1442,17 +1636,124 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="25">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFED7F7F"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFED7F7F"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1556,9 +1857,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFED7F7F"/>
       <color rgb="FFA2F4DF"/>
       <color rgb="FFA669FF"/>
-      <color rgb="FFED7F7F"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1573,18 +1874,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9F5046EE-3462-4861-8BA7-BDFE936F9817}" name="Tableau1" displayName="Tableau1" ref="A1:I9" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9F5046EE-3462-4861-8BA7-BDFE936F9817}" name="Tableau1" displayName="Tableau1" ref="A1:I9" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22">
   <autoFilter ref="A1:I9" xr:uid="{C03180B4-6AED-435F-B389-4A4563BC2CC7}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{C9803FB6-EDE5-4D36-AE31-771E624ABD45}" name="Native" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{5FC1EA44-BFAD-4BBC-B86E-2A3CF8B5EE66}" name="Price" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{01474069-2C07-4B0D-BCD4-BCBEA8815443}" name="Weight" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{90286B08-5EC7-4290-B829-6A962FFA020D}" name="Hitpoints" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{BEB87F5A-2E44-49CC-B818-CB41CAE1540E}" name="Armor" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{1FC9649F-49E2-4557-9365-90302BBA23F5}" name="Speed" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{9DBEE228-7BC6-4A16-9AEA-276D82F520AF}" name="Width " dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{F49F7FEF-63B8-416A-B721-00BC45756836}" name="Height" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{2B135CC7-F1ED-468C-AA68-F96B873B45CB}" name="Colonne1" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{C9803FB6-EDE5-4D36-AE31-771E624ABD45}" name="Native" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{5FC1EA44-BFAD-4BBC-B86E-2A3CF8B5EE66}" name="Price" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{01474069-2C07-4B0D-BCD4-BCBEA8815443}" name="Weight" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{90286B08-5EC7-4290-B829-6A962FFA020D}" name="Hitpoints" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{BEB87F5A-2E44-49CC-B818-CB41CAE1540E}" name="Armor" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{1FC9649F-49E2-4557-9365-90302BBA23F5}" name="Speed" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{9DBEE228-7BC6-4A16-9AEA-276D82F520AF}" name="Width " dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{F49F7FEF-63B8-416A-B721-00BC45756836}" name="Height" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{2B135CC7-F1ED-468C-AA68-F96B873B45CB}" name="Colonne1" dataDxfId="13">
       <calculatedColumnFormula>((Tableau1[[#This Row],[Hitpoints]]*Tableau1[[#This Row],[Armor]]*2)+(Tableau1[[#This Row],[Width ]]*Tableau1[[#This Row],[Height]]*2)-(Tableau1[[#This Row],[Speed]]*Tableau1[[#This Row],[Weight]]))/100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1592,10 +1893,24 @@
 </table>
 </file>
 
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D59FB3B4-EC06-4D73-9946-6BFE2C2CCBE1}" name="Tableau2" displayName="Tableau2" ref="A7:E71" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
+  <autoFilter ref="A7:E71" xr:uid="{D59FB3B4-EC06-4D73-9946-6BFE2C2CCBE1}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{21613AAF-B76C-4060-ACB4-4C1DBB9C3B0B}" name="ID" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{21CBE435-491F-46CE-AC9C-F4DC60BC75DA}" name="Price" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{0C92D438-FF0E-4E4D-A49D-F1E5D03F952C}" name="Weight" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{974C9707-BBDC-49A3-A159-86CDDB7C55BC}" name="Head Armour" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{53D86C19-4C70-4593-BC24-2F9BB8ACF6DE}" name="Body Armour" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1633,7 +1948,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1739,7 +2054,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1881,7 +2196,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2477,6 +2792,778 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{270FCD42-7C0A-42FB-9872-27F0BB063FAE}">
+  <dimension ref="A1:I32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="6">
+        <v>134</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
+        <v>99</v>
+      </c>
+      <c r="G2" s="3">
+        <v>107</v>
+      </c>
+      <c r="H2" s="1">
+        <v>37</v>
+      </c>
+      <c r="I2">
+        <f>SUM(D2:H2)*0.55</f>
+        <v>134.255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="6">
+        <v>144</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5">
+        <v>97</v>
+      </c>
+      <c r="G3" s="3">
+        <v>128</v>
+      </c>
+      <c r="H3" s="1">
+        <v>36</v>
+      </c>
+      <c r="I3">
+        <f>SUM(D3:H3)*0.55</f>
+        <v>144.26500000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="6">
+        <v>146</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>97</v>
+      </c>
+      <c r="G4" s="3">
+        <v>132</v>
+      </c>
+      <c r="H4" s="1">
+        <v>36</v>
+      </c>
+      <c r="I4">
+        <f>SUM(D4:H4)*0.55</f>
+        <v>146.46500000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="6">
+        <v>165</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>96</v>
+      </c>
+      <c r="G5" s="3">
+        <v>142</v>
+      </c>
+      <c r="H5" s="1">
+        <v>35</v>
+      </c>
+      <c r="I5">
+        <f>SUM(D5:H5)*0.6</f>
+        <v>164.64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="6">
+        <v>166</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>96</v>
+      </c>
+      <c r="G6" s="3">
+        <v>144</v>
+      </c>
+      <c r="H6" s="1">
+        <v>35</v>
+      </c>
+      <c r="I6">
+        <f>SUM(D6:H6)*0.6</f>
+        <v>165.83999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="6">
+        <v>168</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
+        <v>95</v>
+      </c>
+      <c r="G7" s="3">
+        <v>149</v>
+      </c>
+      <c r="H7" s="1">
+        <v>34</v>
+      </c>
+      <c r="I7">
+        <f>SUM(D7:H7)*0.6</f>
+        <v>167.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="6">
+        <v>229</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <v>90</v>
+      </c>
+      <c r="G8" s="3">
+        <v>204</v>
+      </c>
+      <c r="H8" s="1">
+        <v>31</v>
+      </c>
+      <c r="I8">
+        <f>SUM(D8:H8)*0.7</f>
+        <v>228.89999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="6">
+        <v>117</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <v>100</v>
+      </c>
+      <c r="G9" s="3">
+        <v>95</v>
+      </c>
+      <c r="H9" s="1">
+        <v>38</v>
+      </c>
+      <c r="I9">
+        <f>SUM(D9:H9)*0.5</f>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="6">
+        <v>87</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
+        <v>87</v>
+      </c>
+      <c r="G11" s="3">
+        <v>135</v>
+      </c>
+      <c r="H11" s="1">
+        <v>26</v>
+      </c>
+      <c r="I11">
+        <f>SUM(D11:H11)*0.35</f>
+        <v>87.324999999999989</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="6">
+        <v>84</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1.4</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>88</v>
+      </c>
+      <c r="G12" s="3">
+        <v>126</v>
+      </c>
+      <c r="H12" s="1">
+        <v>25</v>
+      </c>
+      <c r="I12">
+        <f>SUM(D12:H12)*0.35</f>
+        <v>84.14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="6">
+        <v>142</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
+        <v>84</v>
+      </c>
+      <c r="G13" s="3">
+        <v>168</v>
+      </c>
+      <c r="H13" s="1">
+        <v>31</v>
+      </c>
+      <c r="I13">
+        <f>SUM(D13:H13)*0.5</f>
+        <v>142.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="6">
+        <v>285</v>
+      </c>
+      <c r="D15" s="4">
+        <v>3</v>
+      </c>
+      <c r="E15" s="7">
+        <v>9</v>
+      </c>
+      <c r="F15" s="5">
+        <v>84</v>
+      </c>
+      <c r="G15" s="3">
+        <v>355</v>
+      </c>
+      <c r="H15" s="1">
+        <v>25</v>
+      </c>
+      <c r="I15">
+        <f>SUM(D15:H15)*0.6</f>
+        <v>285.59999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="6">
+        <v>214</v>
+      </c>
+      <c r="D16" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="E16" s="7">
+        <v>9</v>
+      </c>
+      <c r="F16" s="5">
+        <v>92</v>
+      </c>
+      <c r="G16" s="3">
+        <v>175</v>
+      </c>
+      <c r="H16" s="1">
+        <v>27</v>
+      </c>
+      <c r="I16">
+        <f>SUM(D16:H16)*0.7</f>
+        <v>213.85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="6">
+        <v>224</v>
+      </c>
+      <c r="D17" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="E17" s="7">
+        <v>9</v>
+      </c>
+      <c r="F17" s="5">
+        <v>90</v>
+      </c>
+      <c r="G17" s="3">
+        <v>190</v>
+      </c>
+      <c r="H17" s="1">
+        <v>29</v>
+      </c>
+      <c r="I17">
+        <f>SUM(D17:H17)*0.7</f>
+        <v>224.27999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="6">
+        <v>320</v>
+      </c>
+      <c r="D19" s="4">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E19" s="7">
+        <v>12</v>
+      </c>
+      <c r="F19" s="5">
+        <v>82</v>
+      </c>
+      <c r="G19" s="3">
+        <v>267</v>
+      </c>
+      <c r="H19" s="1">
+        <v>35</v>
+      </c>
+      <c r="I19">
+        <f t="shared" ref="I19:I24" si="0">SUM(D19:H19)*0.8</f>
+        <v>320.32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="6">
+        <v>286</v>
+      </c>
+      <c r="D20" s="4">
+        <v>4</v>
+      </c>
+      <c r="E20" s="7">
+        <v>12</v>
+      </c>
+      <c r="F20" s="5">
+        <v>85</v>
+      </c>
+      <c r="G20" s="3">
+        <v>226</v>
+      </c>
+      <c r="H20" s="1">
+        <v>31</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>286.40000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="6">
+        <v>307</v>
+      </c>
+      <c r="D21" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="E21" s="7">
+        <v>12</v>
+      </c>
+      <c r="F21" s="5">
+        <v>83</v>
+      </c>
+      <c r="G21" s="3">
+        <v>253</v>
+      </c>
+      <c r="H21" s="1">
+        <v>32</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>307.36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="6">
+        <v>307</v>
+      </c>
+      <c r="D22" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="E22" s="7">
+        <v>12</v>
+      </c>
+      <c r="F22" s="5">
+        <v>83</v>
+      </c>
+      <c r="G22" s="3">
+        <v>253</v>
+      </c>
+      <c r="H22" s="1">
+        <v>32</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>307.36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="6">
+        <v>308</v>
+      </c>
+      <c r="D23" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="E23" s="7">
+        <v>12</v>
+      </c>
+      <c r="F23" s="5">
+        <v>83</v>
+      </c>
+      <c r="G23" s="3">
+        <v>252</v>
+      </c>
+      <c r="H23" s="1">
+        <v>34</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>308.16000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="6">
+        <v>296</v>
+      </c>
+      <c r="D24" s="4">
+        <v>4.3</v>
+      </c>
+      <c r="E24" s="7">
+        <v>12</v>
+      </c>
+      <c r="F24" s="5">
+        <v>83</v>
+      </c>
+      <c r="G24" s="3">
+        <v>241</v>
+      </c>
+      <c r="H24" s="1">
+        <v>30</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>296.24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="6">
+        <v>308</v>
+      </c>
+      <c r="D26" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="E26" s="7">
+        <v>12</v>
+      </c>
+      <c r="F26" s="5">
+        <v>83</v>
+      </c>
+      <c r="G26" s="3">
+        <v>252</v>
+      </c>
+      <c r="H26" s="1">
+        <v>34</v>
+      </c>
+      <c r="I26">
+        <f>SUM(D26:H26)*0.8</f>
+        <v>308.16000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="6">
+        <v>308</v>
+      </c>
+      <c r="D27" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="E27" s="7">
+        <v>12</v>
+      </c>
+      <c r="F27" s="5">
+        <v>83</v>
+      </c>
+      <c r="G27" s="3">
+        <v>252</v>
+      </c>
+      <c r="H27" s="1">
+        <v>34</v>
+      </c>
+      <c r="I27">
+        <f>SUM(D27:H27)*0.8</f>
+        <v>308.16000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="6">
+        <v>320</v>
+      </c>
+      <c r="D28" s="4">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E28" s="7">
+        <v>12</v>
+      </c>
+      <c r="F28" s="5">
+        <v>82</v>
+      </c>
+      <c r="G28" s="3">
+        <v>267</v>
+      </c>
+      <c r="H28" s="1">
+        <v>35</v>
+      </c>
+      <c r="I28">
+        <f>SUM(D28:H28)*0.8</f>
+        <v>320.32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="6">
+        <v>308</v>
+      </c>
+      <c r="D30" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="E30" s="7">
+        <v>12</v>
+      </c>
+      <c r="F30" s="5">
+        <v>83</v>
+      </c>
+      <c r="G30" s="3">
+        <v>252</v>
+      </c>
+      <c r="H30" s="1">
+        <v>34</v>
+      </c>
+      <c r="I30">
+        <f>SUM(D30:H30)*0.8</f>
+        <v>308.16000000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="6">
+        <v>308</v>
+      </c>
+      <c r="D31" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="E31" s="7">
+        <v>12</v>
+      </c>
+      <c r="F31" s="5">
+        <v>83</v>
+      </c>
+      <c r="G31" s="3">
+        <v>252</v>
+      </c>
+      <c r="H31" s="1">
+        <v>34</v>
+      </c>
+      <c r="I31">
+        <f>SUM(D31:H31)*0.8</f>
+        <v>308.16000000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="6">
+        <v>308</v>
+      </c>
+      <c r="D32" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="E32" s="7">
+        <v>12</v>
+      </c>
+      <c r="F32" s="5">
+        <v>83</v>
+      </c>
+      <c r="G32" s="3">
+        <v>252</v>
+      </c>
+      <c r="H32" s="1">
+        <v>34</v>
+      </c>
+      <c r="I32">
+        <f>SUM(D32:H32)*0.8</f>
+        <v>308.16000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C18765D9-5E60-43F7-8EAE-7692D37C4247}">
   <dimension ref="A1:J23"/>
   <sheetViews>
@@ -2522,7 +3609,7 @@
       <c r="A2" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="B2" s="27">
+      <c r="B2" s="25">
         <v>1047</v>
       </c>
       <c r="C2" s="4">
@@ -2543,7 +3630,7 @@
       <c r="H2" s="1">
         <v>33</v>
       </c>
-      <c r="I2" s="28">
+      <c r="I2" s="27">
         <v>35</v>
       </c>
     </row>
@@ -2572,7 +3659,7 @@
       <c r="H3" s="1">
         <v>33</v>
       </c>
-      <c r="I3" s="28">
+      <c r="I3" s="27">
         <v>35</v>
       </c>
     </row>
@@ -2601,7 +3688,7 @@
       <c r="H4" s="1">
         <v>34</v>
       </c>
-      <c r="I4" s="28">
+      <c r="I4" s="27">
         <v>34</v>
       </c>
     </row>
@@ -2630,7 +3717,7 @@
       <c r="H5" s="1">
         <v>34</v>
       </c>
-      <c r="I5" s="28">
+      <c r="I5" s="27">
         <v>34</v>
       </c>
     </row>
@@ -2659,7 +3746,7 @@
       <c r="H6" s="1">
         <v>35</v>
       </c>
-      <c r="I6" s="28">
+      <c r="I6" s="27">
         <v>38</v>
       </c>
     </row>
@@ -2688,7 +3775,7 @@
       <c r="H7" s="1">
         <v>35</v>
       </c>
-      <c r="I7" s="28">
+      <c r="I7" s="27">
         <v>39</v>
       </c>
     </row>
@@ -2717,7 +3804,7 @@
       <c r="H8" s="1">
         <v>34</v>
       </c>
-      <c r="I8" s="28">
+      <c r="I8" s="27">
         <v>38</v>
       </c>
     </row>
@@ -2746,7 +3833,7 @@
       <c r="H9" s="1">
         <v>36</v>
       </c>
-      <c r="I9" s="28">
+      <c r="I9" s="27">
         <v>38</v>
       </c>
     </row>
@@ -2775,7 +3862,7 @@
       <c r="H10" s="1">
         <v>36</v>
       </c>
-      <c r="I10" s="28">
+      <c r="I10" s="27">
         <v>39</v>
       </c>
     </row>
@@ -2804,7 +3891,7 @@
       <c r="H11" s="1">
         <v>34</v>
       </c>
-      <c r="I11" s="28">
+      <c r="I11" s="27">
         <v>34</v>
       </c>
     </row>
@@ -2833,7 +3920,7 @@
       <c r="H12" s="1">
         <v>33</v>
       </c>
-      <c r="I12" s="28">
+      <c r="I12" s="27">
         <v>37</v>
       </c>
     </row>
@@ -2862,7 +3949,7 @@
       <c r="H13" s="1">
         <v>37</v>
       </c>
-      <c r="I13" s="28">
+      <c r="I13" s="27">
         <v>35</v>
       </c>
     </row>
@@ -2892,7 +3979,7 @@
       <c r="H15" s="1">
         <v>34</v>
       </c>
-      <c r="I15" s="28">
+      <c r="I15" s="27">
         <v>34</v>
       </c>
       <c r="J15" t="s">
@@ -2924,7 +4011,7 @@
       <c r="H16" s="1">
         <v>36</v>
       </c>
-      <c r="I16" s="28">
+      <c r="I16" s="27">
         <v>35</v>
       </c>
       <c r="J16" t="s">
@@ -2956,7 +4043,7 @@
       <c r="H17" s="1">
         <v>34</v>
       </c>
-      <c r="I17" s="28">
+      <c r="I17" s="27">
         <v>35</v>
       </c>
       <c r="J17" t="s">
@@ -2988,7 +4075,7 @@
       <c r="H18" s="1">
         <v>35</v>
       </c>
-      <c r="I18" s="28">
+      <c r="I18" s="27">
         <v>36</v>
       </c>
       <c r="J18" t="s">
@@ -3020,7 +4107,7 @@
       <c r="H19" s="1">
         <v>36</v>
       </c>
-      <c r="I19" s="28">
+      <c r="I19" s="27">
         <v>36</v>
       </c>
       <c r="J19" t="s">
@@ -3052,7 +4139,7 @@
       <c r="H20" s="1">
         <v>36</v>
       </c>
-      <c r="I20" s="28">
+      <c r="I20" s="27">
         <v>38</v>
       </c>
       <c r="J20" t="s">
@@ -3084,7 +4171,7 @@
       <c r="H21" s="1">
         <v>36</v>
       </c>
-      <c r="I21" s="28">
+      <c r="I21" s="27">
         <v>38</v>
       </c>
       <c r="J21" t="s">
@@ -3116,7 +4203,7 @@
       <c r="H22" s="1">
         <v>37</v>
       </c>
-      <c r="I22" s="28">
+      <c r="I22" s="27">
         <v>38</v>
       </c>
       <c r="J22" t="s">
@@ -3148,7 +4235,7 @@
       <c r="H23" s="1">
         <v>36</v>
       </c>
-      <c r="I23" s="28">
+      <c r="I23" s="27">
         <v>37</v>
       </c>
       <c r="J23" t="s">
@@ -3161,7 +4248,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96551E4B-D0DF-400F-B6DB-43F70FA502C4}">
   <dimension ref="A1:I29"/>
   <sheetViews>
@@ -3831,7 +4918,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DAD396-9A3B-4E45-8468-1404C7D6E830}">
   <dimension ref="A1:J9"/>
   <sheetViews>
@@ -4128,7 +5215,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3C8FEF-B598-4AEC-9E3E-97CE35ABD837}">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -4386,7 +5473,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6EE9141-0B58-4213-922A-6EE4F5E15BD3}">
   <dimension ref="A1:I9"/>
   <sheetViews>
@@ -4673,6 +5760,1210 @@
       <c r="I9">
         <f>((Tableau1[[#This Row],[Hitpoints]]*Tableau1[[#This Row],[Armor]]*2)+(Tableau1[[#This Row],[Width ]]*Tableau1[[#This Row],[Height]]*2)-(Tableau1[[#This Row],[Speed]]*Tableau1[[#This Row],[Weight]]))/100</f>
         <v>114.02</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43106BCE-1E0C-42D9-8C47-8A875A3B9B28}">
+  <dimension ref="A1:E71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="46.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B1">
+        <v>1.2</v>
+      </c>
+      <c r="C1">
+        <v>1.4</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B2">
+        <v>1.35</v>
+      </c>
+      <c r="C2">
+        <v>1.8</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>391</v>
+      </c>
+      <c r="B3">
+        <v>1.5</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>392</v>
+      </c>
+      <c r="B4">
+        <v>1.8</v>
+      </c>
+      <c r="C4">
+        <v>3.5</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>387</v>
+      </c>
+      <c r="E7" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="30" t="s">
+        <v>394</v>
+      </c>
+      <c r="B8" s="31">
+        <v>132</v>
+      </c>
+      <c r="C8" s="21">
+        <v>1</v>
+      </c>
+      <c r="D8" s="32">
+        <v>12</v>
+      </c>
+      <c r="E8" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="30" t="s">
+        <v>395</v>
+      </c>
+      <c r="B9" s="31">
+        <v>216</v>
+      </c>
+      <c r="C9" s="21">
+        <v>1.2</v>
+      </c>
+      <c r="D9" s="32">
+        <v>14</v>
+      </c>
+      <c r="E9" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="30" t="s">
+        <v>396</v>
+      </c>
+      <c r="B10" s="31">
+        <v>320</v>
+      </c>
+      <c r="C10" s="21">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D10" s="32">
+        <v>20</v>
+      </c>
+      <c r="E10" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="30"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="33"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="30" t="s">
+        <v>397</v>
+      </c>
+      <c r="B12" s="31">
+        <v>280</v>
+      </c>
+      <c r="C12" s="21">
+        <v>1.5</v>
+      </c>
+      <c r="D12" s="32">
+        <v>18</v>
+      </c>
+      <c r="E12" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="30" t="s">
+        <v>398</v>
+      </c>
+      <c r="B13" s="31">
+        <f>B12*B1</f>
+        <v>336</v>
+      </c>
+      <c r="C13" s="21">
+        <f>C12+C1</f>
+        <v>2.9</v>
+      </c>
+      <c r="D13" s="32">
+        <f>D12+D1</f>
+        <v>22</v>
+      </c>
+      <c r="E13" s="33">
+        <f>E1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="30" t="s">
+        <v>400</v>
+      </c>
+      <c r="B14" s="31">
+        <f>B12*B2</f>
+        <v>378</v>
+      </c>
+      <c r="C14" s="21">
+        <f>C12+C2</f>
+        <v>3.3</v>
+      </c>
+      <c r="D14" s="32">
+        <f>D12+D2</f>
+        <v>24</v>
+      </c>
+      <c r="E14" s="33">
+        <f>E2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="30" t="s">
+        <v>399</v>
+      </c>
+      <c r="B15" s="31">
+        <f>B12*B4</f>
+        <v>504</v>
+      </c>
+      <c r="C15" s="21">
+        <f>C12+C4</f>
+        <v>5</v>
+      </c>
+      <c r="D15" s="32">
+        <f>D12+D4</f>
+        <v>28</v>
+      </c>
+      <c r="E15" s="33">
+        <f>E4</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="30"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="33"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="30" t="s">
+        <v>401</v>
+      </c>
+      <c r="B17" s="31">
+        <v>320</v>
+      </c>
+      <c r="C17" s="21">
+        <v>1.6</v>
+      </c>
+      <c r="D17" s="32">
+        <v>20</v>
+      </c>
+      <c r="E17" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="30" t="s">
+        <v>402</v>
+      </c>
+      <c r="B18" s="31">
+        <f>B17*B1</f>
+        <v>384</v>
+      </c>
+      <c r="C18" s="21">
+        <f>C17+C1</f>
+        <v>3</v>
+      </c>
+      <c r="D18" s="32">
+        <f>D17+D1</f>
+        <v>24</v>
+      </c>
+      <c r="E18" s="33">
+        <f>E1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="30" t="s">
+        <v>403</v>
+      </c>
+      <c r="B19" s="31">
+        <f>B17*B2</f>
+        <v>432</v>
+      </c>
+      <c r="C19" s="21">
+        <f>C17+C2</f>
+        <v>3.4000000000000004</v>
+      </c>
+      <c r="D19" s="32">
+        <f>D17+D2</f>
+        <v>26</v>
+      </c>
+      <c r="E19" s="33">
+        <f>E2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="30" t="s">
+        <v>404</v>
+      </c>
+      <c r="B20" s="31">
+        <f>B17*B4</f>
+        <v>576</v>
+      </c>
+      <c r="C20" s="21">
+        <f>C17+C4</f>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D20" s="32">
+        <f>D17+D4</f>
+        <v>30</v>
+      </c>
+      <c r="E20" s="33">
+        <f>E4</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="30"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="33"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="30" t="s">
+        <v>405</v>
+      </c>
+      <c r="B22" s="31">
+        <v>336</v>
+      </c>
+      <c r="C22" s="21">
+        <v>1.8</v>
+      </c>
+      <c r="D22" s="32">
+        <v>22</v>
+      </c>
+      <c r="E22" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="30" t="s">
+        <v>406</v>
+      </c>
+      <c r="B23" s="31">
+        <f>B22*B1</f>
+        <v>403.2</v>
+      </c>
+      <c r="C23" s="21">
+        <f>C22+C1</f>
+        <v>3.2</v>
+      </c>
+      <c r="D23" s="32">
+        <f>D22+D1</f>
+        <v>26</v>
+      </c>
+      <c r="E23" s="33">
+        <f>E1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="30" t="s">
+        <v>407</v>
+      </c>
+      <c r="B24" s="31">
+        <f>B22*B2</f>
+        <v>453.6</v>
+      </c>
+      <c r="C24" s="21">
+        <f>C22+C2</f>
+        <v>3.6</v>
+      </c>
+      <c r="D24" s="32">
+        <f>D22+D2</f>
+        <v>28</v>
+      </c>
+      <c r="E24" s="33">
+        <f>E2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="30" t="s">
+        <v>408</v>
+      </c>
+      <c r="B25" s="31">
+        <f>B22*B4</f>
+        <v>604.80000000000007</v>
+      </c>
+      <c r="C25" s="21">
+        <f>C22+C4</f>
+        <v>5.3</v>
+      </c>
+      <c r="D25" s="32">
+        <f>D22+D4</f>
+        <v>32</v>
+      </c>
+      <c r="E25" s="33">
+        <f>E4</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="30"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="33"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="30" t="s">
+        <v>409</v>
+      </c>
+      <c r="B27" s="31">
+        <v>384</v>
+      </c>
+      <c r="C27" s="21">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D27" s="32">
+        <v>24</v>
+      </c>
+      <c r="E27" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="30" t="s">
+        <v>410</v>
+      </c>
+      <c r="B28" s="31">
+        <f>B27*B1</f>
+        <v>460.79999999999995</v>
+      </c>
+      <c r="C28" s="21">
+        <f>C27+C1</f>
+        <v>3.6</v>
+      </c>
+      <c r="D28" s="32">
+        <f>D27+D1</f>
+        <v>28</v>
+      </c>
+      <c r="E28" s="33">
+        <f>E1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="30" t="s">
+        <v>411</v>
+      </c>
+      <c r="B29" s="31">
+        <f>B27*B2</f>
+        <v>518.40000000000009</v>
+      </c>
+      <c r="C29" s="21">
+        <f>C27+C2</f>
+        <v>4</v>
+      </c>
+      <c r="D29" s="32">
+        <f>D27+D3</f>
+        <v>32</v>
+      </c>
+      <c r="E29" s="33">
+        <f>E2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="30" t="s">
+        <v>412</v>
+      </c>
+      <c r="B30" s="31">
+        <f>B27*B4</f>
+        <v>691.2</v>
+      </c>
+      <c r="C30" s="21">
+        <f>C27+C4</f>
+        <v>5.7</v>
+      </c>
+      <c r="D30" s="32">
+        <f>D27+D4</f>
+        <v>34</v>
+      </c>
+      <c r="E30" s="33">
+        <f>E4</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="30"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="33"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="30" t="s">
+        <v>413</v>
+      </c>
+      <c r="B32" s="31">
+        <v>432</v>
+      </c>
+      <c r="C32" s="21">
+        <v>2.4</v>
+      </c>
+      <c r="D32" s="32">
+        <v>26</v>
+      </c>
+      <c r="E32" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="30" t="s">
+        <v>414</v>
+      </c>
+      <c r="B33" s="31">
+        <f>B32*B1</f>
+        <v>518.4</v>
+      </c>
+      <c r="C33" s="21">
+        <f>C32+C1</f>
+        <v>3.8</v>
+      </c>
+      <c r="D33" s="32">
+        <f>D32+D1</f>
+        <v>30</v>
+      </c>
+      <c r="E33" s="33">
+        <f>E1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="30" t="s">
+        <v>415</v>
+      </c>
+      <c r="B34" s="31">
+        <f>B32*B2</f>
+        <v>583.20000000000005</v>
+      </c>
+      <c r="C34" s="21">
+        <f>C32+C2</f>
+        <v>4.2</v>
+      </c>
+      <c r="D34" s="32">
+        <f>D32+D2</f>
+        <v>32</v>
+      </c>
+      <c r="E34" s="33">
+        <f>E2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="30" t="s">
+        <v>416</v>
+      </c>
+      <c r="B35" s="31">
+        <f>B32*B4</f>
+        <v>777.6</v>
+      </c>
+      <c r="C35" s="21">
+        <f>C32+C4</f>
+        <v>5.9</v>
+      </c>
+      <c r="D35" s="32">
+        <f>D32+D4</f>
+        <v>36</v>
+      </c>
+      <c r="E35" s="33">
+        <f>E4</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="30"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="33"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="30" t="s">
+        <v>432</v>
+      </c>
+      <c r="B37" s="31">
+        <v>518</v>
+      </c>
+      <c r="C37" s="21">
+        <v>2.8</v>
+      </c>
+      <c r="D37" s="32">
+        <v>30</v>
+      </c>
+      <c r="E37" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="30" t="s">
+        <v>433</v>
+      </c>
+      <c r="B38" s="31">
+        <f>B37*B1</f>
+        <v>621.6</v>
+      </c>
+      <c r="C38" s="21">
+        <f>C37+C1</f>
+        <v>4.1999999999999993</v>
+      </c>
+      <c r="D38" s="32">
+        <f>D37+D1</f>
+        <v>34</v>
+      </c>
+      <c r="E38" s="33">
+        <f>E1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="30" t="s">
+        <v>434</v>
+      </c>
+      <c r="B39" s="31">
+        <f>B37*B2</f>
+        <v>699.30000000000007</v>
+      </c>
+      <c r="C39" s="21">
+        <f>C37+C2</f>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D39" s="32">
+        <f>D37+D2</f>
+        <v>36</v>
+      </c>
+      <c r="E39" s="33">
+        <f>E2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="30" t="s">
+        <v>435</v>
+      </c>
+      <c r="B40" s="31">
+        <f>B37*B4</f>
+        <v>932.4</v>
+      </c>
+      <c r="C40" s="21">
+        <f>C37+C4</f>
+        <v>6.3</v>
+      </c>
+      <c r="D40" s="32">
+        <f>D37+D4</f>
+        <v>40</v>
+      </c>
+      <c r="E40" s="33">
+        <f>E4</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="30"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="33"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="30" t="s">
+        <v>417</v>
+      </c>
+      <c r="B42" s="31">
+        <v>690</v>
+      </c>
+      <c r="C42" s="21">
+        <v>3</v>
+      </c>
+      <c r="D42" s="32">
+        <v>34</v>
+      </c>
+      <c r="E42" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="30" t="s">
+        <v>419</v>
+      </c>
+      <c r="B43" s="31">
+        <f>B42*B3</f>
+        <v>1035</v>
+      </c>
+      <c r="C43" s="21">
+        <f>C42+C3</f>
+        <v>6</v>
+      </c>
+      <c r="D43" s="32">
+        <f>D42+D3</f>
+        <v>42</v>
+      </c>
+      <c r="E43" s="33">
+        <f>E3</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="30" t="s">
+        <v>418</v>
+      </c>
+      <c r="B44" s="31">
+        <f>B42*B4</f>
+        <v>1242</v>
+      </c>
+      <c r="C44" s="21">
+        <f>C42+C4</f>
+        <v>6.5</v>
+      </c>
+      <c r="D44" s="32">
+        <f>D42+D4</f>
+        <v>44</v>
+      </c>
+      <c r="E44" s="33">
+        <f>E4</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="30" t="s">
+        <v>420</v>
+      </c>
+      <c r="B45" s="31">
+        <f>B42*B5</f>
+        <v>1380</v>
+      </c>
+      <c r="C45" s="21">
+        <f>C42+C5</f>
+        <v>7</v>
+      </c>
+      <c r="D45" s="32">
+        <f>D42+D5</f>
+        <v>46</v>
+      </c>
+      <c r="E45" s="33">
+        <f>E5</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="30"/>
+      <c r="B46" s="31"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="33"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="30" t="s">
+        <v>421</v>
+      </c>
+      <c r="B47" s="31">
+        <v>920</v>
+      </c>
+      <c r="C47" s="21">
+        <v>3.4</v>
+      </c>
+      <c r="D47" s="32">
+        <v>38</v>
+      </c>
+      <c r="E47" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="30" t="s">
+        <v>422</v>
+      </c>
+      <c r="B48" s="31">
+        <f>B47*B3</f>
+        <v>1380</v>
+      </c>
+      <c r="C48" s="21">
+        <f>C47+C3</f>
+        <v>6.4</v>
+      </c>
+      <c r="D48" s="32">
+        <f>D47+D3</f>
+        <v>46</v>
+      </c>
+      <c r="E48" s="33">
+        <f>E3</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="30" t="s">
+        <v>423</v>
+      </c>
+      <c r="B49" s="31">
+        <f>B47*B4</f>
+        <v>1656</v>
+      </c>
+      <c r="C49" s="21">
+        <f>C47+C4</f>
+        <v>6.9</v>
+      </c>
+      <c r="D49" s="32">
+        <f>D47+D4</f>
+        <v>48</v>
+      </c>
+      <c r="E49" s="33">
+        <f>E4</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="30" t="s">
+        <v>424</v>
+      </c>
+      <c r="B50" s="31">
+        <f>B47*B5</f>
+        <v>1840</v>
+      </c>
+      <c r="C50" s="21">
+        <f>C47+C5</f>
+        <v>7.4</v>
+      </c>
+      <c r="D50" s="32">
+        <f>D47+D5</f>
+        <v>50</v>
+      </c>
+      <c r="E50" s="33">
+        <f>E5</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="30"/>
+      <c r="B51" s="31"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="33"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="30" t="s">
+        <v>425</v>
+      </c>
+      <c r="B52" s="31">
+        <v>1035</v>
+      </c>
+      <c r="C52" s="21">
+        <v>4</v>
+      </c>
+      <c r="D52" s="32">
+        <v>42</v>
+      </c>
+      <c r="E52" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="30" t="s">
+        <v>426</v>
+      </c>
+      <c r="B53" s="31">
+        <f>B52*B3</f>
+        <v>1552.5</v>
+      </c>
+      <c r="C53" s="21">
+        <f>C52+C3</f>
+        <v>7</v>
+      </c>
+      <c r="D53" s="32">
+        <f>D52+D3</f>
+        <v>50</v>
+      </c>
+      <c r="E53" s="33">
+        <f>E3</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="30" t="s">
+        <v>427</v>
+      </c>
+      <c r="B54" s="31">
+        <f>B52*B4</f>
+        <v>1863</v>
+      </c>
+      <c r="C54" s="21">
+        <f>C52+C4</f>
+        <v>7.5</v>
+      </c>
+      <c r="D54" s="32">
+        <f>D52+D4</f>
+        <v>52</v>
+      </c>
+      <c r="E54" s="33">
+        <f>E4</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="30" t="s">
+        <v>428</v>
+      </c>
+      <c r="B55" s="31">
+        <f>B52*B5</f>
+        <v>2070</v>
+      </c>
+      <c r="C55" s="21">
+        <f>C52+C5</f>
+        <v>8</v>
+      </c>
+      <c r="D55" s="32">
+        <f>D52+D5</f>
+        <v>54</v>
+      </c>
+      <c r="E55" s="33">
+        <f>E5</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="30"/>
+      <c r="B56" s="31"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="33"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="30" t="s">
+        <v>429</v>
+      </c>
+      <c r="B57" s="31">
+        <v>1300</v>
+      </c>
+      <c r="C57" s="21">
+        <v>7.5</v>
+      </c>
+      <c r="D57" s="32">
+        <v>45</v>
+      </c>
+      <c r="E57" s="33">
+        <f>E4</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="30" t="s">
+        <v>430</v>
+      </c>
+      <c r="B58" s="31">
+        <v>2100</v>
+      </c>
+      <c r="C58" s="21">
+        <v>8.5</v>
+      </c>
+      <c r="D58" s="32">
+        <v>54</v>
+      </c>
+      <c r="E58" s="33">
+        <f>E4</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="30" t="s">
+        <v>431</v>
+      </c>
+      <c r="B59" s="31">
+        <v>2225</v>
+      </c>
+      <c r="C59" s="21">
+        <v>8.6</v>
+      </c>
+      <c r="D59" s="32">
+        <v>56</v>
+      </c>
+      <c r="E59" s="33">
+        <f>E4</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="30"/>
+      <c r="B60" s="31"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="32"/>
+      <c r="E60" s="33"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="30" t="s">
+        <v>436</v>
+      </c>
+      <c r="B61" s="31">
+        <v>1380</v>
+      </c>
+      <c r="C61" s="21">
+        <v>3.5</v>
+      </c>
+      <c r="D61" s="32">
+        <v>46</v>
+      </c>
+      <c r="E61" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="30" t="s">
+        <v>437</v>
+      </c>
+      <c r="B62" s="31">
+        <f>B61*B3</f>
+        <v>2070</v>
+      </c>
+      <c r="C62" s="21">
+        <f>C61+C3</f>
+        <v>6.5</v>
+      </c>
+      <c r="D62" s="32">
+        <f>D61+D3</f>
+        <v>54</v>
+      </c>
+      <c r="E62" s="33">
+        <f>E3</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="30" t="s">
+        <v>438</v>
+      </c>
+      <c r="B63" s="31">
+        <f>B61*B5</f>
+        <v>2760</v>
+      </c>
+      <c r="C63" s="21">
+        <f>C61+C5</f>
+        <v>7.5</v>
+      </c>
+      <c r="D63" s="32">
+        <f>D61+D5</f>
+        <v>58</v>
+      </c>
+      <c r="E63" s="33">
+        <f>E5</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="30" t="s">
+        <v>439</v>
+      </c>
+      <c r="B64" s="31">
+        <v>1550</v>
+      </c>
+      <c r="C64" s="21">
+        <v>4.2</v>
+      </c>
+      <c r="D64" s="32">
+        <f>D61+4</f>
+        <v>50</v>
+      </c>
+      <c r="E64" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="30"/>
+      <c r="B65" s="31"/>
+      <c r="C65" s="21"/>
+      <c r="D65" s="32"/>
+      <c r="E65" s="33"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="30" t="s">
+        <v>440</v>
+      </c>
+      <c r="B66" s="31">
+        <v>3180</v>
+      </c>
+      <c r="C66" s="21">
+        <v>9</v>
+      </c>
+      <c r="D66" s="32">
+        <v>60</v>
+      </c>
+      <c r="E66" s="33">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="30"/>
+      <c r="B67" s="31"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="32"/>
+      <c r="E67" s="33"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="30" t="s">
+        <v>441</v>
+      </c>
+      <c r="B68" s="31">
+        <v>2225</v>
+      </c>
+      <c r="C68" s="21">
+        <v>6</v>
+      </c>
+      <c r="D68" s="32">
+        <v>56</v>
+      </c>
+      <c r="E68" s="33">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="30" t="s">
+        <v>442</v>
+      </c>
+      <c r="B69" s="31">
+        <f>B68*2.2</f>
+        <v>4895</v>
+      </c>
+      <c r="C69" s="21">
+        <v>7.2</v>
+      </c>
+      <c r="D69" s="32">
+        <v>66</v>
+      </c>
+      <c r="E69" s="33">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="30" t="s">
+        <v>443</v>
+      </c>
+      <c r="B70" s="31">
+        <v>3000</v>
+      </c>
+      <c r="C70" s="21">
+        <v>6.8</v>
+      </c>
+      <c r="D70" s="32">
+        <v>58</v>
+      </c>
+      <c r="E70" s="33">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="30" t="s">
+        <v>444</v>
+      </c>
+      <c r="B71" s="31">
+        <v>6000</v>
+      </c>
+      <c r="C71" s="21">
+        <v>8</v>
+      </c>
+      <c r="D71" s="32">
+        <v>68</v>
+      </c>
+      <c r="E71" s="33">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -9753,7 +12044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC772471-31F7-4C6C-832D-6D1F31BC4A1E}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -9992,6 +12283,18 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53C74D93-0A0F-4AF8-A6DA-437C48E3A356}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE67CB9-8D30-45BB-9729-53435DBF7C02}">
   <dimension ref="A1:I13"/>
   <sheetViews>
@@ -10320,7 +12623,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{042C4405-AEC3-4A36-A3E7-7EA75E4B87DD}">
   <dimension ref="A1:J9"/>
   <sheetViews>
@@ -10549,16 +12852,16 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="29"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="30"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="29"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -10589,778 +12892,6 @@
       <c r="J9">
         <f>SUM(D9:I9)*0.8</f>
         <v>276.16000000000003</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{270FCD42-7C0A-42FB-9872-27F0BB063FAE}">
-  <dimension ref="A1:I32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="26.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="6">
-        <v>134</v>
-      </c>
-      <c r="D2" s="4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E2" s="7">
-        <v>0</v>
-      </c>
-      <c r="F2" s="5">
-        <v>99</v>
-      </c>
-      <c r="G2" s="3">
-        <v>107</v>
-      </c>
-      <c r="H2" s="1">
-        <v>37</v>
-      </c>
-      <c r="I2">
-        <f>SUM(D2:H2)*0.55</f>
-        <v>134.255</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="6">
-        <v>144</v>
-      </c>
-      <c r="D3" s="4">
-        <v>1.3</v>
-      </c>
-      <c r="E3" s="7">
-        <v>0</v>
-      </c>
-      <c r="F3" s="5">
-        <v>97</v>
-      </c>
-      <c r="G3" s="3">
-        <v>128</v>
-      </c>
-      <c r="H3" s="1">
-        <v>36</v>
-      </c>
-      <c r="I3">
-        <f>SUM(D3:H3)*0.55</f>
-        <v>144.26500000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="6">
-        <v>146</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1.3</v>
-      </c>
-      <c r="E4" s="7">
-        <v>0</v>
-      </c>
-      <c r="F4" s="5">
-        <v>97</v>
-      </c>
-      <c r="G4" s="3">
-        <v>132</v>
-      </c>
-      <c r="H4" s="1">
-        <v>36</v>
-      </c>
-      <c r="I4">
-        <f>SUM(D4:H4)*0.55</f>
-        <v>146.46500000000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="6">
-        <v>165</v>
-      </c>
-      <c r="D5" s="4">
-        <v>1.4</v>
-      </c>
-      <c r="E5" s="7">
-        <v>0</v>
-      </c>
-      <c r="F5" s="5">
-        <v>96</v>
-      </c>
-      <c r="G5" s="3">
-        <v>142</v>
-      </c>
-      <c r="H5" s="1">
-        <v>35</v>
-      </c>
-      <c r="I5">
-        <f>SUM(D5:H5)*0.6</f>
-        <v>164.64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="6">
-        <v>166</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1.4</v>
-      </c>
-      <c r="E6" s="7">
-        <v>0</v>
-      </c>
-      <c r="F6" s="5">
-        <v>96</v>
-      </c>
-      <c r="G6" s="3">
-        <v>144</v>
-      </c>
-      <c r="H6" s="1">
-        <v>35</v>
-      </c>
-      <c r="I6">
-        <f>SUM(D6:H6)*0.6</f>
-        <v>165.83999999999997</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="6">
-        <v>168</v>
-      </c>
-      <c r="D7" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="E7" s="7">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5">
-        <v>95</v>
-      </c>
-      <c r="G7" s="3">
-        <v>149</v>
-      </c>
-      <c r="H7" s="1">
-        <v>34</v>
-      </c>
-      <c r="I7">
-        <f>SUM(D7:H7)*0.6</f>
-        <v>167.7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="6">
-        <v>229</v>
-      </c>
-      <c r="D8" s="4">
-        <v>2</v>
-      </c>
-      <c r="E8" s="7">
-        <v>0</v>
-      </c>
-      <c r="F8" s="5">
-        <v>90</v>
-      </c>
-      <c r="G8" s="3">
-        <v>204</v>
-      </c>
-      <c r="H8" s="1">
-        <v>31</v>
-      </c>
-      <c r="I8">
-        <f>SUM(D8:H8)*0.7</f>
-        <v>228.89999999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="6">
-        <v>117</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1</v>
-      </c>
-      <c r="E9" s="7">
-        <v>0</v>
-      </c>
-      <c r="F9" s="5">
-        <v>100</v>
-      </c>
-      <c r="G9" s="3">
-        <v>95</v>
-      </c>
-      <c r="H9" s="1">
-        <v>38</v>
-      </c>
-      <c r="I9">
-        <f>SUM(D9:H9)*0.5</f>
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="6">
-        <v>87</v>
-      </c>
-      <c r="D11" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="E11" s="7">
-        <v>0</v>
-      </c>
-      <c r="F11" s="5">
-        <v>87</v>
-      </c>
-      <c r="G11" s="3">
-        <v>135</v>
-      </c>
-      <c r="H11" s="1">
-        <v>26</v>
-      </c>
-      <c r="I11">
-        <f>SUM(D11:H11)*0.35</f>
-        <v>87.324999999999989</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="6">
-        <v>84</v>
-      </c>
-      <c r="D12" s="4">
-        <v>1.4</v>
-      </c>
-      <c r="E12" s="7">
-        <v>0</v>
-      </c>
-      <c r="F12" s="5">
-        <v>88</v>
-      </c>
-      <c r="G12" s="3">
-        <v>126</v>
-      </c>
-      <c r="H12" s="1">
-        <v>25</v>
-      </c>
-      <c r="I12">
-        <f>SUM(D12:H12)*0.35</f>
-        <v>84.14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="6">
-        <v>142</v>
-      </c>
-      <c r="D13" s="4">
-        <v>2</v>
-      </c>
-      <c r="E13" s="7">
-        <v>0</v>
-      </c>
-      <c r="F13" s="5">
-        <v>84</v>
-      </c>
-      <c r="G13" s="3">
-        <v>168</v>
-      </c>
-      <c r="H13" s="1">
-        <v>31</v>
-      </c>
-      <c r="I13">
-        <f>SUM(D13:H13)*0.5</f>
-        <v>142.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="6">
-        <v>285</v>
-      </c>
-      <c r="D15" s="4">
-        <v>3</v>
-      </c>
-      <c r="E15" s="7">
-        <v>9</v>
-      </c>
-      <c r="F15" s="5">
-        <v>84</v>
-      </c>
-      <c r="G15" s="3">
-        <v>355</v>
-      </c>
-      <c r="H15" s="1">
-        <v>25</v>
-      </c>
-      <c r="I15">
-        <f>SUM(D15:H15)*0.6</f>
-        <v>285.59999999999997</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="6">
-        <v>214</v>
-      </c>
-      <c r="D16" s="4">
-        <v>2.5</v>
-      </c>
-      <c r="E16" s="7">
-        <v>9</v>
-      </c>
-      <c r="F16" s="5">
-        <v>92</v>
-      </c>
-      <c r="G16" s="3">
-        <v>175</v>
-      </c>
-      <c r="H16" s="1">
-        <v>27</v>
-      </c>
-      <c r="I16">
-        <f>SUM(D16:H16)*0.7</f>
-        <v>213.85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="6">
-        <v>224</v>
-      </c>
-      <c r="D17" s="4">
-        <v>2.4</v>
-      </c>
-      <c r="E17" s="7">
-        <v>9</v>
-      </c>
-      <c r="F17" s="5">
-        <v>90</v>
-      </c>
-      <c r="G17" s="3">
-        <v>190</v>
-      </c>
-      <c r="H17" s="1">
-        <v>29</v>
-      </c>
-      <c r="I17">
-        <f>SUM(D17:H17)*0.7</f>
-        <v>224.27999999999997</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="6">
-        <v>320</v>
-      </c>
-      <c r="D19" s="4">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E19" s="7">
-        <v>12</v>
-      </c>
-      <c r="F19" s="5">
-        <v>82</v>
-      </c>
-      <c r="G19" s="3">
-        <v>267</v>
-      </c>
-      <c r="H19" s="1">
-        <v>35</v>
-      </c>
-      <c r="I19">
-        <f t="shared" ref="I19:I24" si="0">SUM(D19:H19)*0.8</f>
-        <v>320.32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="6">
-        <v>286</v>
-      </c>
-      <c r="D20" s="4">
-        <v>4</v>
-      </c>
-      <c r="E20" s="7">
-        <v>12</v>
-      </c>
-      <c r="F20" s="5">
-        <v>85</v>
-      </c>
-      <c r="G20" s="3">
-        <v>226</v>
-      </c>
-      <c r="H20" s="1">
-        <v>31</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="0"/>
-        <v>286.40000000000003</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="6">
-        <v>307</v>
-      </c>
-      <c r="D21" s="4">
-        <v>4.2</v>
-      </c>
-      <c r="E21" s="7">
-        <v>12</v>
-      </c>
-      <c r="F21" s="5">
-        <v>83</v>
-      </c>
-      <c r="G21" s="3">
-        <v>253</v>
-      </c>
-      <c r="H21" s="1">
-        <v>32</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="0"/>
-        <v>307.36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="6">
-        <v>307</v>
-      </c>
-      <c r="D22" s="4">
-        <v>4.2</v>
-      </c>
-      <c r="E22" s="7">
-        <v>12</v>
-      </c>
-      <c r="F22" s="5">
-        <v>83</v>
-      </c>
-      <c r="G22" s="3">
-        <v>253</v>
-      </c>
-      <c r="H22" s="1">
-        <v>32</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="0"/>
-        <v>307.36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="6">
-        <v>308</v>
-      </c>
-      <c r="D23" s="4">
-        <v>4.2</v>
-      </c>
-      <c r="E23" s="7">
-        <v>12</v>
-      </c>
-      <c r="F23" s="5">
-        <v>83</v>
-      </c>
-      <c r="G23" s="3">
-        <v>252</v>
-      </c>
-      <c r="H23" s="1">
-        <v>34</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="0"/>
-        <v>308.16000000000003</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="6">
-        <v>296</v>
-      </c>
-      <c r="D24" s="4">
-        <v>4.3</v>
-      </c>
-      <c r="E24" s="7">
-        <v>12</v>
-      </c>
-      <c r="F24" s="5">
-        <v>83</v>
-      </c>
-      <c r="G24" s="3">
-        <v>241</v>
-      </c>
-      <c r="H24" s="1">
-        <v>30</v>
-      </c>
-      <c r="I24">
-        <f t="shared" si="0"/>
-        <v>296.24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="6">
-        <v>308</v>
-      </c>
-      <c r="D26" s="4">
-        <v>4.2</v>
-      </c>
-      <c r="E26" s="7">
-        <v>12</v>
-      </c>
-      <c r="F26" s="5">
-        <v>83</v>
-      </c>
-      <c r="G26" s="3">
-        <v>252</v>
-      </c>
-      <c r="H26" s="1">
-        <v>34</v>
-      </c>
-      <c r="I26">
-        <f>SUM(D26:H26)*0.8</f>
-        <v>308.16000000000003</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="6">
-        <v>308</v>
-      </c>
-      <c r="D27" s="4">
-        <v>4.2</v>
-      </c>
-      <c r="E27" s="7">
-        <v>12</v>
-      </c>
-      <c r="F27" s="5">
-        <v>83</v>
-      </c>
-      <c r="G27" s="3">
-        <v>252</v>
-      </c>
-      <c r="H27" s="1">
-        <v>34</v>
-      </c>
-      <c r="I27">
-        <f>SUM(D27:H27)*0.8</f>
-        <v>308.16000000000003</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="6">
-        <v>320</v>
-      </c>
-      <c r="D28" s="4">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="E28" s="7">
-        <v>12</v>
-      </c>
-      <c r="F28" s="5">
-        <v>82</v>
-      </c>
-      <c r="G28" s="3">
-        <v>267</v>
-      </c>
-      <c r="H28" s="1">
-        <v>35</v>
-      </c>
-      <c r="I28">
-        <f>SUM(D28:H28)*0.8</f>
-        <v>320.32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="6">
-        <v>308</v>
-      </c>
-      <c r="D30" s="4">
-        <v>4.2</v>
-      </c>
-      <c r="E30" s="7">
-        <v>12</v>
-      </c>
-      <c r="F30" s="5">
-        <v>83</v>
-      </c>
-      <c r="G30" s="3">
-        <v>252</v>
-      </c>
-      <c r="H30" s="1">
-        <v>34</v>
-      </c>
-      <c r="I30">
-        <f>SUM(D30:H30)*0.8</f>
-        <v>308.16000000000003</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="6">
-        <v>308</v>
-      </c>
-      <c r="D31" s="4">
-        <v>4.2</v>
-      </c>
-      <c r="E31" s="7">
-        <v>12</v>
-      </c>
-      <c r="F31" s="5">
-        <v>83</v>
-      </c>
-      <c r="G31" s="3">
-        <v>252</v>
-      </c>
-      <c r="H31" s="1">
-        <v>34</v>
-      </c>
-      <c r="I31">
-        <f>SUM(D31:H31)*0.8</f>
-        <v>308.16000000000003</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="6">
-        <v>308</v>
-      </c>
-      <c r="D32" s="4">
-        <v>4.2</v>
-      </c>
-      <c r="E32" s="7">
-        <v>12</v>
-      </c>
-      <c r="F32" s="5">
-        <v>83</v>
-      </c>
-      <c r="G32" s="3">
-        <v>252</v>
-      </c>
-      <c r="H32" s="1">
-        <v>34</v>
-      </c>
-      <c r="I32">
-        <f>SUM(D32:H32)*0.8</f>
-        <v>308.16000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>